<commit_message>
FS cycle is added
</commit_message>
<xml_diff>
--- a/AnimalWill/AnimalWillMaths.xlsx
+++ b/AnimalWill/AnimalWillMaths.xlsx
@@ -5,17 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\konstantin.d\source\repos\AnimalWill\AnimalWill\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AMD\source\repos\microchelick43018\AnimalWill\AnimalWill\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F00A9712-CC87-464C-9DCA-9153A6213C94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E69AEE8-D76A-4936-96D7-1E65CA67A78C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
-    <sheet name="Paytable" sheetId="2" r:id="rId2"/>
-    <sheet name="Paylines" sheetId="14" r:id="rId3"/>
+    <sheet name="Paylines" sheetId="14" r:id="rId2"/>
+    <sheet name="Paytable" sheetId="2" r:id="rId3"/>
     <sheet name="Collect Feature Paytable" sheetId="12" r:id="rId4"/>
     <sheet name="Base Game Reels" sheetId="3" r:id="rId5"/>
     <sheet name="Outer Collector Reels" sheetId="15" r:id="rId6"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1636" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1641" uniqueCount="82">
   <si>
     <t xml:space="preserve">Slot Name: </t>
   </si>
@@ -810,7 +810,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -827,6 +826,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1768,284 +1770,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B3:G15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="2:7">
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>3</v>
-      </c>
-      <c r="F3">
-        <v>4</v>
-      </c>
-      <c r="G3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7">
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <v>50</v>
-      </c>
-      <c r="F4">
-        <v>200</v>
-      </c>
-      <c r="G4">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7">
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>30</v>
-      </c>
-      <c r="F5">
-        <v>150</v>
-      </c>
-      <c r="G5">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7">
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>20</v>
-      </c>
-      <c r="F6">
-        <v>100</v>
-      </c>
-      <c r="G6">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7">
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>20</v>
-      </c>
-      <c r="F7">
-        <v>80</v>
-      </c>
-      <c r="G7">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7">
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>20</v>
-      </c>
-      <c r="F8">
-        <v>60</v>
-      </c>
-      <c r="G8">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7">
-      <c r="B9" t="s">
-        <v>77</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>20</v>
-      </c>
-      <c r="F9">
-        <v>50</v>
-      </c>
-      <c r="G9">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7">
-      <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>5</v>
-      </c>
-      <c r="F10">
-        <v>30</v>
-      </c>
-      <c r="G10">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7">
-      <c r="B11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>5</v>
-      </c>
-      <c r="F11">
-        <v>30</v>
-      </c>
-      <c r="G11">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7">
-      <c r="B12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>5</v>
-      </c>
-      <c r="F12">
-        <v>20</v>
-      </c>
-      <c r="G12">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7">
-      <c r="B13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>5</v>
-      </c>
-      <c r="F13">
-        <v>20</v>
-      </c>
-      <c r="G13">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7">
-      <c r="B14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>5</v>
-      </c>
-      <c r="F14">
-        <v>20</v>
-      </c>
-      <c r="G14">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7">
-      <c r="B15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>3</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{135047FB-1EC6-463A-ADBB-A49C61415168}">
   <dimension ref="A4:F59"/>
   <sheetViews>
@@ -2133,1002 +1857,1002 @@
       <c r="F9" s="56"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="49">
+      <c r="A10" s="48">
         <v>1</v>
       </c>
-      <c r="B10" s="50">
-        <v>0</v>
-      </c>
-      <c r="C10" s="50">
-        <v>0</v>
-      </c>
-      <c r="D10" s="50">
-        <v>0</v>
-      </c>
-      <c r="E10" s="50">
-        <v>0</v>
-      </c>
-      <c r="F10" s="50">
+      <c r="B10" s="49">
+        <v>0</v>
+      </c>
+      <c r="C10" s="49">
+        <v>0</v>
+      </c>
+      <c r="D10" s="49">
+        <v>0</v>
+      </c>
+      <c r="E10" s="49">
+        <v>0</v>
+      </c>
+      <c r="F10" s="49">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="49">
+      <c r="A11" s="48">
         <v>2</v>
       </c>
-      <c r="B11" s="50">
+      <c r="B11" s="49">
         <v>1</v>
       </c>
-      <c r="C11" s="50">
+      <c r="C11" s="49">
         <v>1</v>
       </c>
-      <c r="D11" s="50">
+      <c r="D11" s="49">
         <v>1</v>
       </c>
-      <c r="E11" s="50">
+      <c r="E11" s="49">
         <v>1</v>
       </c>
-      <c r="F11" s="50">
+      <c r="F11" s="49">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="49">
+      <c r="A12" s="48">
         <v>3</v>
       </c>
-      <c r="B12" s="50">
+      <c r="B12" s="49">
         <v>2</v>
       </c>
-      <c r="C12" s="50">
+      <c r="C12" s="49">
         <v>2</v>
       </c>
-      <c r="D12" s="50">
+      <c r="D12" s="49">
         <v>2</v>
       </c>
-      <c r="E12" s="50">
+      <c r="E12" s="49">
         <v>2</v>
       </c>
-      <c r="F12" s="50">
+      <c r="F12" s="49">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="49">
+      <c r="A13" s="48">
         <v>4</v>
       </c>
-      <c r="B13" s="50">
+      <c r="B13" s="49">
         <v>3</v>
       </c>
-      <c r="C13" s="50">
+      <c r="C13" s="49">
         <v>3</v>
       </c>
-      <c r="D13" s="50">
+      <c r="D13" s="49">
         <v>3</v>
       </c>
-      <c r="E13" s="50">
+      <c r="E13" s="49">
         <v>3</v>
       </c>
-      <c r="F13" s="50">
+      <c r="F13" s="49">
         <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="49">
+      <c r="A14" s="48">
         <v>5</v>
       </c>
-      <c r="B14" s="50">
-        <v>0</v>
-      </c>
-      <c r="C14" s="50">
+      <c r="B14" s="49">
+        <v>0</v>
+      </c>
+      <c r="C14" s="49">
         <v>1</v>
       </c>
-      <c r="D14" s="50">
+      <c r="D14" s="49">
         <v>2</v>
       </c>
-      <c r="E14" s="50">
+      <c r="E14" s="49">
         <v>1</v>
       </c>
-      <c r="F14" s="50">
+      <c r="F14" s="49">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="49">
+      <c r="A15" s="48">
         <v>6</v>
       </c>
-      <c r="B15" s="50">
+      <c r="B15" s="49">
         <v>1</v>
       </c>
-      <c r="C15" s="50">
+      <c r="C15" s="49">
         <v>2</v>
       </c>
-      <c r="D15" s="50">
+      <c r="D15" s="49">
         <v>3</v>
       </c>
-      <c r="E15" s="50">
+      <c r="E15" s="49">
         <v>2</v>
       </c>
-      <c r="F15" s="50">
+      <c r="F15" s="49">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="49">
+      <c r="A16" s="48">
         <v>7</v>
       </c>
-      <c r="B16" s="50">
+      <c r="B16" s="49">
         <v>2</v>
       </c>
-      <c r="C16" s="50">
+      <c r="C16" s="49">
         <v>1</v>
       </c>
-      <c r="D16" s="50">
-        <v>0</v>
-      </c>
-      <c r="E16" s="50">
+      <c r="D16" s="49">
+        <v>0</v>
+      </c>
+      <c r="E16" s="49">
         <v>1</v>
       </c>
-      <c r="F16" s="50">
+      <c r="F16" s="49">
         <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="49">
+      <c r="A17" s="48">
         <v>8</v>
       </c>
-      <c r="B17" s="50">
+      <c r="B17" s="49">
         <v>3</v>
       </c>
-      <c r="C17" s="50">
+      <c r="C17" s="49">
         <v>2</v>
       </c>
-      <c r="D17" s="50">
+      <c r="D17" s="49">
         <v>1</v>
       </c>
-      <c r="E17" s="50">
+      <c r="E17" s="49">
         <v>2</v>
       </c>
-      <c r="F17" s="50">
+      <c r="F17" s="49">
         <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="49">
+      <c r="A18" s="48">
         <v>9</v>
       </c>
-      <c r="B18" s="50">
-        <v>0</v>
-      </c>
-      <c r="C18" s="50">
+      <c r="B18" s="49">
+        <v>0</v>
+      </c>
+      <c r="C18" s="49">
         <v>1</v>
       </c>
-      <c r="D18" s="50">
-        <v>0</v>
-      </c>
-      <c r="E18" s="50">
+      <c r="D18" s="49">
+        <v>0</v>
+      </c>
+      <c r="E18" s="49">
         <v>1</v>
       </c>
-      <c r="F18" s="50">
+      <c r="F18" s="49">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="49">
+      <c r="A19" s="48">
         <v>10</v>
       </c>
-      <c r="B19" s="50">
+      <c r="B19" s="49">
         <v>1</v>
       </c>
-      <c r="C19" s="50">
-        <v>0</v>
-      </c>
-      <c r="D19" s="50">
+      <c r="C19" s="49">
+        <v>0</v>
+      </c>
+      <c r="D19" s="49">
         <v>1</v>
       </c>
-      <c r="E19" s="50">
-        <v>0</v>
-      </c>
-      <c r="F19" s="50">
+      <c r="E19" s="49">
+        <v>0</v>
+      </c>
+      <c r="F19" s="49">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="49">
+      <c r="A20" s="48">
         <v>11</v>
       </c>
-      <c r="B20" s="50">
+      <c r="B20" s="49">
         <v>2</v>
       </c>
-      <c r="C20" s="50">
+      <c r="C20" s="49">
         <v>3</v>
       </c>
-      <c r="D20" s="50">
+      <c r="D20" s="49">
         <v>2</v>
       </c>
-      <c r="E20" s="50">
+      <c r="E20" s="49">
         <v>3</v>
       </c>
-      <c r="F20" s="50">
+      <c r="F20" s="49">
         <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="49">
+      <c r="A21" s="48">
         <v>12</v>
       </c>
-      <c r="B21" s="50">
+      <c r="B21" s="49">
         <v>3</v>
       </c>
-      <c r="C21" s="50">
+      <c r="C21" s="49">
         <v>2</v>
       </c>
-      <c r="D21" s="50">
+      <c r="D21" s="49">
         <v>3</v>
       </c>
-      <c r="E21" s="50">
+      <c r="E21" s="49">
         <v>2</v>
       </c>
-      <c r="F21" s="50">
+      <c r="F21" s="49">
         <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="49">
+      <c r="A22" s="48">
         <v>13</v>
       </c>
-      <c r="B22" s="50">
+      <c r="B22" s="49">
         <v>1</v>
       </c>
-      <c r="C22" s="50">
+      <c r="C22" s="49">
         <v>2</v>
       </c>
-      <c r="D22" s="50">
+      <c r="D22" s="49">
         <v>1</v>
       </c>
-      <c r="E22" s="50">
+      <c r="E22" s="49">
         <v>2</v>
       </c>
-      <c r="F22" s="50">
+      <c r="F22" s="49">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="49">
+      <c r="A23" s="48">
         <v>14</v>
       </c>
-      <c r="B23" s="50">
+      <c r="B23" s="49">
         <v>2</v>
       </c>
-      <c r="C23" s="50">
+      <c r="C23" s="49">
         <v>1</v>
       </c>
-      <c r="D23" s="50">
+      <c r="D23" s="49">
         <v>2</v>
       </c>
-      <c r="E23" s="50">
+      <c r="E23" s="49">
         <v>1</v>
       </c>
-      <c r="F23" s="50">
+      <c r="F23" s="49">
         <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="49">
+      <c r="A24" s="48">
         <v>15</v>
       </c>
-      <c r="B24" s="50">
-        <v>0</v>
-      </c>
-      <c r="C24" s="50">
+      <c r="B24" s="49">
+        <v>0</v>
+      </c>
+      <c r="C24" s="49">
         <v>1</v>
       </c>
-      <c r="D24" s="50">
+      <c r="D24" s="49">
         <v>2</v>
       </c>
-      <c r="E24" s="50">
+      <c r="E24" s="49">
         <v>3</v>
       </c>
-      <c r="F24" s="50">
+      <c r="F24" s="49">
         <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="49">
+      <c r="A25" s="48">
         <v>16</v>
       </c>
-      <c r="B25" s="50">
+      <c r="B25" s="49">
         <v>3</v>
       </c>
-      <c r="C25" s="50">
+      <c r="C25" s="49">
         <v>2</v>
       </c>
-      <c r="D25" s="50">
+      <c r="D25" s="49">
         <v>1</v>
       </c>
-      <c r="E25" s="50">
-        <v>0</v>
-      </c>
-      <c r="F25" s="50">
+      <c r="E25" s="49">
+        <v>0</v>
+      </c>
+      <c r="F25" s="49">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="49">
+      <c r="A26" s="48">
         <v>17</v>
       </c>
-      <c r="B26" s="50">
-        <v>0</v>
-      </c>
-      <c r="C26" s="50">
-        <v>0</v>
-      </c>
-      <c r="D26" s="50">
+      <c r="B26" s="49">
+        <v>0</v>
+      </c>
+      <c r="C26" s="49">
+        <v>0</v>
+      </c>
+      <c r="D26" s="49">
         <v>1</v>
       </c>
-      <c r="E26" s="50">
-        <v>0</v>
-      </c>
-      <c r="F26" s="50">
+      <c r="E26" s="49">
+        <v>0</v>
+      </c>
+      <c r="F26" s="49">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="49">
+      <c r="A27" s="48">
         <v>18</v>
       </c>
-      <c r="B27" s="50">
+      <c r="B27" s="49">
         <v>1</v>
       </c>
-      <c r="C27" s="50">
+      <c r="C27" s="49">
         <v>1</v>
       </c>
-      <c r="D27" s="50">
-        <v>0</v>
-      </c>
-      <c r="E27" s="50">
+      <c r="D27" s="49">
+        <v>0</v>
+      </c>
+      <c r="E27" s="49">
         <v>1</v>
       </c>
-      <c r="F27" s="50">
+      <c r="F27" s="49">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="49">
+      <c r="A28" s="48">
         <v>19</v>
       </c>
-      <c r="B28" s="50">
+      <c r="B28" s="49">
         <v>2</v>
       </c>
-      <c r="C28" s="50">
+      <c r="C28" s="49">
         <v>2</v>
       </c>
-      <c r="D28" s="50">
+      <c r="D28" s="49">
         <v>3</v>
       </c>
-      <c r="E28" s="50">
+      <c r="E28" s="49">
         <v>2</v>
       </c>
-      <c r="F28" s="50">
+      <c r="F28" s="49">
         <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="49">
+      <c r="A29" s="48">
         <v>20</v>
       </c>
-      <c r="B29" s="50">
+      <c r="B29" s="49">
         <v>3</v>
       </c>
-      <c r="C29" s="50">
+      <c r="C29" s="49">
         <v>3</v>
       </c>
-      <c r="D29" s="50">
+      <c r="D29" s="49">
         <v>2</v>
       </c>
-      <c r="E29" s="50">
+      <c r="E29" s="49">
         <v>3</v>
       </c>
-      <c r="F29" s="50">
+      <c r="F29" s="49">
         <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="49">
+      <c r="A30" s="48">
         <v>21</v>
       </c>
-      <c r="B30" s="50">
+      <c r="B30" s="49">
         <v>1</v>
       </c>
-      <c r="C30" s="50">
+      <c r="C30" s="49">
         <v>1</v>
       </c>
-      <c r="D30" s="50">
+      <c r="D30" s="49">
         <v>2</v>
       </c>
-      <c r="E30" s="50">
+      <c r="E30" s="49">
         <v>1</v>
       </c>
-      <c r="F30" s="50">
+      <c r="F30" s="49">
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="49">
+      <c r="A31" s="48">
         <v>22</v>
       </c>
-      <c r="B31" s="50">
+      <c r="B31" s="49">
         <v>2</v>
       </c>
-      <c r="C31" s="50">
+      <c r="C31" s="49">
         <v>2</v>
       </c>
-      <c r="D31" s="50">
+      <c r="D31" s="49">
         <v>1</v>
       </c>
-      <c r="E31" s="50">
+      <c r="E31" s="49">
         <v>2</v>
       </c>
-      <c r="F31" s="50">
+      <c r="F31" s="49">
         <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="49">
+      <c r="A32" s="48">
         <v>23</v>
       </c>
-      <c r="B32" s="50">
-        <v>0</v>
-      </c>
-      <c r="C32" s="50">
-        <v>0</v>
-      </c>
-      <c r="D32" s="50">
+      <c r="B32" s="49">
+        <v>0</v>
+      </c>
+      <c r="C32" s="49">
+        <v>0</v>
+      </c>
+      <c r="D32" s="49">
         <v>2</v>
       </c>
-      <c r="E32" s="50">
-        <v>0</v>
-      </c>
-      <c r="F32" s="50">
+      <c r="E32" s="49">
+        <v>0</v>
+      </c>
+      <c r="F32" s="49">
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="49">
+      <c r="A33" s="48">
         <v>24</v>
       </c>
-      <c r="B33" s="50">
+      <c r="B33" s="49">
         <v>1</v>
       </c>
-      <c r="C33" s="50">
+      <c r="C33" s="49">
         <v>1</v>
       </c>
-      <c r="D33" s="50">
+      <c r="D33" s="49">
         <v>3</v>
       </c>
-      <c r="E33" s="50">
+      <c r="E33" s="49">
         <v>1</v>
       </c>
-      <c r="F33" s="50">
+      <c r="F33" s="49">
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" s="49">
+      <c r="A34" s="48">
         <v>25</v>
       </c>
-      <c r="B34" s="50">
+      <c r="B34" s="49">
         <v>2</v>
       </c>
-      <c r="C34" s="50">
+      <c r="C34" s="49">
         <v>2</v>
       </c>
-      <c r="D34" s="50">
-        <v>0</v>
-      </c>
-      <c r="E34" s="50">
+      <c r="D34" s="49">
+        <v>0</v>
+      </c>
+      <c r="E34" s="49">
         <v>2</v>
       </c>
-      <c r="F34" s="50">
+      <c r="F34" s="49">
         <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:6">
-      <c r="A35" s="49">
+      <c r="A35" s="48">
         <v>26</v>
       </c>
-      <c r="B35" s="50">
+      <c r="B35" s="49">
         <v>3</v>
       </c>
-      <c r="C35" s="50">
+      <c r="C35" s="49">
         <v>3</v>
       </c>
-      <c r="D35" s="50">
+      <c r="D35" s="49">
         <v>1</v>
       </c>
-      <c r="E35" s="50">
+      <c r="E35" s="49">
         <v>3</v>
       </c>
-      <c r="F35" s="50">
+      <c r="F35" s="49">
         <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:6">
-      <c r="A36" s="49">
+      <c r="A36" s="48">
         <v>27</v>
       </c>
-      <c r="B36" s="50">
-        <v>0</v>
-      </c>
-      <c r="C36" s="50">
-        <v>0</v>
-      </c>
-      <c r="D36" s="50">
+      <c r="B36" s="49">
+        <v>0</v>
+      </c>
+      <c r="C36" s="49">
+        <v>0</v>
+      </c>
+      <c r="D36" s="49">
         <v>3</v>
       </c>
-      <c r="E36" s="50">
-        <v>0</v>
-      </c>
-      <c r="F36" s="50">
+      <c r="E36" s="49">
+        <v>0</v>
+      </c>
+      <c r="F36" s="49">
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="49">
+      <c r="A37" s="48">
         <v>28</v>
       </c>
-      <c r="B37" s="50">
+      <c r="B37" s="49">
         <v>3</v>
       </c>
-      <c r="C37" s="50">
+      <c r="C37" s="49">
         <v>3</v>
       </c>
-      <c r="D37" s="50">
-        <v>0</v>
-      </c>
-      <c r="E37" s="50">
+      <c r="D37" s="49">
+        <v>0</v>
+      </c>
+      <c r="E37" s="49">
         <v>3</v>
       </c>
-      <c r="F37" s="50">
+      <c r="F37" s="49">
         <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" s="49">
+      <c r="A38" s="48">
         <v>29</v>
       </c>
-      <c r="B38" s="50">
+      <c r="B38" s="49">
         <v>1</v>
       </c>
-      <c r="C38" s="50">
-        <v>0</v>
-      </c>
-      <c r="D38" s="50">
+      <c r="C38" s="49">
+        <v>0</v>
+      </c>
+      <c r="D38" s="49">
         <v>1</v>
       </c>
-      <c r="E38" s="50">
+      <c r="E38" s="49">
         <v>2</v>
       </c>
-      <c r="F38" s="50">
+      <c r="F38" s="49">
         <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="49">
+      <c r="A39" s="48">
         <v>30</v>
       </c>
-      <c r="B39" s="50">
+      <c r="B39" s="49">
         <v>2</v>
       </c>
-      <c r="C39" s="50">
+      <c r="C39" s="49">
         <v>3</v>
       </c>
-      <c r="D39" s="50">
+      <c r="D39" s="49">
         <v>2</v>
       </c>
-      <c r="E39" s="50">
+      <c r="E39" s="49">
         <v>1</v>
       </c>
-      <c r="F39" s="50">
+      <c r="F39" s="49">
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" s="49">
+      <c r="A40" s="48">
         <v>31</v>
       </c>
-      <c r="B40" s="50">
-        <v>0</v>
-      </c>
-      <c r="C40" s="50">
-        <v>0</v>
-      </c>
-      <c r="D40" s="50">
+      <c r="B40" s="49">
+        <v>0</v>
+      </c>
+      <c r="C40" s="49">
+        <v>0</v>
+      </c>
+      <c r="D40" s="49">
         <v>1</v>
       </c>
-      <c r="E40" s="50">
+      <c r="E40" s="49">
         <v>2</v>
       </c>
-      <c r="F40" s="50">
+      <c r="F40" s="49">
         <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:6">
-      <c r="A41" s="49">
+      <c r="A41" s="48">
         <v>32</v>
       </c>
-      <c r="B41" s="50">
+      <c r="B41" s="49">
         <v>1</v>
       </c>
-      <c r="C41" s="50">
+      <c r="C41" s="49">
         <v>1</v>
       </c>
-      <c r="D41" s="50">
+      <c r="D41" s="49">
         <v>2</v>
       </c>
-      <c r="E41" s="50">
+      <c r="E41" s="49">
         <v>3</v>
       </c>
-      <c r="F41" s="50">
+      <c r="F41" s="49">
         <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" s="49">
+      <c r="A42" s="48">
         <v>33</v>
       </c>
-      <c r="B42" s="50">
+      <c r="B42" s="49">
         <v>2</v>
       </c>
-      <c r="C42" s="50">
+      <c r="C42" s="49">
         <v>2</v>
       </c>
-      <c r="D42" s="50">
+      <c r="D42" s="49">
         <v>1</v>
       </c>
-      <c r="E42" s="50">
-        <v>0</v>
-      </c>
-      <c r="F42" s="50">
+      <c r="E42" s="49">
+        <v>0</v>
+      </c>
+      <c r="F42" s="49">
         <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:6">
-      <c r="A43" s="49">
+      <c r="A43" s="48">
         <v>34</v>
       </c>
-      <c r="B43" s="50">
+      <c r="B43" s="49">
         <v>3</v>
       </c>
-      <c r="C43" s="50">
+      <c r="C43" s="49">
         <v>3</v>
       </c>
-      <c r="D43" s="50">
+      <c r="D43" s="49">
         <v>2</v>
       </c>
-      <c r="E43" s="50">
+      <c r="E43" s="49">
         <v>1</v>
       </c>
-      <c r="F43" s="50">
+      <c r="F43" s="49">
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:6">
-      <c r="A44" s="49">
+      <c r="A44" s="48">
         <v>35</v>
       </c>
-      <c r="B44" s="50">
-        <v>0</v>
-      </c>
-      <c r="C44" s="50">
+      <c r="B44" s="49">
+        <v>0</v>
+      </c>
+      <c r="C44" s="49">
         <v>1</v>
       </c>
-      <c r="D44" s="50">
+      <c r="D44" s="49">
         <v>2</v>
       </c>
-      <c r="E44" s="50">
+      <c r="E44" s="49">
         <v>3</v>
       </c>
-      <c r="F44" s="50">
+      <c r="F44" s="49">
         <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:6">
-      <c r="A45" s="49">
+      <c r="A45" s="48">
         <v>36</v>
       </c>
-      <c r="B45" s="50">
+      <c r="B45" s="49">
         <v>1</v>
       </c>
-      <c r="C45" s="50">
-        <v>0</v>
-      </c>
-      <c r="D45" s="50">
+      <c r="C45" s="49">
+        <v>0</v>
+      </c>
+      <c r="D45" s="49">
         <v>1</v>
       </c>
-      <c r="E45" s="50">
+      <c r="E45" s="49">
         <v>2</v>
       </c>
-      <c r="F45" s="50">
+      <c r="F45" s="49">
         <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:6">
-      <c r="A46" s="49">
+      <c r="A46" s="48">
         <v>37</v>
       </c>
-      <c r="B46" s="50">
+      <c r="B46" s="49">
         <v>2</v>
       </c>
-      <c r="C46" s="50">
+      <c r="C46" s="49">
         <v>3</v>
       </c>
-      <c r="D46" s="50">
+      <c r="D46" s="49">
         <v>2</v>
       </c>
-      <c r="E46" s="50">
+      <c r="E46" s="49">
         <v>1</v>
       </c>
-      <c r="F46" s="50">
+      <c r="F46" s="49">
         <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:6">
-      <c r="A47" s="49">
+      <c r="A47" s="48">
         <v>38</v>
       </c>
-      <c r="B47" s="50">
+      <c r="B47" s="49">
         <v>3</v>
       </c>
-      <c r="C47" s="50">
+      <c r="C47" s="49">
         <v>2</v>
       </c>
-      <c r="D47" s="50">
+      <c r="D47" s="49">
         <v>1</v>
       </c>
-      <c r="E47" s="50">
-        <v>0</v>
-      </c>
-      <c r="F47" s="50">
+      <c r="E47" s="49">
+        <v>0</v>
+      </c>
+      <c r="F47" s="49">
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:6">
-      <c r="A48" s="49">
+      <c r="A48" s="48">
         <v>39</v>
       </c>
-      <c r="B48" s="50">
-        <v>0</v>
-      </c>
-      <c r="C48" s="50">
-        <v>0</v>
-      </c>
-      <c r="D48" s="50">
+      <c r="B48" s="49">
+        <v>0</v>
+      </c>
+      <c r="C48" s="49">
+        <v>0</v>
+      </c>
+      <c r="D48" s="49">
         <v>1</v>
       </c>
-      <c r="E48" s="50">
+      <c r="E48" s="49">
         <v>1</v>
       </c>
-      <c r="F48" s="50">
+      <c r="F48" s="49">
         <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:6">
-      <c r="A49" s="49">
+      <c r="A49" s="48">
         <v>40</v>
       </c>
-      <c r="B49" s="50">
+      <c r="B49" s="49">
         <v>1</v>
       </c>
-      <c r="C49" s="50">
+      <c r="C49" s="49">
         <v>1</v>
       </c>
-      <c r="D49" s="50">
-        <v>0</v>
-      </c>
-      <c r="E49" s="50">
-        <v>0</v>
-      </c>
-      <c r="F49" s="50">
+      <c r="D49" s="49">
+        <v>0</v>
+      </c>
+      <c r="E49" s="49">
+        <v>0</v>
+      </c>
+      <c r="F49" s="49">
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" s="49">
+      <c r="A50" s="48">
         <v>41</v>
       </c>
-      <c r="B50" s="50">
+      <c r="B50" s="49">
         <v>2</v>
       </c>
-      <c r="C50" s="50">
+      <c r="C50" s="49">
         <v>2</v>
       </c>
-      <c r="D50" s="50">
+      <c r="D50" s="49">
         <v>3</v>
       </c>
-      <c r="E50" s="50">
+      <c r="E50" s="49">
         <v>3</v>
       </c>
-      <c r="F50" s="50">
+      <c r="F50" s="49">
         <v>3</v>
       </c>
     </row>
     <row r="51" spans="1:6">
-      <c r="A51" s="49">
+      <c r="A51" s="48">
         <v>42</v>
       </c>
-      <c r="B51" s="50">
+      <c r="B51" s="49">
         <v>3</v>
       </c>
-      <c r="C51" s="50">
+      <c r="C51" s="49">
         <v>3</v>
       </c>
-      <c r="D51" s="50">
+      <c r="D51" s="49">
         <v>2</v>
       </c>
-      <c r="E51" s="50">
+      <c r="E51" s="49">
         <v>2</v>
       </c>
-      <c r="F51" s="50">
+      <c r="F51" s="49">
         <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:6">
-      <c r="A52" s="49">
+      <c r="A52" s="48">
         <v>43</v>
       </c>
-      <c r="B52" s="50">
-        <v>0</v>
-      </c>
-      <c r="C52" s="50">
-        <v>0</v>
-      </c>
-      <c r="D52" s="50">
-        <v>0</v>
-      </c>
-      <c r="E52" s="50">
+      <c r="B52" s="49">
+        <v>0</v>
+      </c>
+      <c r="C52" s="49">
+        <v>0</v>
+      </c>
+      <c r="D52" s="49">
+        <v>0</v>
+      </c>
+      <c r="E52" s="49">
         <v>1</v>
       </c>
-      <c r="F52" s="50">
+      <c r="F52" s="49">
         <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:6">
-      <c r="A53" s="49">
+      <c r="A53" s="48">
         <v>44</v>
       </c>
-      <c r="B53" s="50">
+      <c r="B53" s="49">
         <v>1</v>
       </c>
-      <c r="C53" s="50">
+      <c r="C53" s="49">
         <v>1</v>
       </c>
-      <c r="D53" s="50">
+      <c r="D53" s="49">
         <v>1</v>
       </c>
-      <c r="E53" s="50">
-        <v>0</v>
-      </c>
-      <c r="F53" s="50">
+      <c r="E53" s="49">
+        <v>0</v>
+      </c>
+      <c r="F53" s="49">
         <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" s="49">
+      <c r="A54" s="48">
         <v>45</v>
       </c>
-      <c r="B54" s="50">
+      <c r="B54" s="49">
         <v>2</v>
       </c>
-      <c r="C54" s="50">
+      <c r="C54" s="49">
         <v>2</v>
       </c>
-      <c r="D54" s="50">
+      <c r="D54" s="49">
         <v>2</v>
       </c>
-      <c r="E54" s="50">
+      <c r="E54" s="49">
         <v>3</v>
       </c>
-      <c r="F54" s="50">
+      <c r="F54" s="49">
         <v>3</v>
       </c>
     </row>
     <row r="55" spans="1:6">
-      <c r="A55" s="49">
+      <c r="A55" s="48">
         <v>46</v>
       </c>
-      <c r="B55" s="50">
+      <c r="B55" s="49">
         <v>3</v>
       </c>
-      <c r="C55" s="50">
+      <c r="C55" s="49">
         <v>3</v>
       </c>
-      <c r="D55" s="50">
+      <c r="D55" s="49">
         <v>3</v>
       </c>
-      <c r="E55" s="50">
+      <c r="E55" s="49">
         <v>2</v>
       </c>
-      <c r="F55" s="50">
+      <c r="F55" s="49">
         <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:6">
-      <c r="A56" s="49">
+      <c r="A56" s="48">
         <v>47</v>
       </c>
-      <c r="B56" s="50">
+      <c r="B56" s="49">
         <v>1</v>
       </c>
-      <c r="C56" s="50">
+      <c r="C56" s="49">
         <v>1</v>
       </c>
-      <c r="D56" s="50">
+      <c r="D56" s="49">
         <v>2</v>
       </c>
-      <c r="E56" s="50">
+      <c r="E56" s="49">
         <v>2</v>
       </c>
-      <c r="F56" s="50">
+      <c r="F56" s="49">
         <v>2</v>
       </c>
     </row>
     <row r="57" spans="1:6">
-      <c r="A57" s="49">
+      <c r="A57" s="48">
         <v>48</v>
       </c>
-      <c r="B57" s="50">
+      <c r="B57" s="49">
         <v>2</v>
       </c>
-      <c r="C57" s="50">
+      <c r="C57" s="49">
         <v>2</v>
       </c>
-      <c r="D57" s="50">
+      <c r="D57" s="49">
         <v>1</v>
       </c>
-      <c r="E57" s="50">
+      <c r="E57" s="49">
         <v>1</v>
       </c>
-      <c r="F57" s="50">
+      <c r="F57" s="49">
         <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:6">
-      <c r="A58" s="49">
+      <c r="A58" s="48">
         <v>49</v>
       </c>
-      <c r="B58" s="50">
+      <c r="B58" s="49">
         <v>1</v>
       </c>
-      <c r="C58" s="50">
+      <c r="C58" s="49">
         <v>1</v>
       </c>
-      <c r="D58" s="50">
+      <c r="D58" s="49">
         <v>1</v>
       </c>
-      <c r="E58" s="50">
+      <c r="E58" s="49">
         <v>2</v>
       </c>
-      <c r="F58" s="50">
+      <c r="F58" s="49">
         <v>2</v>
       </c>
     </row>
     <row r="59" spans="1:6">
-      <c r="A59" s="49">
+      <c r="A59" s="48">
         <v>50</v>
       </c>
-      <c r="B59" s="50">
+      <c r="B59" s="49">
         <v>2</v>
       </c>
-      <c r="C59" s="50">
+      <c r="C59" s="49">
         <v>2</v>
       </c>
-      <c r="D59" s="50">
+      <c r="D59" s="49">
         <v>2</v>
       </c>
-      <c r="E59" s="50">
+      <c r="E59" s="49">
         <v>1</v>
       </c>
-      <c r="F59" s="50">
+      <c r="F59" s="49">
         <v>1</v>
       </c>
     </row>
@@ -3143,6 +2867,284 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="B3:G15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:7">
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <v>4</v>
+      </c>
+      <c r="G3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>50</v>
+      </c>
+      <c r="F4">
+        <v>200</v>
+      </c>
+      <c r="G4">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>30</v>
+      </c>
+      <c r="F5">
+        <v>150</v>
+      </c>
+      <c r="G5">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7">
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>25</v>
+      </c>
+      <c r="F6">
+        <v>125</v>
+      </c>
+      <c r="G6">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7">
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>20</v>
+      </c>
+      <c r="F7">
+        <v>100</v>
+      </c>
+      <c r="G7">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7">
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>20</v>
+      </c>
+      <c r="F8">
+        <v>100</v>
+      </c>
+      <c r="G8">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7">
+      <c r="B9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>20</v>
+      </c>
+      <c r="F9">
+        <v>100</v>
+      </c>
+      <c r="G9">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7">
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>10</v>
+      </c>
+      <c r="F10">
+        <v>75</v>
+      </c>
+      <c r="G10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7">
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>10</v>
+      </c>
+      <c r="F11">
+        <v>75</v>
+      </c>
+      <c r="G11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7">
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>10</v>
+      </c>
+      <c r="F12">
+        <v>50</v>
+      </c>
+      <c r="G12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7">
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>10</v>
+      </c>
+      <c r="F13">
+        <v>50</v>
+      </c>
+      <c r="G13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7">
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>10</v>
+      </c>
+      <c r="F14">
+        <v>50</v>
+      </c>
+      <c r="G14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7">
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -3284,8 +3286,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B2:Z198"/>
   <sheetViews>
-    <sheetView topLeftCell="A124" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J160" sqref="J160"/>
+    <sheetView tabSelected="1" topLeftCell="A123" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K184" sqref="K184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -3416,7 +3418,7 @@
         <v>8</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G7" s="20" t="s">
         <v>9</v>
@@ -3522,7 +3524,7 @@
         <v>8</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D12" s="20" t="s">
         <v>7</v>
@@ -3545,7 +3547,7 @@
         <v>9</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D13" s="20" t="s">
         <v>7</v>
@@ -3640,7 +3642,7 @@
         <v>7</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>77</v>
+        <v>11</v>
       </c>
       <c r="E17" s="20" t="s">
         <v>77</v>
@@ -3663,7 +3665,7 @@
         <v>7</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E18" s="20" t="s">
         <v>15</v>
@@ -3689,7 +3691,7 @@
         <v>10</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F19" s="20" t="s">
         <v>10</v>
@@ -3702,7 +3704,7 @@
       </c>
       <c r="I19" s="25">
         <f>I62</f>
-        <v>0.66737081372929807</v>
+        <v>0.5228803972936914</v>
       </c>
     </row>
     <row r="20" spans="2:9">
@@ -3710,7 +3712,7 @@
         <v>16</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D20" s="20" t="s">
         <v>10</v>
@@ -3754,10 +3756,10 @@
         <v>18</v>
       </c>
       <c r="C22" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="20" t="s">
         <v>12</v>
-      </c>
-      <c r="D22" s="20" t="s">
-        <v>9</v>
       </c>
       <c r="E22" s="20" t="s">
         <v>10</v>
@@ -3778,7 +3780,7 @@
         <v>10</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E23" s="20" t="s">
         <v>10</v>
@@ -3838,10 +3840,10 @@
         <v>22</v>
       </c>
       <c r="C26" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="20" t="s">
         <v>9</v>
-      </c>
-      <c r="D26" s="20" t="s">
-        <v>12</v>
       </c>
       <c r="E26" s="20" t="s">
         <v>9</v>
@@ -3862,7 +3864,7 @@
         <v>12</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E27" s="20" t="s">
         <v>9</v>
@@ -3880,10 +3882,10 @@
         <v>24</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>10</v>
+        <v>77</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E28" s="20" t="s">
         <v>14</v>
@@ -3904,7 +3906,7 @@
         <v>14</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E29" s="20" t="s">
         <v>16</v>
@@ -3943,7 +3945,7 @@
         <v>27</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D31" s="20" t="s">
         <v>13</v>
@@ -3991,7 +3993,7 @@
         <v>9</v>
       </c>
       <c r="E33" s="20" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F33" s="20" t="s">
         <v>9</v>
@@ -4222,7 +4224,7 @@
         <v>12</v>
       </c>
       <c r="E44" s="20" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F44" s="20" t="s">
         <v>12</v>
@@ -4282,7 +4284,7 @@
         <v>8</v>
       </c>
       <c r="D47" s="20" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E47" s="20" t="s">
         <v>15</v>
@@ -4387,7 +4389,7 @@
         <v>10</v>
       </c>
       <c r="D52" s="20" t="s">
-        <v>13</v>
+        <v>77</v>
       </c>
       <c r="E52" s="20" t="s">
         <v>15</v>
@@ -4408,7 +4410,7 @@
         <v>77</v>
       </c>
       <c r="D53" s="20" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E53" s="20" t="s">
         <v>13</v>
@@ -4429,7 +4431,7 @@
         <v>77</v>
       </c>
       <c r="D54" s="20" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E54" s="20" t="s">
         <v>16</v>
@@ -4447,7 +4449,7 @@
         <v>51</v>
       </c>
       <c r="C55" s="20" t="s">
-        <v>77</v>
+        <v>15</v>
       </c>
       <c r="D55" s="20" t="s">
         <v>11</v>
@@ -4470,13 +4472,13 @@
       <c r="C56" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="D56" s="53" t="s">
+      <c r="D56" s="52" t="s">
         <v>14</v>
       </c>
       <c r="E56" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="F56" s="53" t="s">
+      <c r="F56" s="52" t="s">
         <v>14</v>
       </c>
       <c r="G56" s="20" t="s">
@@ -4534,7 +4536,7 @@
         <v>14</v>
       </c>
       <c r="D59" s="20" t="s">
-        <v>77</v>
+        <v>14</v>
       </c>
       <c r="E59" s="20" t="s">
         <v>77</v>
@@ -4552,7 +4554,7 @@
         <v>56</v>
       </c>
       <c r="C60" s="20" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D60" s="20" t="s">
         <v>15</v>
@@ -4573,7 +4575,7 @@
         <v>57</v>
       </c>
       <c r="C61" s="20" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D61" s="20" t="s">
         <v>77</v>
@@ -4611,7 +4613,7 @@
       <c r="H62" s="36"/>
       <c r="I62" s="25">
         <f>I127</f>
-        <v>0.66737081372929807</v>
+        <v>0.5228803972936914</v>
       </c>
     </row>
     <row r="63" spans="2:9">
@@ -4622,7 +4624,7 @@
         <v>77</v>
       </c>
       <c r="D63" s="20" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E63" s="20" t="s">
         <v>7</v>
@@ -4640,10 +4642,10 @@
         <v>60</v>
       </c>
       <c r="C64" s="20" t="s">
-        <v>15</v>
+        <v>77</v>
       </c>
       <c r="D64" s="20" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E64" s="20" t="s">
         <v>5</v>
@@ -4667,7 +4669,7 @@
         <v>10</v>
       </c>
       <c r="E65" s="20" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F65" s="20" t="s">
         <v>10</v>
@@ -4727,7 +4729,7 @@
         <v>5</v>
       </c>
       <c r="D68" s="20" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E68" s="20" t="s">
         <v>11</v>
@@ -4745,7 +4747,7 @@
         <v>65</v>
       </c>
       <c r="C69" s="20" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D69" s="20" t="s">
         <v>10</v>
@@ -4769,7 +4771,7 @@
         <v>7</v>
       </c>
       <c r="D70" s="20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E70" s="20" t="s">
         <v>11</v>
@@ -4793,7 +4795,7 @@
         <v>12</v>
       </c>
       <c r="E71" s="20" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F71" s="20" t="s">
         <v>12</v>
@@ -4829,7 +4831,7 @@
         <v>69</v>
       </c>
       <c r="C73" s="20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D73" s="20" t="s">
         <v>12</v>
@@ -4856,7 +4858,7 @@
         <v>8</v>
       </c>
       <c r="E74" s="20" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F74" s="20" t="s">
         <v>8</v>
@@ -4871,7 +4873,7 @@
         <v>71</v>
       </c>
       <c r="C75" s="20" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D75" s="20" t="s">
         <v>8</v>
@@ -4997,10 +4999,10 @@
         <v>77</v>
       </c>
       <c r="C81" s="20" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D81" s="20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E81" s="20" t="s">
         <v>59</v>
@@ -5018,7 +5020,7 @@
         <v>78</v>
       </c>
       <c r="C82" s="20" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D82" s="20" t="s">
         <v>7</v>
@@ -5063,7 +5065,7 @@
         <v>59</v>
       </c>
       <c r="D84" s="20" t="s">
-        <v>77</v>
+        <v>13</v>
       </c>
       <c r="E84" s="20" t="s">
         <v>59</v>
@@ -5084,7 +5086,7 @@
         <v>59</v>
       </c>
       <c r="D85" s="20" t="s">
-        <v>77</v>
+        <v>14</v>
       </c>
       <c r="E85" s="20" t="s">
         <v>59</v>
@@ -5105,7 +5107,7 @@
         <v>59</v>
       </c>
       <c r="D86" s="20" t="s">
-        <v>77</v>
+        <v>14</v>
       </c>
       <c r="E86" s="20" t="s">
         <v>59</v>
@@ -5126,7 +5128,7 @@
         <v>59</v>
       </c>
       <c r="D87" s="20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E87" s="20" t="s">
         <v>59</v>
@@ -5147,7 +5149,7 @@
         <v>59</v>
       </c>
       <c r="D88" s="20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E88" s="20" t="s">
         <v>10</v>
@@ -5168,7 +5170,7 @@
         <v>59</v>
       </c>
       <c r="D89" s="20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E89" s="20" t="s">
         <v>10</v>
@@ -5189,7 +5191,7 @@
         <v>59</v>
       </c>
       <c r="D90" s="20" t="s">
-        <v>77</v>
+        <v>14</v>
       </c>
       <c r="E90" s="20" t="s">
         <v>16</v>
@@ -5210,10 +5212,10 @@
         <v>59</v>
       </c>
       <c r="D91" s="20" t="s">
-        <v>77</v>
+        <v>15</v>
       </c>
       <c r="E91" s="20" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F91" s="20" t="s">
         <v>77</v>
@@ -5255,7 +5257,7 @@
         <v>14</v>
       </c>
       <c r="E93" s="20" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F93" s="20" t="s">
         <v>14</v>
@@ -5291,13 +5293,13 @@
         <v>91</v>
       </c>
       <c r="C95" s="20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D95" s="20" t="s">
         <v>10</v>
       </c>
       <c r="E95" s="20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F95" s="20" t="s">
         <v>10</v>
@@ -5318,7 +5320,7 @@
         <v>10</v>
       </c>
       <c r="E96" s="20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F96" s="20" t="s">
         <v>10</v>
@@ -5328,7 +5330,7 @@
       </c>
       <c r="H96" s="36"/>
     </row>
-    <row r="97" spans="2:8">
+    <row r="97" spans="2:9">
       <c r="B97" s="16">
         <v>93</v>
       </c>
@@ -5339,7 +5341,7 @@
         <v>10</v>
       </c>
       <c r="E97" s="20" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F97" s="20" t="s">
         <v>10</v>
@@ -5349,7 +5351,7 @@
       </c>
       <c r="H97" s="36"/>
     </row>
-    <row r="98" spans="2:8">
+    <row r="98" spans="2:9">
       <c r="B98" s="16">
         <v>94</v>
       </c>
@@ -5360,7 +5362,7 @@
         <v>14</v>
       </c>
       <c r="E98" s="20" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F98" s="20" t="s">
         <v>14</v>
@@ -5370,18 +5372,18 @@
       </c>
       <c r="H98" s="36"/>
     </row>
-    <row r="99" spans="2:8">
+    <row r="99" spans="2:9">
       <c r="B99" s="16">
         <v>95</v>
       </c>
       <c r="C99" s="20" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D99" s="20" t="s">
         <v>14</v>
       </c>
       <c r="E99" s="20" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F99" s="20" t="s">
         <v>11</v>
@@ -5391,15 +5393,15 @@
       </c>
       <c r="H99" s="36"/>
     </row>
-    <row r="100" spans="2:8">
+    <row r="100" spans="2:9">
       <c r="B100" s="16">
         <v>96</v>
       </c>
       <c r="C100" s="20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D100" s="20" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E100" s="20" t="s">
         <v>15</v>
@@ -5411,16 +5413,20 @@
         <v>14</v>
       </c>
       <c r="H100" s="36"/>
-    </row>
-    <row r="101" spans="2:8">
+      <c r="I100" s="25">
+        <f>I127</f>
+        <v>0.5228803972936914</v>
+      </c>
+    </row>
+    <row r="101" spans="2:9">
       <c r="B101" s="16">
         <v>97</v>
       </c>
       <c r="C101" s="20" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D101" s="20" t="s">
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="E101" s="20" t="s">
         <v>77</v>
@@ -5433,12 +5439,12 @@
       </c>
       <c r="H101" s="36"/>
     </row>
-    <row r="102" spans="2:8">
+    <row r="102" spans="2:9">
       <c r="B102" s="16">
         <v>98</v>
       </c>
       <c r="C102" s="20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D102" s="20" t="s">
         <v>77</v>
@@ -5454,7 +5460,7 @@
       </c>
       <c r="H102" s="36"/>
     </row>
-    <row r="103" spans="2:8">
+    <row r="103" spans="2:9">
       <c r="B103" s="16">
         <v>99</v>
       </c>
@@ -5475,7 +5481,7 @@
       </c>
       <c r="H103" s="36"/>
     </row>
-    <row r="104" spans="2:8">
+    <row r="104" spans="2:9">
       <c r="B104" s="16">
         <v>100</v>
       </c>
@@ -5496,7 +5502,7 @@
       </c>
       <c r="H104" s="36"/>
     </row>
-    <row r="105" spans="2:8">
+    <row r="105" spans="2:9">
       <c r="B105" s="16">
         <v>101</v>
       </c>
@@ -5517,7 +5523,7 @@
       </c>
       <c r="H105" s="36"/>
     </row>
-    <row r="106" spans="2:8">
+    <row r="106" spans="2:9">
       <c r="B106" s="16">
         <v>102</v>
       </c>
@@ -5525,9 +5531,9 @@
         <v>77</v>
       </c>
       <c r="D106" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="E106" s="52" t="s">
+        <v>9</v>
+      </c>
+      <c r="E106" s="51" t="s">
         <v>9</v>
       </c>
       <c r="F106" s="20" t="s">
@@ -5538,7 +5544,7 @@
       </c>
       <c r="H106" s="36"/>
     </row>
-    <row r="107" spans="2:8">
+    <row r="107" spans="2:9">
       <c r="B107" s="16">
         <v>103</v>
       </c>
@@ -5546,7 +5552,7 @@
         <v>15</v>
       </c>
       <c r="D107" s="20" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E107" s="20" t="s">
         <v>9</v>
@@ -5555,11 +5561,11 @@
         <v>15</v>
       </c>
       <c r="G107" s="20" t="s">
-        <v>15</v>
+        <v>77</v>
       </c>
       <c r="H107" s="36"/>
     </row>
-    <row r="108" spans="2:8">
+    <row r="108" spans="2:9">
       <c r="B108" s="16">
         <v>104</v>
       </c>
@@ -5576,11 +5582,11 @@
         <v>9</v>
       </c>
       <c r="G108" s="20" t="s">
-        <v>15</v>
+        <v>77</v>
       </c>
       <c r="H108" s="36"/>
     </row>
-    <row r="109" spans="2:8">
+    <row r="109" spans="2:9">
       <c r="B109" s="16">
         <v>105</v>
       </c>
@@ -5601,7 +5607,7 @@
       </c>
       <c r="H109" s="36"/>
     </row>
-    <row r="110" spans="2:8">
+    <row r="110" spans="2:9">
       <c r="B110" s="16">
         <v>106</v>
       </c>
@@ -5609,7 +5615,7 @@
         <v>77</v>
       </c>
       <c r="D110" s="20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E110" s="20" t="s">
         <v>77</v>
@@ -5622,12 +5628,12 @@
       </c>
       <c r="H110" s="36"/>
     </row>
-    <row r="111" spans="2:8">
+    <row r="111" spans="2:9">
       <c r="B111" s="16">
         <v>107</v>
       </c>
       <c r="C111" s="20" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D111" s="20" t="s">
         <v>7</v>
@@ -5643,7 +5649,7 @@
       </c>
       <c r="H111" s="36"/>
     </row>
-    <row r="112" spans="2:8">
+    <row r="112" spans="2:9">
       <c r="B112" s="16">
         <v>108</v>
       </c>
@@ -5672,7 +5678,7 @@
         <v>14</v>
       </c>
       <c r="D113" s="20" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E113" s="20" t="s">
         <v>77</v>
@@ -5693,7 +5699,7 @@
         <v>77</v>
       </c>
       <c r="D114" s="20" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E114" s="20" t="s">
         <v>15</v>
@@ -5741,7 +5747,7 @@
         <v>7</v>
       </c>
       <c r="F116" s="20" t="s">
-        <v>59</v>
+        <v>13</v>
       </c>
       <c r="G116" s="20" t="s">
         <v>77</v>
@@ -5753,7 +5759,7 @@
         <v>113</v>
       </c>
       <c r="C117" s="20" t="s">
-        <v>77</v>
+        <v>9</v>
       </c>
       <c r="D117" s="20" t="s">
         <v>59</v>
@@ -5774,7 +5780,7 @@
         <v>114</v>
       </c>
       <c r="C118" s="20" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D118" s="20" t="s">
         <v>59</v>
@@ -5795,7 +5801,7 @@
         <v>115</v>
       </c>
       <c r="C119" s="20" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D119" s="20" t="s">
         <v>59</v>
@@ -5822,7 +5828,7 @@
         <v>59</v>
       </c>
       <c r="E120" s="20" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F120" s="20" t="s">
         <v>59</v>
@@ -5843,7 +5849,7 @@
         <v>59</v>
       </c>
       <c r="E121" s="20" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F121" s="20" t="s">
         <v>59</v>
@@ -5882,7 +5888,7 @@
         <v>77</v>
       </c>
       <c r="D123" s="20" t="s">
-        <v>59</v>
+        <v>10</v>
       </c>
       <c r="E123" s="20" t="s">
         <v>13</v>
@@ -5900,10 +5906,10 @@
         <v>120</v>
       </c>
       <c r="C124" s="20" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D124" s="20" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E124" s="20" t="s">
         <v>7</v>
@@ -5921,10 +5927,10 @@
         <v>121</v>
       </c>
       <c r="C125" s="20" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D125" s="20" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E125" s="20" t="s">
         <v>7</v>
@@ -5945,7 +5951,7 @@
         <v>14</v>
       </c>
       <c r="D126" s="20" t="s">
-        <v>77</v>
+        <v>13</v>
       </c>
       <c r="E126" s="20" t="s">
         <v>7</v>
@@ -5963,10 +5969,10 @@
         <v>123</v>
       </c>
       <c r="C127" s="20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D127" s="20" t="s">
-        <v>77</v>
+        <v>10</v>
       </c>
       <c r="E127" s="20" t="s">
         <v>7</v>
@@ -5980,7 +5986,7 @@
       <c r="H127" s="36"/>
       <c r="I127" s="25">
         <f>J147</f>
-        <v>0.66737081372929807</v>
+        <v>0.5228803972936914</v>
       </c>
     </row>
     <row r="128" spans="2:9">
@@ -5994,7 +6000,7 @@
         <v>10</v>
       </c>
       <c r="E128" s="20" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F128" s="20" t="s">
         <v>10</v>
@@ -6015,7 +6021,7 @@
         <v>10</v>
       </c>
       <c r="E129" s="20" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F129" s="20" t="s">
         <v>10</v>
@@ -6054,7 +6060,7 @@
         <v>7</v>
       </c>
       <c r="D131" s="20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E131" s="20" t="s">
         <v>9</v>
@@ -6072,13 +6078,13 @@
         <v>128</v>
       </c>
       <c r="C132" s="20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D132" s="20" t="s">
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="E132" s="20" t="s">
-        <v>77</v>
+        <v>15</v>
       </c>
       <c r="F132" s="20" t="s">
         <v>11</v>
@@ -6093,9 +6099,9 @@
         <v>129</v>
       </c>
       <c r="C133" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="D133" s="54" t="s">
+        <v>15</v>
+      </c>
+      <c r="D133" s="53" t="s">
         <v>12</v>
       </c>
       <c r="E133" s="20" t="s">
@@ -6114,10 +6120,10 @@
         <v>130</v>
       </c>
       <c r="C134" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="D134" s="54" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="D134" s="53" t="s">
+        <v>8</v>
       </c>
       <c r="E134" s="20" t="s">
         <v>9</v>
@@ -6137,10 +6143,10 @@
       <c r="C135" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="D135" s="54" t="s">
-        <v>11</v>
-      </c>
-      <c r="E135" s="52" t="s">
+      <c r="D135" s="53" t="s">
+        <v>12</v>
+      </c>
+      <c r="E135" s="51" t="s">
         <v>15</v>
       </c>
       <c r="F135" s="20" t="s">
@@ -6156,15 +6162,15 @@
         <v>132</v>
       </c>
       <c r="C136" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="D136" s="54" t="s">
-        <v>7</v>
-      </c>
-      <c r="E136" s="54" t="s">
+        <v>15</v>
+      </c>
+      <c r="D136" s="53" t="s">
+        <v>12</v>
+      </c>
+      <c r="E136" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="F136" s="54" t="s">
+      <c r="F136" s="53" t="s">
         <v>7</v>
       </c>
       <c r="G136" s="20" t="s">
@@ -6179,13 +6185,13 @@
       <c r="C137" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D137" s="54" t="s">
+      <c r="D137" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="E137" s="54" t="s">
+      <c r="E137" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="F137" s="54"/>
+      <c r="F137" s="53"/>
       <c r="G137" s="20" t="s">
         <v>7</v>
       </c>
@@ -6196,15 +6202,15 @@
         <v>134</v>
       </c>
       <c r="C138" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="D138" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="D138" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="E138" s="54" t="s">
-        <v>77</v>
-      </c>
-      <c r="F138" s="54"/>
+      <c r="E138" s="53" t="s">
+        <v>7</v>
+      </c>
+      <c r="F138" s="53"/>
       <c r="G138" s="20" t="s">
         <v>9</v>
       </c>
@@ -6214,16 +6220,20 @@
       <c r="B139" s="16">
         <v>135</v>
       </c>
-      <c r="C139" s="52" t="s">
+      <c r="C139" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="D139" s="53" t="s">
+        <v>14</v>
+      </c>
+      <c r="E139" s="53" t="s">
+        <v>11</v>
+      </c>
+      <c r="F139" s="53"/>
+      <c r="G139" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="D139" s="54"/>
-      <c r="E139" s="54"/>
-      <c r="F139" s="54"/>
-      <c r="G139" s="52" t="s">
-        <v>15</v>
-      </c>
-      <c r="H139" s="51"/>
+      <c r="H139" s="50"/>
     </row>
     <row r="140" spans="2:8">
       <c r="B140" s="16">
@@ -6232,24 +6242,30 @@
       <c r="C140" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="D140" s="54"/>
-      <c r="E140" s="54"/>
-      <c r="F140" s="54"/>
+      <c r="D140" s="53" t="s">
+        <v>12</v>
+      </c>
+      <c r="E140" s="53" t="s">
+        <v>13</v>
+      </c>
+      <c r="F140" s="53"/>
       <c r="G140" s="33"/>
-      <c r="H140" s="51"/>
+      <c r="H140" s="50"/>
     </row>
     <row r="141" spans="2:8">
       <c r="B141" s="16">
         <v>137</v>
       </c>
       <c r="C141" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D141" s="53"/>
+      <c r="E141" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="D141" s="54"/>
-      <c r="E141" s="54"/>
       <c r="F141" s="21"/>
       <c r="G141" s="33"/>
-      <c r="H141" s="51"/>
+      <c r="H141" s="50"/>
     </row>
     <row r="142" spans="2:8" ht="15" thickBot="1">
       <c r="B142" s="16">
@@ -6265,12 +6281,12 @@
       <c r="H142" s="37"/>
     </row>
     <row r="143" spans="2:8">
-      <c r="C143" s="55"/>
-      <c r="D143" s="55"/>
-      <c r="E143" s="55"/>
-      <c r="F143" s="55"/>
-      <c r="G143" s="55"/>
-      <c r="H143" s="55"/>
+      <c r="C143" s="54"/>
+      <c r="D143" s="54"/>
+      <c r="E143" s="54"/>
+      <c r="F143" s="54"/>
+      <c r="G143" s="54"/>
+      <c r="H143" s="54"/>
     </row>
     <row r="145" spans="2:13">
       <c r="B145" s="64" t="s">
@@ -6316,7 +6332,7 @@
       </c>
       <c r="D147" s="22">
         <f t="shared" ref="D147:G147" si="0">COUNTIF(D$4:D$142,$B147)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E147" s="22">
         <f t="shared" si="0"/>
@@ -6324,7 +6340,7 @@
       </c>
       <c r="F147" s="22">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G147" s="22">
         <f t="shared" si="0"/>
@@ -6338,7 +6354,7 @@
       </c>
       <c r="J147" s="17">
         <f>Q181</f>
-        <v>0.66737081372929807</v>
+        <v>0.5228803972936914</v>
       </c>
     </row>
     <row r="148" spans="2:13">
@@ -6347,15 +6363,15 @@
       </c>
       <c r="C148" s="22">
         <f t="shared" ref="C148:G160" si="1">COUNTIF(C$4:C$142,$B148)</f>
-        <v>10</v>
-      </c>
-      <c r="D148" s="22">
+        <v>15</v>
+      </c>
+      <c r="D148" s="55">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E148" s="22">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F148" s="22">
         <f t="shared" si="1"/>
@@ -6374,28 +6390,28 @@
       </c>
       <c r="M148" s="17">
         <f>1/(C180*E180*G180*64)</f>
-        <v>118.67745535714285</v>
+        <v>121.31473214285712</v>
       </c>
     </row>
     <row r="149" spans="2:13">
       <c r="B149" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C149" s="22">
+      <c r="C149" s="55">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D149" s="22">
         <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-      <c r="E149" s="22">
+        <v>20</v>
+      </c>
+      <c r="E149" s="55">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F149" s="22">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G149" s="22">
         <f t="shared" si="1"/>
@@ -6412,15 +6428,15 @@
       </c>
       <c r="C150" s="22">
         <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="D150" s="22">
+        <v>16</v>
+      </c>
+      <c r="D150" s="55">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E150" s="22">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F150" s="22">
         <f t="shared" si="1"/>
@@ -6439,17 +6455,17 @@
       <c r="B151" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C151" s="22">
+      <c r="C151" s="55">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D151" s="22">
         <f t="shared" si="1"/>
-        <v>17</v>
-      </c>
-      <c r="E151" s="22">
+        <v>20</v>
+      </c>
+      <c r="E151" s="55">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F151" s="22">
         <f t="shared" si="1"/>
@@ -6470,15 +6486,15 @@
       </c>
       <c r="C152" s="22">
         <f t="shared" si="1"/>
-        <v>19</v>
-      </c>
-      <c r="D152" s="22">
+        <v>18</v>
+      </c>
+      <c r="D152" s="55">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="E152" s="22">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F152" s="22">
         <f t="shared" si="1"/>
@@ -6486,10 +6502,10 @@
       </c>
       <c r="G152" s="22">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H152" s="22">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I152" s="31"/>
     </row>
@@ -6499,15 +6515,15 @@
       </c>
       <c r="C153" s="22">
         <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="D153" s="22">
+        <v>13</v>
+      </c>
+      <c r="D153" s="55">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E153" s="22">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F153" s="22">
         <f t="shared" si="1"/>
@@ -6526,17 +6542,17 @@
       <c r="B154" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="C154" s="22">
+      <c r="C154" s="55">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D154" s="22">
         <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="E154" s="22">
+        <v>17</v>
+      </c>
+      <c r="E154" s="55">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F154" s="22">
         <f t="shared" si="1"/>
@@ -6557,19 +6573,19 @@
       </c>
       <c r="C155" s="22">
         <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="D155" s="22">
+        <v>12</v>
+      </c>
+      <c r="D155" s="55">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E155" s="22">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F155" s="22">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G155" s="22">
         <f t="shared" si="1"/>
@@ -6584,17 +6600,17 @@
       <c r="B156" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="C156" s="22">
+      <c r="C156" s="55">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="D156" s="22">
         <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="E156" s="22">
+        <v>16</v>
+      </c>
+      <c r="E156" s="55">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F156" s="22">
         <f t="shared" si="1"/>
@@ -6615,15 +6631,15 @@
       </c>
       <c r="C157" s="22">
         <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="D157" s="22">
+        <v>13</v>
+      </c>
+      <c r="D157" s="55">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="E157" s="22">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F157" s="22">
         <f t="shared" si="1"/>
@@ -6631,7 +6647,7 @@
       </c>
       <c r="G157" s="22">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H157" s="22">
         <v>3</v>
@@ -6676,7 +6692,7 @@
       </c>
       <c r="D159" s="22">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E159" s="22">
         <f t="shared" si="1"/>
@@ -6684,7 +6700,7 @@
       </c>
       <c r="F159" s="22">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G159" s="22">
         <f t="shared" si="1"/>
@@ -6732,11 +6748,11 @@
       </c>
       <c r="D161" s="29">
         <f t="shared" ref="D161:G161" si="2">SUM(D147:D160)</f>
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E161" s="29">
         <f t="shared" si="2"/>
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="F161" s="29">
         <f t="shared" si="2"/>
@@ -6748,7 +6764,7 @@
       </c>
       <c r="H161" s="29">
         <f>SUM(H147:H160)</f>
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="165" spans="2:26">
@@ -6855,15 +6871,15 @@
       </c>
       <c r="D167" s="22">
         <f t="shared" ref="D167:G167" si="3">D147/D$161</f>
-        <v>2.9629629629629631E-2</v>
+        <v>2.1897810218978103E-2</v>
       </c>
       <c r="E167" s="22">
         <f t="shared" si="3"/>
-        <v>2.2222222222222223E-2</v>
+        <v>2.1739130434782608E-2</v>
       </c>
       <c r="F167" s="22">
         <f t="shared" si="3"/>
-        <v>3.007518796992481E-2</v>
+        <v>2.2556390977443608E-2</v>
       </c>
       <c r="G167" s="22">
         <f t="shared" si="3"/>
@@ -6881,7 +6897,7 @@
       </c>
       <c r="M167" s="22">
         <f>(C167*D167*(E180+E178))*D186</f>
-        <v>6.631731651715665E-5</v>
+        <v>4.7946409613026818E-5</v>
       </c>
       <c r="N167" s="22">
         <f>C167*D167*E167*(F178+F180)*E186</f>
@@ -6889,11 +6905,11 @@
       </c>
       <c r="O167" s="22">
         <f>C167*D167*E167*F167*(G178+G180+SUM(G173:G177)+G179*SUM(H173:H177))*F186</f>
-        <v>3.1105362295013476E-5</v>
+        <v>1.6209689111152059E-5</v>
       </c>
       <c r="P167" s="22">
         <f>C167*D167*E167*F167*G167*G186</f>
-        <v>4.7139054199659591E-6</v>
+        <v>2.5560613578689189E-6</v>
       </c>
       <c r="Q167" s="22"/>
       <c r="T167" s="22" t="s">
@@ -6912,15 +6928,15 @@
       </c>
       <c r="C168" s="22">
         <f t="shared" ref="C168:C180" si="5">C148/C$161</f>
-        <v>7.1942446043165464E-2</v>
+        <v>0.1079136690647482</v>
       </c>
       <c r="D168" s="22">
         <f t="shared" ref="D168:G168" si="6">D148/D$161</f>
-        <v>8.1481481481481488E-2</v>
+        <v>6.569343065693431E-2</v>
       </c>
       <c r="E168" s="22">
         <f t="shared" si="6"/>
-        <v>9.6296296296296297E-2</v>
+        <v>0.10144927536231885</v>
       </c>
       <c r="F168" s="22">
         <f t="shared" si="6"/>
@@ -6932,7 +6948,7 @@
       </c>
       <c r="H168" s="22">
         <f t="shared" ref="H168" si="7">H148/H$161</f>
-        <v>8.1632653061224483E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="I168" s="31"/>
       <c r="K168" s="22" t="s">
@@ -6946,15 +6962,15 @@
       </c>
       <c r="N168" s="22">
         <f>((1-$H168)*($C168+C$167)*($D168+D$167)*($E168+E$167)*(1-F$167-$F168)+H168*($C168+C$167+C$179)*($D168+D$167+D$179)*($E168+E$167+E$179)*(1-F$167-$F168-F$179))*$E187-(1-F$167-F168-$H168*F$179)*$E187*PRODUCT(C$167:E$167)</f>
-        <v>3.866113185866836E-2</v>
+        <v>4.3625160050969114E-2</v>
       </c>
       <c r="O168" s="22">
         <f>((1-$H168)*($C168+C$167)*($D168+D$167)*($E168+E$167)*(F$167+$F168)*(1-G$167-G168)+H168*($C168+C$167+C$179)*($D168+D$167+D$179)*($E168+E$167+E$179)*(F$167+$F168+F$179)*(1-G$167-G168-G$179))*F187-(1-G$167-G168-$H168*G$179)*$F187*PRODUCT(C$167:F$167)</f>
-        <v>2.6429068709517427E-2</v>
+        <v>2.7250190384874744E-2</v>
       </c>
       <c r="P168" s="22">
         <f>((1-$H168)*($C168+C$167)*($D168+D$167)*($E168+E$167)*(F$167+$F168)*(G$167+G168)+H168*($C168+C$167+C$179)*($D168+D$167+D$179)*($E168+E$167+E$179)*(F$167+$F168+F$179)*(+G$167+G168+G$179))*G187-PRODUCT(C$167:G$167)*G187</f>
-        <v>1.0757324572665173E-2</v>
+        <v>1.0943788274363894E-2</v>
       </c>
       <c r="Q168" s="22"/>
       <c r="T168" s="22" t="s">
@@ -6975,19 +6991,19 @@
       </c>
       <c r="C169" s="22">
         <f t="shared" si="5"/>
-        <v>9.3525179856115109E-2</v>
+        <v>5.7553956834532377E-2</v>
       </c>
       <c r="D169" s="22">
         <f t="shared" ref="D169:G169" si="8">D149/D$161</f>
-        <v>0.1037037037037037</v>
+        <v>0.145985401459854</v>
       </c>
       <c r="E169" s="22">
         <f t="shared" si="8"/>
-        <v>0.1111111111111111</v>
+        <v>7.2463768115942032E-2</v>
       </c>
       <c r="F169" s="22">
         <f t="shared" si="8"/>
-        <v>0.11278195488721804</v>
+        <v>0.12030075187969924</v>
       </c>
       <c r="G169" s="22">
         <f t="shared" si="8"/>
@@ -6995,7 +7011,7 @@
       </c>
       <c r="H169" s="22">
         <f t="shared" ref="H169" si="9">H149/H$161</f>
-        <v>0.10204081632653061</v>
+        <v>0.10416666666666667</v>
       </c>
       <c r="K169" s="22" t="s">
         <v>8</v>
@@ -7008,15 +7024,15 @@
       </c>
       <c r="N169" s="22">
         <f t="shared" ref="N169:N177" si="10">((1-$H169)*($C169+C$167)*($D169+D$167)*($E169+E$167)*(1-F$167-$F169)+H169*($C169+C$167+C$179)*($D169+D$167+D$179)*($E169+E$167+E$179)*(1-F$167-$F169-F$179))*$E188-(1-F$167-F169-$H169*F$179)*$E188*PRODUCT(C$167:E$167)</f>
-        <v>4.1675779341972925E-2</v>
+        <v>3.3349508701798404E-2</v>
       </c>
       <c r="O169" s="22">
         <f t="shared" ref="O169:O177" si="11">((1-$H169)*($C169+C$167)*($D169+D$167)*($E169+E$167)*(F$167+$F169)*(1-G$167-G169)+H169*($C169+C$167+C$179)*($D169+D$167+D$179)*($E169+E$167+E$179)*(F$167+$F169+F$179)*(1-G$167-G169-G$179))*F188-(1-G$167-G169-$H169*G$179)*$F188*PRODUCT(C$167:F$167)</f>
-        <v>3.3952913909894807E-2</v>
+        <v>2.710324312085368E-2</v>
       </c>
       <c r="P169" s="22">
         <f t="shared" ref="P169:P177" si="12">((1-$H169)*($C169+C$167)*($D169+D$167)*($E169+E$167)*(F$167+$F169)*(G$167+G169)+H169*($C169+C$167+C$179)*($D169+D$167+D$179)*($E169+E$167+E$179)*(F$167+$F169+F$179)*(+G$167+G169+G$179))*G188-PRODUCT(C$167:G$167)*G188</f>
-        <v>1.6578305110832855E-2</v>
+        <v>1.076657275366528E-2</v>
       </c>
       <c r="Q169" s="22"/>
       <c r="T169" s="22" t="s">
@@ -7035,15 +7051,15 @@
       </c>
       <c r="C170" s="22">
         <f t="shared" si="5"/>
-        <v>0.1079136690647482</v>
+        <v>0.11510791366906475</v>
       </c>
       <c r="D170" s="22">
         <f t="shared" ref="D170:G170" si="13">D150/D$161</f>
-        <v>0.11851851851851852</v>
+        <v>6.569343065693431E-2</v>
       </c>
       <c r="E170" s="22">
         <f t="shared" si="13"/>
-        <v>0.11851851851851852</v>
+        <v>0.13768115942028986</v>
       </c>
       <c r="F170" s="22">
         <f t="shared" si="13"/>
@@ -7055,7 +7071,7 @@
       </c>
       <c r="H170" s="22">
         <f t="shared" ref="H170" si="14">H150/H$161</f>
-        <v>0.12244897959183673</v>
+        <v>0.125</v>
       </c>
       <c r="K170" s="22" t="s">
         <v>9</v>
@@ -7068,15 +7084,15 @@
       </c>
       <c r="N170" s="22">
         <f t="shared" si="10"/>
-        <v>5.5024852298612224E-2</v>
+        <v>4.0234749775790883E-2</v>
       </c>
       <c r="O170" s="22">
         <f t="shared" si="11"/>
-        <v>3.7200356062440827E-2</v>
+        <v>3.1870300741781675E-2</v>
       </c>
       <c r="P170" s="22">
         <f t="shared" si="12"/>
-        <v>2.2737362456286749E-2</v>
+        <v>1.5697561706499531E-2</v>
       </c>
       <c r="Q170" s="22"/>
       <c r="T170" s="22" t="s">
@@ -7095,15 +7111,15 @@
       </c>
       <c r="C171" s="22">
         <f t="shared" si="5"/>
-        <v>0.11510791366906475</v>
+        <v>7.1942446043165464E-2</v>
       </c>
       <c r="D171" s="22">
         <f t="shared" ref="D171:G171" si="15">D151/D$161</f>
-        <v>0.12592592592592591</v>
+        <v>0.145985401459854</v>
       </c>
       <c r="E171" s="22">
         <f t="shared" si="15"/>
-        <v>0.14074074074074075</v>
+        <v>8.6956521739130432E-2</v>
       </c>
       <c r="F171" s="22">
         <f t="shared" si="15"/>
@@ -7115,7 +7131,7 @@
       </c>
       <c r="H171" s="22">
         <f t="shared" ref="H171" si="16">H151/H$161</f>
-        <v>0.14285714285714285</v>
+        <v>0.14583333333333334</v>
       </c>
       <c r="K171" s="22" t="s">
         <v>10</v>
@@ -7128,15 +7144,15 @@
       </c>
       <c r="N171" s="22">
         <f t="shared" si="10"/>
-        <v>7.1145394222872096E-2</v>
+        <v>3.77540530981509E-2</v>
       </c>
       <c r="O171" s="22">
         <f t="shared" si="11"/>
-        <v>3.5999678174942831E-2</v>
+        <v>3.0110634866081485E-2</v>
       </c>
       <c r="P171" s="22">
         <f t="shared" si="12"/>
-        <v>2.5027380916044603E-2</v>
+        <v>1.2827891605685033E-2</v>
       </c>
       <c r="Q171" s="22"/>
       <c r="T171" s="22" t="s">
@@ -7155,15 +7171,15 @@
       </c>
       <c r="C172" s="22">
         <f t="shared" si="5"/>
-        <v>0.1366906474820144</v>
+        <v>0.12949640287769784</v>
       </c>
       <c r="D172" s="22">
         <f t="shared" ref="D172:G172" si="17">D152/D$161</f>
-        <v>0.14074074074074075</v>
+        <v>5.8394160583941604E-2</v>
       </c>
       <c r="E172" s="22">
         <f t="shared" si="17"/>
-        <v>0.14814814814814814</v>
+        <v>0.13043478260869565</v>
       </c>
       <c r="F172" s="22">
         <f t="shared" si="17"/>
@@ -7171,11 +7187,11 @@
       </c>
       <c r="G172" s="22">
         <f t="shared" si="17"/>
-        <v>0.14705882352941177</v>
+        <v>0.16176470588235295</v>
       </c>
       <c r="H172" s="22">
         <f t="shared" ref="H172" si="18">H152/H$161</f>
-        <v>0.16326530612244897</v>
+        <v>0.14583333333333334</v>
       </c>
       <c r="K172" s="22" t="s">
         <v>77</v>
@@ -7188,15 +7204,15 @@
       </c>
       <c r="N172" s="22">
         <f t="shared" si="10"/>
-        <v>9.0996769169304562E-2</v>
+        <v>3.8924474225045351E-2</v>
       </c>
       <c r="O172" s="22">
         <f t="shared" si="11"/>
-        <v>4.5892778843992899E-2</v>
+        <v>3.6447463482552345E-2</v>
       </c>
       <c r="P172" s="22">
         <f t="shared" si="12"/>
-        <v>3.3373154851053098E-2</v>
+        <v>1.4623457192226465E-2</v>
       </c>
       <c r="Q172" s="22"/>
       <c r="T172" s="22" t="s">
@@ -7215,15 +7231,15 @@
       </c>
       <c r="C173" s="22">
         <f t="shared" si="5"/>
-        <v>6.4748201438848921E-2</v>
+        <v>9.3525179856115109E-2</v>
       </c>
       <c r="D173" s="22">
         <f t="shared" ref="D173:G173" si="19">D153/D$161</f>
-        <v>9.6296296296296297E-2</v>
+        <v>5.1094890510948905E-2</v>
       </c>
       <c r="E173" s="22">
         <f t="shared" si="19"/>
-        <v>6.6666666666666666E-2</v>
+        <v>7.9710144927536225E-2</v>
       </c>
       <c r="F173" s="22">
         <f t="shared" si="19"/>
@@ -7235,7 +7251,7 @@
       </c>
       <c r="H173" s="22">
         <f t="shared" ref="H173" si="20">H153/H$161</f>
-        <v>0.10204081632653061</v>
+        <v>0.10416666666666667</v>
       </c>
       <c r="K173" s="22" t="s">
         <v>11</v>
@@ -7248,15 +7264,15 @@
       </c>
       <c r="N173" s="22">
         <f t="shared" si="10"/>
-        <v>5.4524558924762372E-3</v>
+        <v>9.7369155736894749E-3</v>
       </c>
       <c r="O173" s="22">
         <f t="shared" si="11"/>
-        <v>1.502014451806258E-2</v>
+        <v>9.1938133752756251E-3</v>
       </c>
       <c r="P173" s="22">
         <f t="shared" si="12"/>
-        <v>1.6918053341424071E-3</v>
+        <v>1.37534053089222E-3</v>
       </c>
       <c r="Q173" s="22"/>
       <c r="T173" s="22" t="s">
@@ -7275,15 +7291,15 @@
       </c>
       <c r="C174" s="22">
         <f t="shared" si="5"/>
-        <v>9.3525179856115109E-2</v>
+        <v>5.0359712230215826E-2</v>
       </c>
       <c r="D174" s="22">
         <f t="shared" ref="D174:G174" si="21">D154/D$161</f>
-        <v>7.407407407407407E-2</v>
+        <v>0.12408759124087591</v>
       </c>
       <c r="E174" s="22">
         <f t="shared" si="21"/>
-        <v>3.7037037037037035E-2</v>
+        <v>6.5217391304347824E-2</v>
       </c>
       <c r="F174" s="22">
         <f t="shared" si="21"/>
@@ -7295,7 +7311,7 @@
       </c>
       <c r="H174" s="22">
         <f t="shared" ref="H174" si="22">H154/H$161</f>
-        <v>0.10204081632653061</v>
+        <v>0.10416666666666667</v>
       </c>
       <c r="K174" s="22" t="s">
         <v>12</v>
@@ -7308,15 +7324,15 @@
       </c>
       <c r="N174" s="22">
         <f t="shared" si="10"/>
-        <v>4.2708287388733513E-3</v>
+        <v>1.0742398724482448E-2</v>
       </c>
       <c r="O174" s="22">
         <f t="shared" si="11"/>
-        <v>9.5137407394128848E-3</v>
+        <v>7.9182788007042208E-3</v>
       </c>
       <c r="P174" s="22">
         <f t="shared" si="12"/>
-        <v>1.2948873716959826E-3</v>
+        <v>1.4016935585544187E-3</v>
       </c>
       <c r="Q174" s="22"/>
       <c r="T174" s="22" t="s">
@@ -7335,19 +7351,19 @@
       </c>
       <c r="C175" s="22">
         <f t="shared" si="5"/>
-        <v>4.3165467625899283E-2</v>
+        <v>8.6330935251798566E-2</v>
       </c>
       <c r="D175" s="22">
         <f t="shared" ref="D175:G175" si="23">D155/D$161</f>
-        <v>8.8888888888888892E-2</v>
+        <v>0.10948905109489052</v>
       </c>
       <c r="E175" s="22">
         <f t="shared" si="23"/>
-        <v>3.7037037037037035E-2</v>
+        <v>5.7971014492753624E-2</v>
       </c>
       <c r="F175" s="22">
         <f t="shared" si="23"/>
-        <v>7.5187969924812026E-2</v>
+        <v>8.2706766917293228E-2</v>
       </c>
       <c r="G175" s="22">
         <f t="shared" si="23"/>
@@ -7355,7 +7371,7 @@
       </c>
       <c r="H175" s="22">
         <f t="shared" ref="H175" si="24">H155/H$161</f>
-        <v>6.1224489795918366E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="K175" s="22" t="s">
         <v>13</v>
@@ -7368,15 +7384,15 @@
       </c>
       <c r="N175" s="22">
         <f t="shared" si="10"/>
-        <v>2.5048891717103874E-3</v>
+        <v>1.1576446804940591E-2</v>
       </c>
       <c r="O175" s="22">
         <f t="shared" si="11"/>
-        <v>3.9148657425502427E-3</v>
+        <v>7.0884581157055569E-3</v>
       </c>
       <c r="P175" s="22">
         <f t="shared" si="12"/>
-        <v>2.6868940219967869E-4</v>
+        <v>1.0561913759375384E-3</v>
       </c>
       <c r="Q175" s="22"/>
       <c r="T175" s="22" t="s">
@@ -7399,11 +7415,11 @@
       </c>
       <c r="D176" s="22">
         <f>D156/D$161</f>
-        <v>3.7037037037037035E-2</v>
+        <v>0.11678832116788321</v>
       </c>
       <c r="E176" s="22">
         <f t="shared" ref="E176:G176" si="25">E156/E$161</f>
-        <v>4.4444444444444446E-2</v>
+        <v>5.0724637681159424E-2</v>
       </c>
       <c r="F176" s="22">
         <f t="shared" si="25"/>
@@ -7415,7 +7431,7 @@
       </c>
       <c r="H176" s="22">
         <f t="shared" ref="H176" si="26">H156/H$161</f>
-        <v>6.1224489795918366E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="K176" s="22" t="s">
         <v>14</v>
@@ -7428,15 +7444,15 @@
       </c>
       <c r="N176" s="22">
         <f t="shared" si="10"/>
-        <v>2.0182105044827116E-3</v>
+        <v>8.6451438587129715E-3</v>
       </c>
       <c r="O176" s="22">
         <f t="shared" si="11"/>
-        <v>2.4325075548291076E-3</v>
+        <v>3.6880050438959475E-3</v>
       </c>
       <c r="P176" s="22">
         <f t="shared" si="12"/>
-        <v>2.6637554003668953E-4</v>
+        <v>9.1152461434476954E-4</v>
       </c>
       <c r="Q176" s="22"/>
       <c r="T176" s="22" t="s">
@@ -7455,15 +7471,15 @@
       </c>
       <c r="C177" s="22">
         <f t="shared" si="5"/>
-        <v>7.9136690647482008E-2</v>
+        <v>9.3525179856115109E-2</v>
       </c>
       <c r="D177" s="22">
         <f>D157/D$161</f>
-        <v>4.4444444444444446E-2</v>
+        <v>4.3795620437956206E-2</v>
       </c>
       <c r="E177" s="22">
         <f t="shared" ref="E177:G177" si="27">E157/E$161</f>
-        <v>6.6666666666666666E-2</v>
+        <v>8.6956521739130432E-2</v>
       </c>
       <c r="F177" s="22">
         <f t="shared" si="27"/>
@@ -7471,11 +7487,11 @@
       </c>
       <c r="G177" s="22">
         <f t="shared" si="27"/>
-        <v>8.0882352941176475E-2</v>
+        <v>6.6176470588235295E-2</v>
       </c>
       <c r="H177" s="22">
         <f t="shared" ref="H177" si="28">H157/H$161</f>
-        <v>6.1224489795918366E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="K177" s="22" t="s">
         <v>15</v>
@@ -7488,15 +7504,15 @@
       </c>
       <c r="N177" s="22">
         <f t="shared" si="10"/>
-        <v>3.6408852220220309E-3</v>
+        <v>8.9366011217674544E-3</v>
       </c>
       <c r="O177" s="22">
         <f t="shared" si="11"/>
-        <v>3.7880264126309675E-3</v>
+        <v>3.4349904703191167E-3</v>
       </c>
       <c r="P177" s="22">
         <f t="shared" si="12"/>
-        <v>4.5951385194642767E-4</v>
+        <v>8.4976733187048094E-4</v>
       </c>
       <c r="Q177" s="22"/>
       <c r="T177" s="22" t="s">
@@ -7570,15 +7586,15 @@
       </c>
       <c r="D179" s="22">
         <f t="shared" si="29"/>
-        <v>5.9259259259259262E-2</v>
+        <v>5.1094890510948905E-2</v>
       </c>
       <c r="E179" s="22">
         <f t="shared" si="29"/>
-        <v>5.9259259259259262E-2</v>
+        <v>5.7971014492753624E-2</v>
       </c>
       <c r="F179" s="22">
         <f t="shared" si="29"/>
-        <v>6.0150375939849621E-2</v>
+        <v>5.2631578947368418E-2</v>
       </c>
       <c r="G179" s="22">
         <f t="shared" si="29"/>
@@ -7625,7 +7641,7 @@
       </c>
       <c r="E180" s="22">
         <f t="shared" si="29"/>
-        <v>5.185185185185185E-2</v>
+        <v>5.0724637681159424E-2</v>
       </c>
       <c r="F180" s="22">
         <f t="shared" si="29"/>
@@ -7650,7 +7666,7 @@
       </c>
       <c r="N180" s="27">
         <f>64*C180*E180*G180*E198</f>
-        <v>2.5278600648892653E-2</v>
+        <v>2.4729065852177597E-2</v>
       </c>
       <c r="O180" s="27"/>
       <c r="P180" s="27"/>
@@ -7679,19 +7695,19 @@
       </c>
       <c r="E181" s="29">
         <f t="shared" si="33"/>
-        <v>0.99999999999999978</v>
+        <v>1</v>
       </c>
       <c r="F181" s="29">
         <f t="shared" si="33"/>
-        <v>0.99999999999999989</v>
+        <v>0.99999999999999978</v>
       </c>
       <c r="G181" s="30">
         <f t="shared" si="33"/>
-        <v>1</v>
+        <v>0.99999999999999989</v>
       </c>
       <c r="H181" s="30">
         <f t="shared" si="33"/>
-        <v>0.99999999999999989</v>
+        <v>1</v>
       </c>
       <c r="K181" s="28" t="s">
         <v>57</v>
@@ -7703,7 +7719,7 @@
       <c r="P181" s="30"/>
       <c r="Q181" s="30">
         <f>SUM(L167:P180)</f>
-        <v>0.66737081372929807</v>
+        <v>0.5228803972936914</v>
       </c>
       <c r="T181" s="28" t="s">
         <v>57</v>
@@ -7747,7 +7763,7 @@
       </c>
       <c r="R184" s="17">
         <f>((1-H$168)*IF(K184="Wild",C$167,C$168)*IF(L184="Wild",D$167,D$168)*IF(M184="Wild",E$167,E$168)*(1-F$167-F$168)+H$168*IF(K184="Wild",C$167,C$168+C$179)*IF(L184="Wild",D$167,D$168+D$179)*IF(M184="Wild",E$167,E$168+E$179)*(1-F$167-F$168-F$179))*E$187</f>
-        <v>1.6921535146697233E-3</v>
+        <v>1.3270237483390642E-3</v>
       </c>
       <c r="X184" s="45"/>
     </row>
@@ -7790,7 +7806,7 @@
       </c>
       <c r="R185" s="17">
         <f t="shared" ref="R185:R191" si="34">((1-H$168)*IF(K185="Wild",C$167,C$168)*IF(L185="Wild",D$167,D$168)*IF(M185="Wild",E$167,E$168)*(1-F$167-F$168)+H$168*IF(K185="Wild",C$167,C$168+C$179)*IF(L185="Wild",D$167,D$168+D$179)*IF(M185="Wild",E$167,E$168+E$179)*(1-F$167-F$168-F$179))*E$187</f>
-        <v>1.0826426578035815E-3</v>
+        <v>8.663571167724423E-4</v>
       </c>
     </row>
     <row r="186" spans="2:26">
@@ -7813,7 +7829,7 @@
         <f>Paytable!F4</f>
         <v>200</v>
       </c>
-      <c r="G186" s="47">
+      <c r="G186" s="39">
         <f>Paytable!G4</f>
         <v>500</v>
       </c>
@@ -7837,7 +7853,7 @@
       </c>
       <c r="R186" s="17">
         <f t="shared" si="34"/>
-        <v>1.319208558272302E-3</v>
+        <v>1.4177279523465219E-3</v>
       </c>
     </row>
     <row r="187" spans="2:26">
@@ -7860,7 +7876,7 @@
         <f>Paytable!F5</f>
         <v>150</v>
       </c>
-      <c r="G187" s="40">
+      <c r="G187" s="39">
         <f>Paytable!G5</f>
         <v>400</v>
       </c>
@@ -7884,7 +7900,7 @@
       </c>
       <c r="R187" s="17">
         <f t="shared" si="34"/>
-        <v>3.9700877015128736E-3</v>
+        <v>4.636665009113681E-3</v>
       </c>
     </row>
     <row r="188" spans="2:26">
@@ -7901,13 +7917,13 @@
       </c>
       <c r="E188" s="39">
         <f>Paytable!E6</f>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F188" s="39">
         <f>Paytable!F6</f>
-        <v>100</v>
-      </c>
-      <c r="G188" s="40">
+        <v>125</v>
+      </c>
+      <c r="G188" s="39">
         <f>Paytable!G6</f>
         <v>300</v>
       </c>
@@ -7931,7 +7947,7 @@
       </c>
       <c r="R188" s="17">
         <f t="shared" si="34"/>
-        <v>6.1729226408653651E-3</v>
+        <v>7.0543279514160917E-3</v>
       </c>
     </row>
     <row r="189" spans="2:26">
@@ -7952,9 +7968,9 @@
       </c>
       <c r="F189" s="39">
         <f>Paytable!F7</f>
-        <v>80</v>
-      </c>
-      <c r="G189" s="40">
+        <v>100</v>
+      </c>
+      <c r="G189" s="39">
         <f>Paytable!G7</f>
         <v>250</v>
       </c>
@@ -7978,7 +7994,7 @@
       </c>
       <c r="R189" s="17">
         <f t="shared" si="34"/>
-        <v>5.0527303593164551E-3</v>
+        <v>4.3478793035228681E-3</v>
       </c>
     </row>
     <row r="190" spans="2:26">
@@ -7999,9 +8015,9 @@
       </c>
       <c r="F190" s="39">
         <f>Paytable!F8</f>
-        <v>60</v>
-      </c>
-      <c r="G190" s="40">
+        <v>100</v>
+      </c>
+      <c r="G190" s="39">
         <f>Paytable!G8</f>
         <v>200</v>
       </c>
@@ -8025,11 +8041,11 @@
       </c>
       <c r="R190" s="17">
         <f t="shared" si="34"/>
-        <v>1.9371386426228054E-2</v>
+        <v>2.3975178969458451E-2</v>
       </c>
       <c r="S190" s="17">
         <f>SUM(R184:R190)</f>
-        <v>3.866113185866836E-2</v>
+        <v>4.3625160050969121E-2</v>
       </c>
     </row>
     <row r="191" spans="2:26">
@@ -8050,9 +8066,9 @@
       </c>
       <c r="F191" s="39">
         <f>Paytable!F9</f>
-        <v>50</v>
-      </c>
-      <c r="G191" s="40">
+        <v>100</v>
+      </c>
+      <c r="G191" s="39">
         <f>Paytable!G9</f>
         <v>150</v>
       </c>
@@ -8067,7 +8083,7 @@
       </c>
       <c r="R191" s="17">
         <f t="shared" si="34"/>
-        <v>3.7294495639742111E-4</v>
+        <v>2.7211261202237432E-4</v>
       </c>
     </row>
     <row r="192" spans="2:26">
@@ -8084,18 +8100,19 @@
       </c>
       <c r="E192" s="39">
         <f>Paytable!E10</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F192" s="39">
-        <v>100</v>
-      </c>
-      <c r="G192" s="40">
+        <f>Paytable!F10</f>
+        <v>75</v>
+      </c>
+      <c r="G192" s="39">
         <f>Paytable!G10</f>
         <v>100</v>
       </c>
       <c r="R192" s="17">
         <f>(1-F167-F168-F179*0.1)*50*C167*D167*E167</f>
-        <v>6.2078991777338383E-4</v>
+        <v>4.5307039588679212E-4</v>
       </c>
     </row>
     <row r="193" spans="2:7">
@@ -8112,12 +8129,13 @@
       </c>
       <c r="E193" s="39">
         <f>Paytable!E11</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F193" s="39">
-        <v>100</v>
-      </c>
-      <c r="G193" s="40">
+        <f>Paytable!F11</f>
+        <v>75</v>
+      </c>
+      <c r="G193" s="39">
         <f>Paytable!G11</f>
         <v>100</v>
       </c>
@@ -8136,14 +8154,15 @@
       </c>
       <c r="E194" s="39">
         <f>Paytable!E12</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F194" s="39">
-        <v>60</v>
-      </c>
-      <c r="G194" s="40">
+        <f>Paytable!F12</f>
+        <v>50</v>
+      </c>
+      <c r="G194" s="39">
         <f>Paytable!G12</f>
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="195" spans="2:7">
@@ -8160,14 +8179,15 @@
       </c>
       <c r="E195" s="39">
         <f>Paytable!E13</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F195" s="39">
-        <v>60</v>
-      </c>
-      <c r="G195" s="40">
+        <f>Paytable!F13</f>
+        <v>50</v>
+      </c>
+      <c r="G195" s="39">
         <f>Paytable!G13</f>
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="196" spans="2:7">
@@ -8184,14 +8204,15 @@
       </c>
       <c r="E196" s="39">
         <f>Paytable!E14</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F196" s="39">
-        <v>60</v>
-      </c>
-      <c r="G196" s="40">
+        <f>Paytable!F14</f>
+        <v>50</v>
+      </c>
+      <c r="G196" s="39">
         <f>Paytable!G14</f>
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="197" spans="2:7">
@@ -8207,7 +8228,7 @@
       <c r="E197" s="39">
         <v>0</v>
       </c>
-      <c r="F197" s="48">
+      <c r="F197" s="47">
         <v>0</v>
       </c>
       <c r="G197" s="40">
@@ -8235,67 +8256,67 @@
     <mergeCell ref="B145:H145"/>
     <mergeCell ref="B165:H165"/>
   </mergeCells>
-  <conditionalFormatting sqref="A1:H162 A164:H1048576 A163:F163">
+  <conditionalFormatting sqref="A163:F163 A1:H162 A164:H1048576">
     <cfRule type="containsText" dxfId="38" priority="48" operator="containsText" text="Lion">
       <formula>NOT(ISERROR(SEARCH("Lion",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T27:T141 T1:T15 A1:L141 A142:T162 A164:T1048576 A163:R163">
+  <conditionalFormatting sqref="T27:T141 T1:T15 A142:T162 A163:R163 A1:L141 A164:T1048576">
     <cfRule type="containsText" dxfId="37" priority="47" operator="containsText" text="Elephant">
       <formula>NOT(ISERROR(SEARCH("Elephant",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:L141 A142:Q162 A164:Q1048576 A163:O163">
+  <conditionalFormatting sqref="A142:Q162 A163:O163 A1:L141 A164:Q1048576">
     <cfRule type="containsText" dxfId="36" priority="46" operator="containsText" text="Leopard">
       <formula>NOT(ISERROR(SEARCH("Leopard",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:L141 A142:S162 A164:S1048576 A163:Q163">
+  <conditionalFormatting sqref="A142:S162 A163:Q163 A1:L141 A164:S1048576">
     <cfRule type="containsText" dxfId="35" priority="45" operator="containsText" text="WaterBuffalo">
       <formula>NOT(ISERROR(SEARCH("WaterBuffalo",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T27:Z141 T16:Y26 T1:Z15 A1:L141 A142:Z162 A164:Z1048576 A163:X163">
+  <conditionalFormatting sqref="T27:Z141 T16:Y26 T1:Z15 A142:Z162 A163:X163 A1:L141 A164:Z1048576">
     <cfRule type="containsText" dxfId="34" priority="44" operator="containsText" text="Rhino">
       <formula>NOT(ISERROR(SEARCH("Rhino",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T27:V141 T16:U26 T1:V15 A1:L141 A142:V162 A164:V1048576 A163:T163">
+  <conditionalFormatting sqref="T27:V141 T16:U26 T1:V15 A142:V162 A163:T163 A1:L141 A164:V1048576">
     <cfRule type="containsText" dxfId="33" priority="43" operator="containsText" text="Wild">
       <formula>NOT(ISERROR(SEARCH("Wild",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T27:X141 T16:W26 T1:X15 A1:L141 A142:X162 A164:X1048576 A163:V163">
+  <conditionalFormatting sqref="T27:X141 T16:W26 T1:X15 A142:X162 A163:V163 A1:L141 A164:X1048576">
     <cfRule type="containsText" dxfId="32" priority="42" operator="containsText" text="Ace">
       <formula>NOT(ISERROR(SEARCH("Ace",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T27:U141 T16:T26 T1:U15 A1:L141 A142:U162 A164:U1048576 A163:S163">
+  <conditionalFormatting sqref="T27:U141 T16:T26 T1:U15 A142:U162 A163:S163 A1:L141 A164:U1048576">
     <cfRule type="containsText" dxfId="31" priority="41" operator="containsText" text="King">
       <formula>NOT(ISERROR(SEARCH("King",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T27:W141 T16:V26 T1:W15 A1:L141 A142:W162 A164:W1048576 A163:U163">
+  <conditionalFormatting sqref="T27:W141 T16:V26 T1:W15 A142:W162 A163:U163 A1:L141 A164:W1048576">
     <cfRule type="containsText" dxfId="30" priority="40" operator="containsText" text="Queen">
       <formula>NOT(ISERROR(SEARCH("Queen",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T27:Y141 T16:X26 T1:Y15 A1:L141 A142:Y162 A164:Y1048576 A163:W163">
+  <conditionalFormatting sqref="T27:Y141 T16:X26 T1:Y15 A142:Y162 A163:W163 A1:L141 A164:Y1048576">
     <cfRule type="containsText" dxfId="29" priority="39" operator="containsText" text="Jack">
       <formula>NOT(ISERROR(SEARCH("Jack",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T27:V141 T16:U26 T1:V15 B1:L141 B142:V162 B164:V1048576 B163:T163">
+  <conditionalFormatting sqref="T27:V141 T16:U26 T1:V15 B142:V162 B163:T163 B1:L141 B164:V1048576">
     <cfRule type="containsText" dxfId="28" priority="38" operator="containsText" text="Ten">
       <formula>NOT(ISERROR(SEARCH("Ten",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T27:AA141 T16:Z26 T1:AA15 A1:L141 A142:AA162 A164:AA1048576 A163:Y163">
+  <conditionalFormatting sqref="T27:AA141 T16:Z26 T1:AA15 A142:AA162 A163:Y163 A1:L141 A164:AA1048576">
     <cfRule type="containsText" dxfId="27" priority="37" operator="containsText" text="Collector">
       <formula>NOT(ISERROR(SEARCH("Collector",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:L141 A142:O162 A164:O1048576 A163:M163">
+  <conditionalFormatting sqref="A142:O162 A163:M163 A1:L141 A164:O1048576">
     <cfRule type="containsText" dxfId="26" priority="36" operator="containsText" text="Scatter">
       <formula>NOT(ISERROR(SEARCH("Scatter",A1)))</formula>
     </cfRule>
@@ -8424,8 +8445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5091FB6-A1FC-4569-9527-D3BFD417E752}">
   <dimension ref="B2:I160"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView topLeftCell="A140" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C160" sqref="C160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -11339,7 +11360,7 @@
       <c r="G139" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="H139" s="51"/>
+      <c r="H139" s="50"/>
     </row>
     <row r="140" spans="2:8">
       <c r="B140" s="16">
@@ -11360,7 +11381,7 @@
       <c r="G140" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="H140" s="51"/>
+      <c r="H140" s="50"/>
     </row>
     <row r="141" spans="2:8">
       <c r="B141" s="16">
@@ -11381,7 +11402,7 @@
       <c r="G141" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="H141" s="51"/>
+      <c r="H141" s="50"/>
     </row>
     <row r="142" spans="2:8" ht="15" thickBot="1">
       <c r="B142" s="16">
@@ -11405,12 +11426,12 @@
       <c r="H142" s="37"/>
     </row>
     <row r="143" spans="2:8">
-      <c r="C143" s="55"/>
-      <c r="D143" s="55"/>
-      <c r="E143" s="55"/>
-      <c r="F143" s="55"/>
-      <c r="G143" s="55"/>
-      <c r="H143" s="55"/>
+      <c r="C143" s="54"/>
+      <c r="D143" s="54"/>
+      <c r="E143" s="54"/>
+      <c r="F143" s="54"/>
+      <c r="G143" s="54"/>
+      <c r="H143" s="54"/>
     </row>
     <row r="145" spans="2:8">
       <c r="B145" s="64" t="s">

</xml_diff>

<commit_message>
Making Beautiful reels. Outer Reel Wieght is added
</commit_message>
<xml_diff>
--- a/AnimalWill/AnimalWillMaths.xlsx
+++ b/AnimalWill/AnimalWillMaths.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AMD\source\repos\microchelick43018\AnimalWill\AnimalWill\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\konstantin.d\source\repos\AnimalWill\AnimalWill\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{484748D8-5BAB-4353-AF56-A3E7CD2FA21B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6F53031-61EA-4F01-A6E5-908FDC8B78F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Paytable" sheetId="2" r:id="rId3"/>
     <sheet name="Collect Feature Paytable" sheetId="12" r:id="rId4"/>
     <sheet name="Base Game Reels" sheetId="3" r:id="rId5"/>
-    <sheet name="Outer Reels Weights" sheetId="16" r:id="rId6"/>
+    <sheet name="Outer Reels Weights" sheetId="17" r:id="rId6"/>
     <sheet name="Outer Collector Reels" sheetId="15" r:id="rId7"/>
     <sheet name="FreeSpinsTriggerReels" sheetId="6" r:id="rId8"/>
     <sheet name="LionFeature Reels" sheetId="7" r:id="rId9"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1676" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1673" uniqueCount="92">
   <si>
     <t xml:space="preserve">Slot Name: </t>
   </si>
@@ -318,17 +318,17 @@
     <t>No</t>
   </si>
   <si>
-    <t>Chance to use outer reels during BG</t>
+    <t>Chance to use Outer Reels</t>
   </si>
   <si>
-    <t>Chance to use outer reels during Rhino Feature</t>
+    <t>Base Game</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -377,8 +377,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -415,8 +422,14 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="26">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -722,17 +735,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -740,7 +742,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -900,18 +902,12 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -920,7 +916,577 @@
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="標準_KS534 P82" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
-  <dxfs count="42">
+  <dxfs count="106">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="7"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="7"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFFFF00"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1032,6 +1598,183 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF66CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1204,145 +1947,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1" tint="4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1" tint="4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1" tint="4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1" tint="4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1" tint="4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2952,7 +3556,7 @@
     <mergeCell ref="B9:F9"/>
   </mergeCells>
   <conditionalFormatting sqref="O10:O59">
-    <cfRule type="containsText" dxfId="41" priority="1" operator="containsText" text="0">
+    <cfRule type="containsText" dxfId="105" priority="1" operator="containsText" text="0">
       <formula>NOT(ISERROR(SEARCH("0",O10)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2966,7 +3570,7 @@
   <dimension ref="B3:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3377,8 +3981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B2:Z198"/>
   <sheetViews>
-    <sheetView topLeftCell="A132" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E142" sqref="E142"/>
+    <sheetView tabSelected="1" topLeftCell="A121" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P127" sqref="P127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -3391,7 +3995,8 @@
     <col min="17" max="17" width="11" style="17" customWidth="1"/>
     <col min="18" max="23" width="9.109375" style="17"/>
     <col min="24" max="24" width="10" style="17" bestFit="1" customWidth="1"/>
-    <col min="25" max="16384" width="9.109375" style="17"/>
+    <col min="25" max="25" width="9.109375" style="17" customWidth="1"/>
+    <col min="26" max="16384" width="9.109375" style="17"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="15" thickBot="1">
@@ -3434,7 +4039,7 @@
         <v>9</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E4" s="20" t="s">
         <v>11</v>
@@ -3523,7 +4128,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D8" s="20" t="s">
         <v>8</v>
@@ -3592,10 +4197,10 @@
         <v>7</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E11" s="20" t="s">
         <v>12</v>
@@ -3661,7 +4266,7 @@
         <v>10</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D14" s="20" t="s">
         <v>7</v>
@@ -3684,7 +4289,7 @@
         <v>11</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D15" s="20" t="s">
         <v>7</v>
@@ -3707,10 +4312,10 @@
         <v>12</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E16" s="20" t="s">
         <v>7</v>
@@ -3733,7 +4338,7 @@
         <v>7</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E17" s="20" t="s">
         <v>77</v>
@@ -3795,7 +4400,7 @@
       </c>
       <c r="I19" s="25">
         <f>I62</f>
-        <v>0.51846029624859524</v>
+        <v>0.50630741199105156</v>
       </c>
     </row>
     <row r="20" spans="2:9">
@@ -3850,7 +4455,7 @@
         <v>10</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E22" s="20" t="s">
         <v>10</v>
@@ -3910,7 +4515,7 @@
         <v>21</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D25" s="20" t="s">
         <v>9</v>
@@ -3952,7 +4557,7 @@
         <v>23</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D27" s="20" t="s">
         <v>9</v>
@@ -4039,7 +4644,7 @@
         <v>9</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E31" s="20" t="s">
         <v>77</v>
@@ -4057,10 +4662,10 @@
         <v>28</v>
       </c>
       <c r="C32" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="20" t="s">
         <v>14</v>
-      </c>
-      <c r="D32" s="20" t="s">
-        <v>13</v>
       </c>
       <c r="E32" s="20" t="s">
         <v>13</v>
@@ -4165,7 +4770,7 @@
         <v>9</v>
       </c>
       <c r="D37" s="20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E37" s="20" t="s">
         <v>11</v>
@@ -4186,7 +4791,7 @@
         <v>13</v>
       </c>
       <c r="D38" s="20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E38" s="20" t="s">
         <v>12</v>
@@ -4204,7 +4809,7 @@
         <v>35</v>
       </c>
       <c r="C39" s="20" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D39" s="20" t="s">
         <v>8</v>
@@ -4225,7 +4830,7 @@
         <v>36</v>
       </c>
       <c r="C40" s="20" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D40" s="20" t="s">
         <v>8</v>
@@ -4246,7 +4851,7 @@
         <v>37</v>
       </c>
       <c r="C41" s="20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D41" s="20" t="s">
         <v>8</v>
@@ -4267,7 +4872,7 @@
         <v>38</v>
       </c>
       <c r="C42" s="20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D42" s="20" t="s">
         <v>8</v>
@@ -4312,7 +4917,7 @@
         <v>9</v>
       </c>
       <c r="D44" s="20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E44" s="20" t="s">
         <v>12</v>
@@ -4501,7 +5106,7 @@
         <v>77</v>
       </c>
       <c r="D53" s="20" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E53" s="20" t="s">
         <v>13</v>
@@ -4543,7 +5148,7 @@
         <v>15</v>
       </c>
       <c r="D55" s="20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E55" s="20" t="s">
         <v>14</v>
@@ -4606,7 +5211,7 @@
         <v>16</v>
       </c>
       <c r="D58" s="20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E58" s="20" t="s">
         <v>77</v>
@@ -4624,7 +5229,7 @@
         <v>55</v>
       </c>
       <c r="C59" s="20" t="s">
-        <v>14</v>
+        <v>77</v>
       </c>
       <c r="D59" s="20" t="s">
         <v>14</v>
@@ -4645,7 +5250,7 @@
         <v>56</v>
       </c>
       <c r="C60" s="20" t="s">
-        <v>15</v>
+        <v>77</v>
       </c>
       <c r="D60" s="20" t="s">
         <v>15</v>
@@ -4666,7 +5271,7 @@
         <v>57</v>
       </c>
       <c r="C61" s="20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D61" s="20" t="s">
         <v>77</v>
@@ -4704,7 +5309,7 @@
       <c r="H62" s="36"/>
       <c r="I62" s="25">
         <f>I127</f>
-        <v>0.51846029624859524</v>
+        <v>0.50630741199105156</v>
       </c>
     </row>
     <row r="63" spans="2:9">
@@ -4754,7 +5359,7 @@
         <v>61</v>
       </c>
       <c r="C65" s="20" t="s">
-        <v>77</v>
+        <v>14</v>
       </c>
       <c r="D65" s="20" t="s">
         <v>10</v>
@@ -4796,10 +5401,10 @@
         <v>63</v>
       </c>
       <c r="C67" s="20" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D67" s="20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E67" s="20" t="s">
         <v>11</v>
@@ -4838,7 +5443,7 @@
         <v>65</v>
       </c>
       <c r="C69" s="20" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D69" s="20" t="s">
         <v>10</v>
@@ -4880,10 +5485,10 @@
         <v>67</v>
       </c>
       <c r="C71" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D71" s="20" t="s">
         <v>11</v>
-      </c>
-      <c r="D71" s="20" t="s">
-        <v>12</v>
       </c>
       <c r="E71" s="20" t="s">
         <v>8</v>
@@ -4901,7 +5506,7 @@
         <v>68</v>
       </c>
       <c r="C72" s="20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D72" s="20" t="s">
         <v>5</v>
@@ -4925,7 +5530,7 @@
         <v>9</v>
       </c>
       <c r="D73" s="20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E73" s="20" t="s">
         <v>12</v>
@@ -4943,7 +5548,7 @@
         <v>70</v>
       </c>
       <c r="C74" s="20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D74" s="20" t="s">
         <v>8</v>
@@ -4988,7 +5593,7 @@
         <v>5</v>
       </c>
       <c r="D76" s="20" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E76" s="20" t="s">
         <v>5</v>
@@ -5005,8 +5610,8 @@
       <c r="B77" s="16">
         <v>73</v>
       </c>
-      <c r="C77" s="20" t="s">
-        <v>12</v>
+      <c r="C77" s="67" t="s">
+        <v>8</v>
       </c>
       <c r="D77" s="20" t="s">
         <v>5</v>
@@ -5026,8 +5631,8 @@
       <c r="B78" s="16">
         <v>74</v>
       </c>
-      <c r="C78" s="20" t="s">
-        <v>8</v>
+      <c r="C78" s="51" t="s">
+        <v>11</v>
       </c>
       <c r="D78" s="20" t="s">
         <v>8</v>
@@ -5048,10 +5653,10 @@
         <v>75</v>
       </c>
       <c r="C79" s="20" t="s">
-        <v>8</v>
+        <v>77</v>
       </c>
       <c r="D79" s="20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E79" s="20" t="s">
         <v>11</v>
@@ -5072,7 +5677,7 @@
         <v>5</v>
       </c>
       <c r="D80" s="20" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E80" s="20" t="s">
         <v>59</v>
@@ -5090,7 +5695,7 @@
         <v>77</v>
       </c>
       <c r="C81" s="20" t="s">
-        <v>10</v>
+        <v>77</v>
       </c>
       <c r="D81" s="20" t="s">
         <v>8</v>
@@ -5111,7 +5716,7 @@
         <v>78</v>
       </c>
       <c r="C82" s="20" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D82" s="20" t="s">
         <v>7</v>
@@ -5132,10 +5737,10 @@
         <v>79</v>
       </c>
       <c r="C83" s="20" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D83" s="20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E83" s="20" t="s">
         <v>59</v>
@@ -5240,7 +5845,7 @@
         <v>59</v>
       </c>
       <c r="D88" s="20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E88" s="20" t="s">
         <v>10</v>
@@ -5261,7 +5866,7 @@
         <v>59</v>
       </c>
       <c r="D89" s="20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E89" s="20" t="s">
         <v>10</v>
@@ -5345,7 +5950,7 @@
         <v>77</v>
       </c>
       <c r="D93" s="20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E93" s="20" t="s">
         <v>15</v>
@@ -5384,7 +5989,7 @@
         <v>91</v>
       </c>
       <c r="C95" s="20" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D95" s="20" t="s">
         <v>10</v>
@@ -5489,10 +6094,10 @@
         <v>96</v>
       </c>
       <c r="C100" s="20" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D100" s="20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E100" s="20" t="s">
         <v>15</v>
@@ -5506,7 +6111,7 @@
       <c r="H100" s="36"/>
       <c r="I100" s="25">
         <f>I127</f>
-        <v>0.51846029624859524</v>
+        <v>0.50630741199105156</v>
       </c>
     </row>
     <row r="101" spans="2:9">
@@ -5514,10 +6119,10 @@
         <v>97</v>
       </c>
       <c r="C101" s="20" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D101" s="20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E101" s="20" t="s">
         <v>77</v>
@@ -5556,7 +6161,7 @@
         <v>99</v>
       </c>
       <c r="C103" s="20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D103" s="20" t="s">
         <v>77</v>
@@ -5580,7 +6185,7 @@
         <v>15</v>
       </c>
       <c r="D104" s="20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E104" s="20" t="s">
         <v>77</v>
@@ -5664,7 +6269,7 @@
         <v>11</v>
       </c>
       <c r="D108" s="20" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E108" s="20" t="s">
         <v>11</v>
@@ -5682,7 +6287,7 @@
         <v>105</v>
       </c>
       <c r="C109" s="20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D109" s="20" t="s">
         <v>14</v>
@@ -5703,7 +6308,7 @@
         <v>106</v>
       </c>
       <c r="C110" s="20" t="s">
-        <v>77</v>
+        <v>9</v>
       </c>
       <c r="D110" s="20" t="s">
         <v>8</v>
@@ -5745,7 +6350,7 @@
         <v>108</v>
       </c>
       <c r="C112" s="20" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D112" s="20" t="s">
         <v>7</v>
@@ -5790,7 +6395,7 @@
         <v>77</v>
       </c>
       <c r="D114" s="20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E114" s="20" t="s">
         <v>15</v>
@@ -5811,7 +6416,7 @@
         <v>77</v>
       </c>
       <c r="D115" s="20" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E115" s="20" t="s">
         <v>8</v>
@@ -5913,7 +6518,7 @@
         <v>116</v>
       </c>
       <c r="C120" s="20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D120" s="20" t="s">
         <v>59</v>
@@ -6018,10 +6623,10 @@
         <v>121</v>
       </c>
       <c r="C125" s="20" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D125" s="20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E125" s="20" t="s">
         <v>7</v>
@@ -6039,7 +6644,7 @@
         <v>122</v>
       </c>
       <c r="C126" s="20" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D126" s="20" t="s">
         <v>13</v>
@@ -6077,7 +6682,7 @@
       <c r="H127" s="36"/>
       <c r="I127" s="25">
         <f>J147</f>
-        <v>0.51846029624859524</v>
+        <v>0.50630741199105156</v>
       </c>
     </row>
     <row r="128" spans="2:9">
@@ -6193,7 +6798,7 @@
         <v>15</v>
       </c>
       <c r="D133" s="53" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E133" s="20" t="s">
         <v>16</v>
@@ -6235,7 +6840,7 @@
         <v>9</v>
       </c>
       <c r="D135" s="53" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E135" s="51" t="s">
         <v>15</v>
@@ -6259,7 +6864,7 @@
         <v>12</v>
       </c>
       <c r="E136" s="53" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F136" s="53" t="s">
         <v>7</v>
@@ -6334,7 +6939,7 @@
         <v>11</v>
       </c>
       <c r="D140" s="53" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E140" s="53" t="s">
         <v>13</v>
@@ -6348,7 +6953,7 @@
         <v>137</v>
       </c>
       <c r="C141" s="20" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D141" s="53"/>
       <c r="E141" s="53" t="s">
@@ -6445,30 +7050,30 @@
       </c>
       <c r="J147" s="17">
         <f>Q181</f>
-        <v>0.51846029624859524</v>
+        <v>0.50630741199105156</v>
       </c>
     </row>
     <row r="148" spans="2:13">
       <c r="B148" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C148" s="22">
+      <c r="C148" s="66">
         <f t="shared" ref="C148:G160" si="1">COUNTIF(C$4:C$142,$B148)</f>
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D148" s="55">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="E148" s="22">
+      <c r="E148" s="66">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="F148" s="22">
+      <c r="F148" s="55">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="G148" s="22">
+      <c r="G148" s="66">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
@@ -6490,9 +7095,9 @@
       </c>
       <c r="C149" s="55">
         <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="D149" s="22">
+        <v>5</v>
+      </c>
+      <c r="D149" s="66">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
@@ -6500,11 +7105,11 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="F149" s="22">
+      <c r="F149" s="66">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="G149" s="22">
+      <c r="G149" s="55">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
@@ -6517,23 +7122,23 @@
       <c r="B150" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="C150" s="22">
+      <c r="C150" s="66">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="D150" s="55">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="E150" s="66">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="F150" s="55">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="D150" s="55">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="E150" s="22">
-        <f t="shared" si="1"/>
-        <v>19</v>
-      </c>
-      <c r="F150" s="22">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="G150" s="22">
+      <c r="G150" s="66">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
@@ -6548,21 +7153,21 @@
       </c>
       <c r="C151" s="55">
         <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="D151" s="22">
+        <v>5</v>
+      </c>
+      <c r="D151" s="66">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E151" s="55">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="F151" s="22">
+      <c r="F151" s="66">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="G151" s="22">
+      <c r="G151" s="55">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
@@ -6575,23 +7180,23 @@
       <c r="B152" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="C152" s="22">
+      <c r="C152" s="66">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D152" s="55">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="E152" s="22">
+      <c r="E152" s="66">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="F152" s="22">
+      <c r="F152" s="55">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="G152" s="22">
+      <c r="G152" s="66">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
@@ -6604,23 +7209,23 @@
       <c r="B153" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C153" s="22">
+      <c r="C153" s="66">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="D153" s="55">
         <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="E153" s="22">
+        <v>15</v>
+      </c>
+      <c r="E153" s="66">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="F153" s="66">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="F153" s="22">
-        <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="G153" s="22">
+      <c r="G153" s="55">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
@@ -6635,21 +7240,21 @@
       </c>
       <c r="C154" s="55">
         <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="D154" s="22">
+        <v>9</v>
+      </c>
+      <c r="D154" s="66">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E154" s="55">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="F154" s="22">
+      <c r="F154" s="66">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="G154" s="22">
+      <c r="G154" s="55">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
@@ -6662,23 +7267,23 @@
       <c r="B155" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="C155" s="22">
+      <c r="C155" s="66">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="D155" s="55">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="D155" s="55">
+      <c r="E155" s="66">
         <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="E155" s="22">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="F155" s="22">
+        <v>7</v>
+      </c>
+      <c r="F155" s="55">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="G155" s="22">
+      <c r="G155" s="66">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
@@ -6693,21 +7298,21 @@
       </c>
       <c r="C156" s="55">
         <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="D156" s="22">
+        <v>9</v>
+      </c>
+      <c r="D156" s="66">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E156" s="55">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="F156" s="22">
+      <c r="F156" s="66">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="G156" s="22">
+      <c r="G156" s="55">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
@@ -6720,23 +7325,23 @@
       <c r="B157" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C157" s="22">
+      <c r="C157" s="66">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D157" s="55">
         <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="E157" s="22">
+        <v>8</v>
+      </c>
+      <c r="E157" s="66">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="F157" s="22">
+      <c r="F157" s="55">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="G157" s="22">
+      <c r="G157" s="66">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
@@ -6749,15 +7354,15 @@
       <c r="B158" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="C158" s="22">
+      <c r="C158" s="66">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="D158" s="22">
+      <c r="D158" s="66">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E158" s="22">
+      <c r="E158" s="66">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7019,7 +7624,7 @@
       </c>
       <c r="C168" s="22">
         <f t="shared" ref="C168:C180" si="5">C148/C$161</f>
-        <v>0.1079136690647482</v>
+        <v>0.12949640287769784</v>
       </c>
       <c r="D168" s="22">
         <f t="shared" ref="D168:G168" si="6">D148/D$161</f>
@@ -7053,15 +7658,15 @@
       </c>
       <c r="N168" s="22">
         <f>((1-$H168)*($C168+C$167)*($D168+D$167)*($E168+E$167)*(1-F$167-$F168)+H168*($C168+C$167+C$179)*($D168+D$167+D$179)*($E168+E$167+E$179)*(1-F$167-$F168-F$179))*$E187-(1-F$167-F168-$H168*F$179)*$E187*PRODUCT(C$167:E$167)</f>
-        <v>4.0268095962927762E-2</v>
+        <v>4.6548423290130696E-2</v>
       </c>
       <c r="O168" s="22">
         <f>((1-$H168)*($C168+C$167)*($D168+D$167)*($E168+E$167)*(F$167+$F168)*(1-G$167-G168)+H168*($C168+C$167+C$179)*($D168+D$167+D$179)*($E168+E$167+E$179)*(F$167+$F168+F$179)*(1-G$167-G168-G$179))*F187-(1-G$167-G168-$H168*G$179)*$F187*PRODUCT(C$167:F$167)</f>
-        <v>2.5222463228107481E-2</v>
+        <v>2.9042556095529564E-2</v>
       </c>
       <c r="P168" s="22">
         <f>((1-$H168)*($C168+C$167)*($D168+D$167)*($E168+E$167)*(F$167+$F168)*(G$167+G168)+H168*($C168+C$167+C$179)*($D168+D$167+D$179)*($E168+E$167+E$179)*(F$167+$F168+F$179)*(+G$167+G168+G$179))*G187-PRODUCT(C$167:G$167)*G187</f>
-        <v>1.0172026044623805E-2</v>
+        <v>1.1645548082965645E-2</v>
       </c>
       <c r="Q168" s="22"/>
       <c r="T168" s="22" t="s">
@@ -7082,7 +7687,7 @@
       </c>
       <c r="C169" s="22">
         <f t="shared" si="5"/>
-        <v>5.7553956834532377E-2</v>
+        <v>3.5971223021582732E-2</v>
       </c>
       <c r="D169" s="22">
         <f t="shared" ref="D169:G169" si="8">D149/D$161</f>
@@ -7115,15 +7720,15 @@
       </c>
       <c r="N169" s="22">
         <f t="shared" ref="N169:N177" si="10">((1-$H169)*($C169+C$167)*($D169+D$167)*($E169+E$167)*(1-F$167-$F169)+H169*($C169+C$167+C$179)*($D169+D$167+D$179)*($E169+E$167+E$179)*(1-F$167-$F169-F$179))*$E188-(1-F$167-F169-$H169*F$179)*$E188*PRODUCT(C$167:E$167)</f>
-        <v>3.3349508701798404E-2</v>
+        <v>2.5290363998796028E-2</v>
       </c>
       <c r="O169" s="22">
         <f t="shared" ref="O169:O177" si="11">((1-$H169)*($C169+C$167)*($D169+D$167)*($E169+E$167)*(F$167+$F169)*(1-G$167-G169)+H169*($C169+C$167+C$179)*($D169+D$167+D$179)*($E169+E$167+E$179)*(F$167+$F169+F$179)*(1-G$167-G169-G$179))*F188-(1-G$167-G169-$H169*G$179)*$F188*PRODUCT(C$167:F$167)</f>
-        <v>2.710324312085368E-2</v>
+        <v>2.0791181739657327E-2</v>
       </c>
       <c r="P169" s="22">
         <f t="shared" ref="P169:P177" si="12">((1-$H169)*($C169+C$167)*($D169+D$167)*($E169+E$167)*(F$167+$F169)*(G$167+G169)+H169*($C169+C$167+C$179)*($D169+D$167+D$179)*($E169+E$167+E$179)*(F$167+$F169+F$179)*(+G$167+G169+G$179))*G188-PRODUCT(C$167:G$167)*G188</f>
-        <v>1.076657275366528E-2</v>
+        <v>8.4171942016305103E-3</v>
       </c>
       <c r="Q169" s="22"/>
       <c r="T169" s="22" t="s">
@@ -7142,11 +7747,11 @@
       </c>
       <c r="C170" s="22">
         <f t="shared" si="5"/>
-        <v>0.11510791366906475</v>
+        <v>0.12949640287769784</v>
       </c>
       <c r="D170" s="22">
         <f t="shared" ref="D170:G170" si="13">D150/D$161</f>
-        <v>6.569343065693431E-2</v>
+        <v>5.8394160583941604E-2</v>
       </c>
       <c r="E170" s="22">
         <f t="shared" si="13"/>
@@ -7175,15 +7780,15 @@
       </c>
       <c r="N170" s="22">
         <f t="shared" si="10"/>
-        <v>4.0234749775790883E-2</v>
+        <v>4.081811492605035E-2</v>
       </c>
       <c r="O170" s="22">
         <f t="shared" si="11"/>
-        <v>3.1870300741781675E-2</v>
+        <v>3.2339749810836052E-2</v>
       </c>
       <c r="P170" s="22">
         <f t="shared" si="12"/>
-        <v>1.5697561706499531E-2</v>
+        <v>1.5936431162747164E-2</v>
       </c>
       <c r="Q170" s="22"/>
       <c r="T170" s="22" t="s">
@@ -7202,11 +7807,11 @@
       </c>
       <c r="C171" s="22">
         <f t="shared" si="5"/>
-        <v>7.1942446043165464E-2</v>
+        <v>3.5971223021582732E-2</v>
       </c>
       <c r="D171" s="22">
         <f t="shared" ref="D171:G171" si="15">D151/D$161</f>
-        <v>0.145985401459854</v>
+        <v>0.15328467153284672</v>
       </c>
       <c r="E171" s="22">
         <f t="shared" si="15"/>
@@ -7235,15 +7840,15 @@
       </c>
       <c r="N171" s="22">
         <f t="shared" si="10"/>
-        <v>3.77540530981509E-2</v>
+        <v>2.6059059358126233E-2</v>
       </c>
       <c r="O171" s="22">
         <f t="shared" si="11"/>
-        <v>3.0110634866081485E-2</v>
+        <v>2.1123524534317175E-2</v>
       </c>
       <c r="P171" s="22">
         <f t="shared" si="12"/>
-        <v>1.2827891605685033E-2</v>
+        <v>9.2100746173218295E-3</v>
       </c>
       <c r="Q171" s="22"/>
       <c r="T171" s="22" t="s">
@@ -7262,7 +7867,7 @@
       </c>
       <c r="C172" s="22">
         <f t="shared" si="5"/>
-        <v>0.12949640287769784</v>
+        <v>0.14388489208633093</v>
       </c>
       <c r="D172" s="22">
         <f t="shared" ref="D172:G172" si="17">D152/D$161</f>
@@ -7295,15 +7900,15 @@
       </c>
       <c r="N172" s="22">
         <f t="shared" si="10"/>
-        <v>3.8924474225045351E-2</v>
+        <v>4.2305757572984916E-2</v>
       </c>
       <c r="O172" s="22">
         <f t="shared" si="11"/>
-        <v>3.6447463482552345E-2</v>
+        <v>3.954705629892339E-2</v>
       </c>
       <c r="P172" s="22">
         <f t="shared" si="12"/>
-        <v>1.4623457192226465E-2</v>
+        <v>1.5829553283270834E-2</v>
       </c>
       <c r="Q172" s="22"/>
       <c r="T172" s="22" t="s">
@@ -7326,11 +7931,11 @@
       </c>
       <c r="D173" s="22">
         <f t="shared" ref="D173:G173" si="19">D153/D$161</f>
-        <v>5.8394160583941604E-2</v>
+        <v>0.10948905109489052</v>
       </c>
       <c r="E173" s="22">
         <f t="shared" si="19"/>
-        <v>7.9710144927536225E-2</v>
+        <v>8.6956521739130432E-2</v>
       </c>
       <c r="F173" s="22">
         <f t="shared" si="19"/>
@@ -7355,15 +7960,15 @@
       </c>
       <c r="N173" s="22">
         <f t="shared" si="10"/>
-        <v>1.0596372657173335E-2</v>
+        <v>1.7691266319153336E-2</v>
       </c>
       <c r="O173" s="22">
         <f t="shared" si="11"/>
-        <v>9.9655403671328E-3</v>
+        <v>1.6328005463818327E-2</v>
       </c>
       <c r="P173" s="22">
         <f t="shared" si="12"/>
-        <v>1.4806088850037409E-3</v>
+        <v>2.3459373360955635E-3</v>
       </c>
       <c r="Q173" s="22"/>
       <c r="T173" s="22" t="s">
@@ -7382,11 +7987,11 @@
       </c>
       <c r="C174" s="22">
         <f t="shared" si="5"/>
-        <v>5.0359712230215826E-2</v>
+        <v>6.4748201438848921E-2</v>
       </c>
       <c r="D174" s="22">
         <f t="shared" ref="D174:G174" si="21">D154/D$161</f>
-        <v>0.12408759124087591</v>
+        <v>7.2992700729927001E-2</v>
       </c>
       <c r="E174" s="22">
         <f t="shared" si="21"/>
@@ -7415,15 +8020,15 @@
       </c>
       <c r="N174" s="22">
         <f t="shared" si="10"/>
-        <v>1.0742398724482448E-2</v>
+        <v>8.5018620686378391E-3</v>
       </c>
       <c r="O174" s="22">
         <f t="shared" si="11"/>
-        <v>7.9182788007042208E-3</v>
+        <v>6.3151439399149354E-3</v>
       </c>
       <c r="P174" s="22">
         <f t="shared" si="12"/>
-        <v>1.4016935585544187E-3</v>
+        <v>1.1278668076066193E-3</v>
       </c>
       <c r="Q174" s="22"/>
       <c r="T174" s="22" t="s">
@@ -7442,15 +8047,15 @@
       </c>
       <c r="C175" s="22">
         <f t="shared" si="5"/>
-        <v>8.6330935251798566E-2</v>
+        <v>7.9136690647482008E-2</v>
       </c>
       <c r="D175" s="22">
         <f t="shared" ref="D175:G175" si="23">D155/D$161</f>
-        <v>0.10948905109489052</v>
+        <v>8.7591240875912413E-2</v>
       </c>
       <c r="E175" s="22">
         <f t="shared" si="23"/>
-        <v>5.7971014492753624E-2</v>
+        <v>5.0724637681159424E-2</v>
       </c>
       <c r="F175" s="22">
         <f t="shared" si="23"/>
@@ -7475,15 +8080,15 @@
       </c>
       <c r="N175" s="22">
         <f t="shared" si="10"/>
-        <v>1.1576446804940591E-2</v>
+        <v>8.3562615908041923E-3</v>
       </c>
       <c r="O175" s="22">
         <f t="shared" si="11"/>
-        <v>7.0884581157055569E-3</v>
+        <v>5.1723942875478634E-3</v>
       </c>
       <c r="P175" s="22">
         <f t="shared" si="12"/>
-        <v>1.0561913759375384E-3</v>
+        <v>7.9026790359564328E-4</v>
       </c>
       <c r="Q175" s="22"/>
       <c r="T175" s="22" t="s">
@@ -7502,11 +8107,11 @@
       </c>
       <c r="C176" s="22">
         <f t="shared" si="5"/>
-        <v>5.7553956834532377E-2</v>
+        <v>6.4748201438848921E-2</v>
       </c>
       <c r="D176" s="22">
         <f>D156/D$161</f>
-        <v>0.11678832116788321</v>
+        <v>0.12408759124087591</v>
       </c>
       <c r="E176" s="22">
         <f t="shared" ref="E176:G176" si="25">E156/E$161</f>
@@ -7535,15 +8140,15 @@
       </c>
       <c r="N176" s="22">
         <f t="shared" si="10"/>
-        <v>8.6451438587129715E-3</v>
+        <v>9.8396519193661922E-3</v>
       </c>
       <c r="O176" s="22">
         <f t="shared" si="11"/>
-        <v>3.6880050438959475E-3</v>
+        <v>4.1734949757866084E-3</v>
       </c>
       <c r="P176" s="22">
         <f t="shared" si="12"/>
-        <v>9.1152461434476954E-4</v>
+        <v>1.0237593751900101E-3</v>
       </c>
       <c r="Q176" s="22"/>
       <c r="T176" s="22" t="s">
@@ -7562,11 +8167,11 @@
       </c>
       <c r="C177" s="22">
         <f t="shared" si="5"/>
-        <v>9.3525179856115109E-2</v>
+        <v>8.6330935251798566E-2</v>
       </c>
       <c r="D177" s="22">
         <f>D157/D$161</f>
-        <v>4.3795620437956206E-2</v>
+        <v>5.8394160583941604E-2</v>
       </c>
       <c r="E177" s="22">
         <f t="shared" ref="E177:G177" si="27">E157/E$161</f>
@@ -7595,15 +8200,15 @@
       </c>
       <c r="N177" s="22">
         <f t="shared" si="10"/>
-        <v>8.9366011217674544E-3</v>
+        <v>1.0128662937032257E-2</v>
       </c>
       <c r="O177" s="22">
         <f t="shared" si="11"/>
-        <v>3.4349904703191167E-3</v>
+        <v>3.8651227400240806E-3</v>
       </c>
       <c r="P177" s="22">
         <f t="shared" si="12"/>
-        <v>8.4976733187048094E-4</v>
+        <v>9.4734734093060641E-4</v>
       </c>
       <c r="Q177" s="22"/>
       <c r="T177" s="22" t="s">
@@ -7778,7 +8383,7 @@
       </c>
       <c r="C181" s="29">
         <f t="shared" ref="C181:H181" si="33">SUM(C167:C180)</f>
-        <v>0.99999999999999989</v>
+        <v>1</v>
       </c>
       <c r="D181" s="29">
         <f t="shared" si="33"/>
@@ -7810,7 +8415,7 @@
       <c r="P181" s="30"/>
       <c r="Q181" s="30">
         <f>SUM(L167:P180)</f>
-        <v>0.51846029624859524</v>
+        <v>0.50630741199105156</v>
       </c>
       <c r="T181" s="28" t="s">
         <v>57</v>
@@ -7944,7 +8549,7 @@
       </c>
       <c r="R186" s="17">
         <f t="shared" si="34"/>
-        <v>1.4177279523465219E-3</v>
+        <v>1.6898405643688962E-3</v>
       </c>
     </row>
     <row r="187" spans="2:26">
@@ -7991,7 +8596,7 @@
       </c>
       <c r="R187" s="17">
         <f t="shared" si="34"/>
-        <v>4.164089024998173E-3</v>
+        <v>4.9397419377631572E-3</v>
       </c>
     </row>
     <row r="188" spans="2:26">
@@ -8038,7 +8643,7 @@
       </c>
       <c r="R188" s="17">
         <f t="shared" si="34"/>
-        <v>7.0543279514160917E-3</v>
+        <v>8.3813516997551553E-3</v>
       </c>
     </row>
     <row r="189" spans="2:26">
@@ -8132,11 +8737,11 @@
       </c>
       <c r="R190" s="17">
         <f t="shared" si="34"/>
-        <v>2.1623736318986418E-2</v>
+        <v>2.5529274373062925E-2</v>
       </c>
       <c r="S190" s="17">
         <f>SUM(R184:R190)</f>
-        <v>4.0268095962927769E-2</v>
+        <v>4.6548423290130696E-2</v>
       </c>
     </row>
     <row r="191" spans="2:26">
@@ -8347,184 +8952,52 @@
     <mergeCell ref="B145:H145"/>
     <mergeCell ref="B165:H165"/>
   </mergeCells>
-  <conditionalFormatting sqref="A163:F163 A1:H162 A164:H1048576">
-    <cfRule type="containsText" dxfId="25" priority="48" operator="containsText" text="Lion">
+  <conditionalFormatting sqref="A1:Z1048576">
+    <cfRule type="containsText" dxfId="5" priority="14" operator="containsText" text="Lion">
       <formula>NOT(ISERROR(SEARCH("Lion",A1)))</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T27:T141 T1:T15 A142:T162 A163:R163 A1:L141 A164:T1048576">
-    <cfRule type="containsText" dxfId="24" priority="47" operator="containsText" text="Elephant">
+    <cfRule type="containsText" dxfId="6" priority="13" operator="containsText" text="Elephant">
       <formula>NOT(ISERROR(SEARCH("Elephant",A1)))</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A142:Q162 A163:O163 A1:L141 A164:Q1048576">
-    <cfRule type="containsText" dxfId="23" priority="46" operator="containsText" text="Leopard">
-      <formula>NOT(ISERROR(SEARCH("Leopard",A1)))</formula>
+    <cfRule type="containsText" dxfId="7" priority="12" operator="containsText" text="Ace">
+      <formula>NOT(ISERROR(SEARCH("Ace",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="11" operator="containsText" text="King">
+      <formula>NOT(ISERROR(SEARCH("King",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="Inner">
+      <formula>NOT(ISERROR(SEARCH("Inner",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A142:S162 A163:Q163 A1:L141 A164:S1048576">
-    <cfRule type="containsText" dxfId="22" priority="45" operator="containsText" text="WaterBuffalo">
-      <formula>NOT(ISERROR(SEARCH("WaterBuffalo",A1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T27:Z141 T16:Y26 T1:Z15 A142:Z162 A163:X163 A1:L141 A164:Z1048576">
-    <cfRule type="containsText" dxfId="21" priority="44" operator="containsText" text="Rhino">
+  <conditionalFormatting sqref="A1:XFD1048576">
+    <cfRule type="containsText" dxfId="45" priority="10" operator="containsText" text="Rhino">
       <formula>NOT(ISERROR(SEARCH("Rhino",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T27:V141 T16:U26 T1:V15 A142:V162 A163:T163 A1:L141 A164:V1048576">
-    <cfRule type="containsText" dxfId="20" priority="43" operator="containsText" text="Wild">
+  <conditionalFormatting sqref="A1:U1048576">
+    <cfRule type="containsText" dxfId="17" priority="9" operator="containsText" text="Wild">
       <formula>NOT(ISERROR(SEARCH("Wild",A1)))</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T27:X141 T16:W26 T1:X15 A142:X162 A163:V163 A1:L141 A164:X1048576">
-    <cfRule type="containsText" dxfId="19" priority="42" operator="containsText" text="Ace">
-      <formula>NOT(ISERROR(SEARCH("Ace",A1)))</formula>
+    <cfRule type="containsText" dxfId="18" priority="8" operator="containsText" text="Leopard">
+      <formula>NOT(ISERROR(SEARCH("Leopard",A1)))</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T27:U141 T16:T26 T1:U15 A142:U162 A163:S163 A1:L141 A164:U1048576">
-    <cfRule type="containsText" dxfId="18" priority="41" operator="containsText" text="King">
-      <formula>NOT(ISERROR(SEARCH("King",A1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T27:W141 T16:V26 T1:W15 A142:W162 A163:U163 A1:L141 A164:W1048576">
-    <cfRule type="containsText" dxfId="17" priority="40" operator="containsText" text="Queen">
+    <cfRule type="containsText" dxfId="19" priority="7" operator="containsText" text="Queen">
       <formula>NOT(ISERROR(SEARCH("Queen",A1)))</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T27:Y141 T16:X26 T1:Y15 A142:Y162 A163:W163 A1:L141 A164:Y1048576">
-    <cfRule type="containsText" dxfId="16" priority="39" operator="containsText" text="Jack">
+    <cfRule type="containsText" dxfId="20" priority="6" operator="containsText" text="Jack">
       <formula>NOT(ISERROR(SEARCH("Jack",A1)))</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T27:V141 T16:U26 T1:V15 B142:V162 B163:T163 B1:L141 B164:V1048576">
-    <cfRule type="containsText" dxfId="15" priority="38" operator="containsText" text="Ten">
-      <formula>NOT(ISERROR(SEARCH("Ten",B1)))</formula>
+    <cfRule type="containsText" dxfId="21" priority="5" operator="containsText" text="WaterBuffalo">
+      <formula>NOT(ISERROR(SEARCH("WaterBuffalo",A1)))</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T27:AA141 T16:Z26 T1:AA15 A142:AA162 A163:Y163 A1:L141 A164:AA1048576">
-    <cfRule type="containsText" dxfId="14" priority="37" operator="containsText" text="Collector">
+    <cfRule type="containsText" dxfId="22" priority="4" operator="containsText" text="Ten">
+      <formula>NOT(ISERROR(SEARCH("Ten",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="23" priority="3" operator="containsText" text="Collector">
       <formula>NOT(ISERROR(SEARCH("Collector",A1)))</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A142:O162 A163:M163 A1:L141 A164:O1048576">
-    <cfRule type="containsText" dxfId="13" priority="36" operator="containsText" text="Scatter">
+    <cfRule type="containsText" dxfId="16" priority="2" operator="containsText" text="Scatter">
       <formula>NOT(ISERROR(SEARCH("Scatter",A1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:H142">
-    <cfRule type="containsText" dxfId="12" priority="23" operator="containsText" text="Lion">
-      <formula>NOT(ISERROR(SEARCH("Lion",B2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:H142">
-    <cfRule type="containsText" dxfId="11" priority="22" operator="containsText" text="Elephant">
-      <formula>NOT(ISERROR(SEARCH("Elephant",B2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:H142">
-    <cfRule type="containsText" dxfId="10" priority="21" operator="containsText" text="Leopard">
-      <formula>NOT(ISERROR(SEARCH("Leopard",B2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:H142">
-    <cfRule type="containsText" dxfId="9" priority="20" operator="containsText" text="WaterBuffalo">
-      <formula>NOT(ISERROR(SEARCH("WaterBuffalo",B2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:H142">
-    <cfRule type="containsText" dxfId="8" priority="19" operator="containsText" text="Rhino">
-      <formula>NOT(ISERROR(SEARCH("Rhino",B2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:H142">
-    <cfRule type="containsText" dxfId="7" priority="18" operator="containsText" text="Wild">
-      <formula>NOT(ISERROR(SEARCH("Wild",B2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:H142">
-    <cfRule type="containsText" dxfId="6" priority="17" operator="containsText" text="Ace">
-      <formula>NOT(ISERROR(SEARCH("Ace",B2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:H142">
-    <cfRule type="containsText" dxfId="5" priority="16" operator="containsText" text="King">
-      <formula>NOT(ISERROR(SEARCH("King",B2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:H142">
-    <cfRule type="containsText" dxfId="4" priority="15" operator="containsText" text="Queen">
-      <formula>NOT(ISERROR(SEARCH("Queen",B2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:H142">
-    <cfRule type="containsText" dxfId="3" priority="14" operator="containsText" text="Jack">
-      <formula>NOT(ISERROR(SEARCH("Jack",B2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:H142">
-    <cfRule type="containsText" dxfId="2" priority="13" operator="containsText" text="Ten">
-      <formula>NOT(ISERROR(SEARCH("Ten",B2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:H142">
-    <cfRule type="containsText" dxfId="1" priority="12" operator="containsText" text="Collector">
-      <formula>NOT(ISERROR(SEARCH("Collector",B2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:H142">
-    <cfRule type="containsText" dxfId="0" priority="11" operator="containsText" text="Scatter">
-      <formula>NOT(ISERROR(SEARCH("Scatter",B2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E39:E46">
-    <cfRule type="containsText" dxfId="40" priority="10" operator="containsText" text="Lion">
-      <formula>NOT(ISERROR(SEARCH("Lion",E39)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E39:E46">
-    <cfRule type="containsText" dxfId="39" priority="9" operator="containsText" text="Scatter">
-      <formula>NOT(ISERROR(SEARCH("Scatter",E39)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D39:D46">
-    <cfRule type="containsText" dxfId="38" priority="8" operator="containsText" text="Lion">
-      <formula>NOT(ISERROR(SEARCH("Lion",D39)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D39:D46">
-    <cfRule type="containsText" dxfId="37" priority="7" operator="containsText" text="Scatter">
-      <formula>NOT(ISERROR(SEARCH("Scatter",D39)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F39:F46">
-    <cfRule type="containsText" dxfId="36" priority="6" operator="containsText" text="Lion">
-      <formula>NOT(ISERROR(SEARCH("Lion",F39)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F39:F46">
-    <cfRule type="containsText" dxfId="35" priority="5" operator="containsText" text="Scatter">
-      <formula>NOT(ISERROR(SEARCH("Scatter",F39)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C43:C50">
-    <cfRule type="containsText" dxfId="34" priority="3" operator="containsText" text="Scatter">
-      <formula>NOT(ISERROR(SEARCH("Scatter",C43)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C43:C50">
-    <cfRule type="containsText" dxfId="33" priority="4" operator="containsText" text="Lion">
-      <formula>NOT(ISERROR(SEARCH("Lion",C43)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G43:G50">
-    <cfRule type="containsText" dxfId="32" priority="1" operator="containsText" text="Scatter">
-      <formula>NOT(ISERROR(SEARCH("Scatter",G43)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G43:G50">
-    <cfRule type="containsText" dxfId="31" priority="2" operator="containsText" text="Lion">
-      <formula>NOT(ISERROR(SEARCH("Lion",G43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8533,91 +9006,50 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62C8EC9A-A08D-4866-80BC-02E5AB308ABB}">
-  <dimension ref="B2:F8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5FC7C96-84EA-4EC5-9C52-FA453D2DB974}">
+  <dimension ref="B2:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="30.21875" customWidth="1"/>
+    <col min="2" max="2" width="23.109375" customWidth="1"/>
+    <col min="3" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6">
-      <c r="B2" s="66" t="s">
+    <row r="2" spans="2:5">
+      <c r="B2" t="s">
         <v>90</v>
       </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="65" t="s">
+      <c r="C2" t="s">
         <v>88</v>
       </c>
-      <c r="E2" s="65" t="s">
+      <c r="D2" t="s">
         <v>89</v>
       </c>
-      <c r="F2" s="65" t="s">
+      <c r="E2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="2:6">
-      <c r="B3" s="68"/>
-      <c r="C3" s="69"/>
+    <row r="3" spans="2:5">
+      <c r="B3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" s="65">
+        <f>ROUND('Outer Collector Reels'!C162*1000,0)</f>
+        <v>154</v>
+      </c>
       <c r="D3" s="65">
-        <v>15</v>
+        <f>E3-C3</f>
+        <v>846</v>
       </c>
       <c r="E3" s="65">
-        <v>85</v>
-      </c>
-      <c r="F3" s="65">
-        <f>SUM(D3:E3)</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6">
-      <c r="B7" s="66" t="s">
-        <v>91</v>
-      </c>
-      <c r="C7" s="67"/>
-      <c r="D7" s="65" t="s">
-        <v>88</v>
-      </c>
-      <c r="E7" s="65" t="s">
-        <v>89</v>
-      </c>
-      <c r="F7" s="65" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6">
-      <c r="B8" s="68"/>
-      <c r="C8" s="69"/>
-      <c r="D8" s="65">
-        <v>15</v>
-      </c>
-      <c r="E8" s="65">
-        <v>85</v>
-      </c>
-      <c r="F8" s="65">
-        <f>SUM(D8:E8)</f>
-        <v>100</v>
+        <v>1000</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="B7:C8"/>
-  </mergeCells>
-  <conditionalFormatting sqref="B2 D2:F3">
-    <cfRule type="containsText" dxfId="30" priority="2" operator="containsText" text="Collector">
-      <formula>NOT(ISERROR(SEARCH("Collector",B2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B7 D7:F8">
-    <cfRule type="containsText" dxfId="26" priority="1" operator="containsText" text="Collector">
-      <formula>NOT(ISERROR(SEARCH("Collector",B7)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -8626,8 +9058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5091FB6-A1FC-4569-9527-D3BFD417E752}">
   <dimension ref="B2:N170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J72" sqref="J72"/>
+    <sheetView topLeftCell="A136" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F157" sqref="F157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -8766,14 +9198,14 @@
       <c r="C8" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="D8" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="E8" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="F8" s="20" t="s">
-        <v>64</v>
+      <c r="D8" s="51" t="s">
+        <v>79</v>
+      </c>
+      <c r="E8" s="51" t="s">
+        <v>79</v>
+      </c>
+      <c r="F8" s="51" t="s">
+        <v>79</v>
       </c>
       <c r="G8" s="20" t="s">
         <v>79</v>
@@ -8914,13 +9346,13 @@
         <v>79</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="G15" s="20" t="s">
         <v>79</v>
@@ -9012,7 +9444,7 @@
       <c r="H19" s="36"/>
       <c r="I19" s="25">
         <f>I62</f>
-        <v>30.834946484707782</v>
+        <v>3.8611111111111112</v>
       </c>
     </row>
     <row r="20" spans="2:9">
@@ -9919,7 +10351,7 @@
       <c r="H62" s="36"/>
       <c r="I62" s="25">
         <f>I127</f>
-        <v>30.834946484707782</v>
+        <v>3.8611111111111112</v>
       </c>
     </row>
     <row r="63" spans="2:9">
@@ -9993,13 +10425,13 @@
         <v>79</v>
       </c>
       <c r="D66" s="20" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="E66" s="20" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="F66" s="20" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="G66" s="20" t="s">
         <v>79</v>
@@ -10392,13 +10824,13 @@
         <v>79</v>
       </c>
       <c r="D85" s="20" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="E85" s="20" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="F85" s="20" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="G85" s="20" t="s">
         <v>79</v>
@@ -10812,13 +11244,13 @@
         <v>79</v>
       </c>
       <c r="D105" s="20" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="E105" s="20" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="F105" s="20" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="G105" s="20" t="s">
         <v>79</v>
@@ -11287,8 +11719,8 @@
       </c>
       <c r="H127" s="36"/>
       <c r="I127" s="25">
-        <f>C162</f>
-        <v>30.834946484707782</v>
+        <f>C165</f>
+        <v>3.8611111111111112</v>
       </c>
     </row>
     <row r="128" spans="2:9">
@@ -11593,13 +12025,13 @@
         <v>79</v>
       </c>
       <c r="D142" s="20" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="E142" s="20" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="F142" s="20" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="G142" s="20" t="s">
         <v>79</v>
@@ -11824,6 +12256,22 @@
       </c>
     </row>
     <row r="156" spans="2:10">
+      <c r="C156" s="17">
+        <f>1/C160</f>
+        <v>0.21620490471656631</v>
+      </c>
+      <c r="D156" s="17">
+        <f t="shared" ref="D156:E156" si="4">1/D160</f>
+        <v>2.0428809894478706E-2</v>
+      </c>
+      <c r="E156" s="17">
+        <f t="shared" si="4"/>
+        <v>6.4342708329066789E-4</v>
+      </c>
+      <c r="F156" s="17">
+        <f>1/SUM(C156:E156)</f>
+        <v>4.2144809772203704</v>
+      </c>
       <c r="H156" s="17" t="s">
         <v>82</v>
       </c>
@@ -11840,11 +12288,11 @@
         <v>8.6330935251798566E-2</v>
       </c>
       <c r="I157" s="17">
-        <f t="shared" ref="I157:J157" si="4">E153</f>
+        <f t="shared" ref="I157:J157" si="5">E153</f>
         <v>8.6330935251798566E-2</v>
       </c>
       <c r="J157" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.6330935251798566E-2</v>
       </c>
     </row>
@@ -11874,11 +12322,11 @@
         <v>0.91366906474820142</v>
       </c>
       <c r="I159" s="17">
-        <f t="shared" ref="I159:J159" si="5">1-I157</f>
+        <f t="shared" ref="I159:J159" si="6">1-I157</f>
         <v>0.91366906474820142</v>
       </c>
       <c r="J159" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.91366906474820142</v>
       </c>
     </row>
@@ -11901,16 +12349,8 @@
     </row>
     <row r="162" spans="3:14">
       <c r="C162" s="17">
-        <f>C160/'Outer Reels Weights'!$D3*'Outer Reels Weights'!$F3</f>
-        <v>30.834946484707782</v>
-      </c>
-      <c r="D162" s="17">
-        <f>D160/'Outer Reels Weights'!$D3*'Outer Reels Weights'!$F3</f>
-        <v>326.33651696315735</v>
-      </c>
-      <c r="E162" s="17">
-        <f>E160/'Outer Reels Weights'!$D3*'Outer Reels Weights'!$F3</f>
-        <v>10361.184413580246</v>
+        <f>C160/30</f>
+        <v>0.15417473242353891</v>
       </c>
       <c r="H162" s="17" t="s">
         <v>82</v>
@@ -11926,11 +12366,11 @@
         <v>8.6330935251798566E-2</v>
       </c>
       <c r="L162" s="17">
-        <f t="shared" ref="L162:M170" si="6">IF(I162=$H$156,$H$157,IF(I162=$H$158,$H$159,IF(I162=$I$156,$I$157,IF(I162=$I$158,$I$159,IF(I162=$J$156,$J$157,IF(I162=$J$158,$J$159,0))))))</f>
+        <f t="shared" ref="L162:M170" si="7">IF(I162=$H$156,$H$157,IF(I162=$H$158,$H$159,IF(I162=$I$156,$I$157,IF(I162=$I$158,$I$159,IF(I162=$J$156,$J$157,IF(I162=$J$158,$J$159,0))))))</f>
         <v>0.91366906474820142</v>
       </c>
       <c r="M162" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.91366906474820142</v>
       </c>
       <c r="N162" s="17">
@@ -11949,19 +12389,19 @@
         <v>87</v>
       </c>
       <c r="K163" s="17">
-        <f t="shared" ref="K163:K170" si="7">IF(H163=$H$156,$H$157,IF(H163=$H$158,$H$159,IF(H163=$I$156,$I$157,IF(H163=$I$158,$I$159,IF(H163=$J$156,$J$157,IF(H163=$J$158,$J$159,0))))))</f>
+        <f t="shared" ref="K163:K170" si="8">IF(H163=$H$156,$H$157,IF(H163=$H$158,$H$159,IF(H163=$I$156,$I$157,IF(H163=$I$158,$I$159,IF(H163=$J$156,$J$157,IF(H163=$J$158,$J$159,0))))))</f>
         <v>0.91366906474820142</v>
       </c>
       <c r="L163" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>8.6330935251798566E-2</v>
       </c>
       <c r="M163" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.91366906474820142</v>
       </c>
       <c r="N163" s="17">
-        <f t="shared" ref="N163:N170" si="8">PRODUCT(K163:M163)</f>
+        <f t="shared" ref="N163:N170" si="9">PRODUCT(K163:M163)</f>
         <v>7.206830157218877E-2</v>
       </c>
     </row>
@@ -11976,37 +12416,41 @@
         <v>84</v>
       </c>
       <c r="K164" s="17">
+        <f t="shared" si="8"/>
+        <v>0.91366906474820142</v>
+      </c>
+      <c r="L164" s="17">
         <f t="shared" si="7"/>
         <v>0.91366906474820142</v>
       </c>
-      <c r="L164" s="17">
-        <f t="shared" si="6"/>
-        <v>0.91366906474820142</v>
-      </c>
       <c r="M164" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>8.6330935251798566E-2</v>
       </c>
       <c r="N164" s="17">
+        <f t="shared" si="9"/>
+        <v>7.206830157218877E-2</v>
+      </c>
+    </row>
+    <row r="165" spans="3:14">
+      <c r="C165" s="17">
+        <f>1/(D153+E153+F153)</f>
+        <v>3.8611111111111112</v>
+      </c>
+      <c r="K165" s="17">
         <f t="shared" si="8"/>
-        <v>7.206830157218877E-2</v>
-      </c>
-    </row>
-    <row r="165" spans="3:14">
-      <c r="K165" s="17">
+        <v>0</v>
+      </c>
+      <c r="L165" s="17">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="L165" s="17">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
       <c r="M165" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N165" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -12021,19 +12465,19 @@
         <v>87</v>
       </c>
       <c r="K166" s="17">
+        <f t="shared" si="8"/>
+        <v>8.6330935251798566E-2</v>
+      </c>
+      <c r="L166" s="17">
         <f t="shared" si="7"/>
         <v>8.6330935251798566E-2</v>
       </c>
-      <c r="L166" s="17">
-        <f t="shared" si="6"/>
-        <v>8.6330935251798566E-2</v>
-      </c>
       <c r="M166" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.91366906474820142</v>
       </c>
       <c r="N166" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.8096032981595682E-3</v>
       </c>
     </row>
@@ -12048,19 +12492,19 @@
         <v>84</v>
       </c>
       <c r="K167" s="17">
+        <f t="shared" si="8"/>
+        <v>8.6330935251798566E-2</v>
+      </c>
+      <c r="L167" s="17">
+        <f t="shared" si="7"/>
+        <v>0.91366906474820142</v>
+      </c>
+      <c r="M167" s="17">
         <f t="shared" si="7"/>
         <v>8.6330935251798566E-2</v>
       </c>
-      <c r="L167" s="17">
-        <f t="shared" si="6"/>
-        <v>0.91366906474820142</v>
-      </c>
-      <c r="M167" s="17">
-        <f t="shared" si="6"/>
-        <v>8.6330935251798566E-2</v>
-      </c>
       <c r="N167" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.8096032981595691E-3</v>
       </c>
     </row>
@@ -12075,37 +12519,37 @@
         <v>84</v>
       </c>
       <c r="K168" s="17">
+        <f t="shared" si="8"/>
+        <v>0.91366906474820142</v>
+      </c>
+      <c r="L168" s="17">
         <f t="shared" si="7"/>
-        <v>0.91366906474820142</v>
-      </c>
-      <c r="L168" s="17">
-        <f t="shared" si="6"/>
         <v>8.6330935251798566E-2</v>
       </c>
       <c r="M168" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>8.6330935251798566E-2</v>
       </c>
       <c r="N168" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.8096032981595691E-3</v>
       </c>
     </row>
     <row r="169" spans="3:14">
       <c r="K169" s="17">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L169" s="17">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="L169" s="17">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
       <c r="M169" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N169" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -12120,19 +12564,19 @@
         <v>84</v>
       </c>
       <c r="K170" s="17">
+        <f t="shared" si="8"/>
+        <v>8.6330935251798566E-2</v>
+      </c>
+      <c r="L170" s="17">
         <f t="shared" si="7"/>
         <v>8.6330935251798566E-2</v>
       </c>
-      <c r="L170" s="17">
-        <f t="shared" si="6"/>
+      <c r="M170" s="17">
+        <f t="shared" si="7"/>
         <v>8.6330935251798566E-2</v>
       </c>
-      <c r="M170" s="17">
-        <f t="shared" si="6"/>
-        <v>8.6330935251798566E-2</v>
-      </c>
       <c r="N170" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.4342708329066789E-4</v>
       </c>
     </row>
@@ -12142,18 +12586,18 @@
     <mergeCell ref="C2:H2"/>
     <mergeCell ref="B145:H145"/>
   </mergeCells>
-  <conditionalFormatting sqref="H16:Z26 H27:AA150 A143:G150 A151:A154 I151:AA154 A4:F142 A155:AA1048576 A3:AA3 A1:J2 P1:AA2 H9:AA15 H4:AA6 H7:J8 P7:AA8">
-    <cfRule type="containsText" dxfId="29" priority="14" operator="containsText" text="Collector">
+  <conditionalFormatting sqref="H16:Z26 H27:AA150 A143:G150 A151:A154 I151:AA154 A3:AA3 A1:J2 P1:AA2 H9:AA15 H4:AA6 H7:J8 P7:AA8 A4:F142 A155:AA1048576">
+    <cfRule type="containsText" dxfId="104" priority="14" operator="containsText" text="Collector">
       <formula>NOT(ISERROR(SEARCH("Collector",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B151:H154">
-    <cfRule type="containsText" dxfId="28" priority="2" operator="containsText" text="Collector">
+    <cfRule type="containsText" dxfId="103" priority="2" operator="containsText" text="Collector">
       <formula>NOT(ISERROR(SEARCH("Collector",B151)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:G142">
-    <cfRule type="containsText" dxfId="27" priority="1" operator="containsText" text="Collector">
+    <cfRule type="containsText" dxfId="102" priority="1" operator="containsText" text="Collector">
       <formula>NOT(ISERROR(SEARCH("Collector",G4)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Leopard Feature is added, need to check correctness of calculating Std.dev
</commit_message>
<xml_diff>
--- a/AnimalWill/AnimalWillMaths.xlsx
+++ b/AnimalWill/AnimalWillMaths.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\konstantin.d\source\repos\AnimalWill\AnimalWill\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31FBC4B7-F09F-493C-A6AC-0F000E1B56D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{817C64FB-CC46-4C44-8239-D1FC8E92C790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="7" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="9" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
     <sheet name="Lion Feature Reels" sheetId="7" r:id="rId12"/>
     <sheet name="Lion Feature Info" sheetId="22" r:id="rId13"/>
     <sheet name="ElephantFeature Reels" sheetId="8" r:id="rId14"/>
-    <sheet name="LeopardFeature Weights" sheetId="9" r:id="rId15"/>
+    <sheet name="Leopard Feature Weights" sheetId="9" r:id="rId15"/>
     <sheet name="RhinoFeature Reels" sheetId="10" r:id="rId16"/>
     <sheet name="BuffaloFeature Reels" sheetId="11" r:id="rId17"/>
   </sheets>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3386" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3409" uniqueCount="104">
   <si>
     <t xml:space="preserve">Slot Name: </t>
   </si>
@@ -324,11 +324,54 @@
   <si>
     <t>Symbol To Turn into Wild</t>
   </si>
+  <si>
+    <t>Win</t>
+  </si>
+  <si>
+    <t>Avg Multiplier</t>
+  </si>
+  <si>
+    <t>Avg. Win</t>
+  </si>
+  <si>
+    <t>Std.dev</t>
+  </si>
+  <si>
+    <t>Avg Total Win</t>
+  </si>
+  <si>
+    <t>WinX</t>
+  </si>
+  <si>
+    <t>Cred. Win</t>
+  </si>
+  <si>
+    <t>Avg multipier</t>
+  </si>
+  <si>
+    <t>RTP Total</t>
+  </si>
+  <si>
+    <t>Weights Total</t>
+  </si>
+  <si>
+    <t>Std. dev sum</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>RTP ~</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="166" formatCode="0.0000%"/>
+    <numFmt numFmtId="172" formatCode="0.00000%"/>
+  </numFmts>
   <fonts count="9">
     <font>
       <sz val="11"/>
@@ -743,13 +786,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -892,6 +936,15 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -919,20 +972,20 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Normal 2" xfId="3" xr:uid="{AC35D676-C183-4380-8910-A0DD10BD5C18}"/>
     <cellStyle name="Normal 4 2" xfId="2" xr:uid="{433B40FB-C0CF-4F64-8A65-686C74055406}"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Процентный" xfId="4" builtinId="5"/>
     <cellStyle name="標準_KS534 P82" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="46">
@@ -1650,7 +1703,7 @@
   <dimension ref="A7:N22"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1827,8 +1880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5091FB6-A1FC-4569-9527-D3BFD417E752}">
   <dimension ref="B2:N170"/>
   <sheetViews>
-    <sheetView topLeftCell="A142" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D163" sqref="D163"/>
+    <sheetView topLeftCell="A109" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H159" sqref="H159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1846,14 +1899,14 @@
   <sheetData>
     <row r="2" spans="2:8" ht="15.75" thickBot="1">
       <c r="B2" s="12"/>
-      <c r="C2" s="61" t="s">
+      <c r="C2" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="63"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="66"/>
     </row>
     <row r="3" spans="2:8">
       <c r="B3" s="12"/>
@@ -4816,15 +4869,15 @@
       <c r="H143" s="50"/>
     </row>
     <row r="145" spans="2:10">
-      <c r="B145" s="68" t="s">
+      <c r="B145" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="C145" s="68"/>
-      <c r="D145" s="68"/>
-      <c r="E145" s="68"/>
-      <c r="F145" s="68"/>
-      <c r="G145" s="68"/>
-      <c r="H145" s="68"/>
+      <c r="C145" s="71"/>
+      <c r="D145" s="71"/>
+      <c r="E145" s="71"/>
+      <c r="F145" s="71"/>
+      <c r="G145" s="71"/>
+      <c r="H145" s="71"/>
     </row>
     <row r="146" spans="2:10">
       <c r="B146" s="19" t="s">
@@ -4935,15 +4988,15 @@
       </c>
     </row>
     <row r="151" spans="2:10">
-      <c r="B151" s="68" t="s">
+      <c r="B151" s="71" t="s">
         <v>65</v>
       </c>
-      <c r="C151" s="68"/>
-      <c r="D151" s="68"/>
-      <c r="E151" s="68"/>
-      <c r="F151" s="68"/>
-      <c r="G151" s="68"/>
-      <c r="H151" s="68"/>
+      <c r="C151" s="71"/>
+      <c r="D151" s="71"/>
+      <c r="E151" s="71"/>
+      <c r="F151" s="71"/>
+      <c r="G151" s="71"/>
+      <c r="H151" s="71"/>
     </row>
     <row r="152" spans="2:10">
       <c r="B152" s="19" t="s">
@@ -5412,8 +5465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="B2:Z198"/>
   <sheetViews>
-    <sheetView topLeftCell="A87" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K88" sqref="K88"/>
+    <sheetView topLeftCell="A103" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -5433,14 +5486,14 @@
   <sheetData>
     <row r="2" spans="2:8" ht="15.75" thickBot="1">
       <c r="B2" s="12"/>
-      <c r="C2" s="61" t="s">
+      <c r="C2" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="63"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="66"/>
     </row>
     <row r="3" spans="2:8">
       <c r="B3" s="12"/>
@@ -5494,7 +5547,7 @@
         <v>61</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E5" s="16" t="s">
         <v>13</v>
@@ -5517,7 +5570,7 @@
         <v>9</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E6" s="16" t="s">
         <v>12</v>
@@ -5632,7 +5685,7 @@
         <v>11</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E11" s="16" t="s">
         <v>12</v>
@@ -5655,7 +5708,7 @@
         <v>9</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E12" s="16" t="s">
         <v>7</v>
@@ -5753,7 +5806,7 @@
         <v>7</v>
       </c>
       <c r="F16" s="16" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G16" s="16" t="s">
         <v>7</v>
@@ -5776,7 +5829,7 @@
         <v>8</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G17" s="16" t="s">
         <v>7</v>
@@ -5799,7 +5852,7 @@
         <v>9</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G18" s="16" t="s">
         <v>7</v>
@@ -5816,7 +5869,7 @@
         <v>7</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E19" s="16" t="s">
         <v>10</v>
@@ -5832,7 +5885,7 @@
       </c>
       <c r="I19" s="21">
         <f>I62</f>
-        <v>1.4006012768370522</v>
+        <v>2.1557797184298213</v>
       </c>
     </row>
     <row r="20" spans="2:9">
@@ -5843,7 +5896,7 @@
         <v>9</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E20" s="16" t="s">
         <v>8</v>
@@ -5893,7 +5946,7 @@
         <v>10</v>
       </c>
       <c r="F22" s="16" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G22" s="16" t="s">
         <v>12</v>
@@ -5971,7 +6024,7 @@
         <v>61</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E26" s="16" t="s">
         <v>12</v>
@@ -6076,7 +6129,7 @@
         <v>9</v>
       </c>
       <c r="D31" s="16" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E31" s="16" t="s">
         <v>61</v>
@@ -6097,7 +6150,7 @@
         <v>13</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E32" s="16" t="s">
         <v>13</v>
@@ -6208,7 +6261,7 @@
         <v>11</v>
       </c>
       <c r="F37" s="16" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G37" s="16" t="s">
         <v>9</v>
@@ -6223,7 +6276,7 @@
         <v>8</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E38" s="16" t="s">
         <v>12</v>
@@ -6244,7 +6297,7 @@
         <v>11</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E39" s="16" t="s">
         <v>8</v>
@@ -6346,7 +6399,7 @@
         <v>40</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D44" s="16" t="s">
         <v>11</v>
@@ -6409,7 +6462,7 @@
         <v>43</v>
       </c>
       <c r="C47" s="16" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D47" s="16" t="s">
         <v>13</v>
@@ -6514,7 +6567,7 @@
         <v>48</v>
       </c>
       <c r="C52" s="16" t="s">
-        <v>61</v>
+        <v>15</v>
       </c>
       <c r="D52" s="16" t="s">
         <v>10</v>
@@ -6649,7 +6702,7 @@
         <v>61</v>
       </c>
       <c r="F58" s="16" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G58" s="16" t="s">
         <v>8</v>
@@ -6664,13 +6717,13 @@
         <v>61</v>
       </c>
       <c r="D59" s="16" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E59" s="16" t="s">
         <v>61</v>
       </c>
       <c r="F59" s="16" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G59" s="16" t="s">
         <v>14</v>
@@ -6703,7 +6756,7 @@
         <v>57</v>
       </c>
       <c r="C61" s="16" t="s">
-        <v>61</v>
+        <v>15</v>
       </c>
       <c r="D61" s="16" t="s">
         <v>61</v>
@@ -6741,7 +6794,7 @@
       <c r="H62" s="32"/>
       <c r="I62" s="21">
         <f>I127</f>
-        <v>1.4006012768370522</v>
+        <v>2.1557797184298213</v>
       </c>
     </row>
     <row r="63" spans="2:9">
@@ -6791,7 +6844,7 @@
         <v>61</v>
       </c>
       <c r="C65" s="16" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D65" s="16" t="s">
         <v>61</v>
@@ -6812,7 +6865,7 @@
         <v>62</v>
       </c>
       <c r="C66" s="16" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="D66" s="16" t="s">
         <v>15</v>
@@ -6821,7 +6874,7 @@
         <v>15</v>
       </c>
       <c r="F66" s="16" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="G66" s="16" t="s">
         <v>15</v>
@@ -6836,13 +6889,13 @@
         <v>14</v>
       </c>
       <c r="D67" s="16" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E67" s="16" t="s">
         <v>11</v>
       </c>
       <c r="F67" s="16" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G67" s="16" t="s">
         <v>12</v>
@@ -6860,10 +6913,10 @@
         <v>14</v>
       </c>
       <c r="E68" s="16" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F68" s="16" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G68" s="16" t="s">
         <v>5</v>
@@ -6881,7 +6934,7 @@
         <v>61</v>
       </c>
       <c r="E69" s="16" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F69" s="16" t="s">
         <v>61</v>
@@ -6902,7 +6955,7 @@
         <v>7</v>
       </c>
       <c r="E70" s="16" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F70" s="16" t="s">
         <v>7</v>
@@ -6917,7 +6970,7 @@
         <v>67</v>
       </c>
       <c r="C71" s="16" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D71" s="16" t="s">
         <v>11</v>
@@ -6926,7 +6979,7 @@
         <v>8</v>
       </c>
       <c r="F71" s="16" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G71" s="16" t="s">
         <v>11</v>
@@ -6938,7 +6991,7 @@
         <v>68</v>
       </c>
       <c r="C72" s="16" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D72" s="16" t="s">
         <v>5</v>
@@ -6968,7 +7021,7 @@
         <v>12</v>
       </c>
       <c r="F73" s="16" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G73" s="16" t="s">
         <v>10</v>
@@ -7031,7 +7084,7 @@
         <v>5</v>
       </c>
       <c r="F76" s="16" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G76" s="16" t="s">
         <v>5</v>
@@ -7298,7 +7351,7 @@
         <v>43</v>
       </c>
       <c r="D89" s="16" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E89" s="16" t="s">
         <v>7</v>
@@ -7487,7 +7540,7 @@
         <v>7</v>
       </c>
       <c r="D98" s="16" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E98" s="16" t="s">
         <v>9</v>
@@ -7529,7 +7582,7 @@
         <v>7</v>
       </c>
       <c r="D100" s="16" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="E100" s="16" t="s">
         <v>15</v>
@@ -7543,7 +7596,7 @@
       <c r="H100" s="32"/>
       <c r="I100" s="21">
         <f>I127</f>
-        <v>1.4006012768370522</v>
+        <v>2.1557797184298213</v>
       </c>
     </row>
     <row r="101" spans="2:9">
@@ -7596,10 +7649,10 @@
         <v>9</v>
       </c>
       <c r="D103" s="16" t="s">
-        <v>10</v>
+        <v>61</v>
       </c>
       <c r="E103" s="16" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="F103" s="16" t="s">
         <v>10</v>
@@ -7617,7 +7670,7 @@
         <v>10</v>
       </c>
       <c r="D104" s="16" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E104" s="16" t="s">
         <v>15</v>
@@ -7704,7 +7757,7 @@
         <v>12</v>
       </c>
       <c r="E108" s="16" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F108" s="16" t="s">
         <v>12</v>
@@ -7725,7 +7778,7 @@
         <v>14</v>
       </c>
       <c r="E109" s="16" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F109" s="16" t="s">
         <v>10</v>
@@ -7746,7 +7799,7 @@
         <v>9</v>
       </c>
       <c r="E110" s="16" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="F110" s="16" t="s">
         <v>9</v>
@@ -7767,7 +7820,7 @@
         <v>9</v>
       </c>
       <c r="E111" s="16" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="F111" s="16" t="s">
         <v>9</v>
@@ -7806,7 +7859,7 @@
         <v>10</v>
       </c>
       <c r="D113" s="16" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E113" s="16" t="s">
         <v>8</v>
@@ -7827,10 +7880,10 @@
         <v>10</v>
       </c>
       <c r="D114" s="16" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E114" s="16" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F114" s="16" t="s">
         <v>61</v>
@@ -8097,7 +8150,7 @@
         <v>123</v>
       </c>
       <c r="C127" s="16" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D127" s="16" t="s">
         <v>61</v>
@@ -8114,7 +8167,7 @@
       <c r="H127" s="32"/>
       <c r="I127" s="21">
         <f>J147</f>
-        <v>1.4006012768370522</v>
+        <v>2.1557797184298213</v>
       </c>
     </row>
     <row r="128" spans="2:9">
@@ -8122,7 +8175,7 @@
         <v>124</v>
       </c>
       <c r="C128" s="16" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D128" s="16" t="s">
         <v>10</v>
@@ -8143,7 +8196,7 @@
         <v>125</v>
       </c>
       <c r="C129" s="16" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D129" s="16" t="s">
         <v>7</v>
@@ -8167,7 +8220,7 @@
         <v>8</v>
       </c>
       <c r="D130" s="16" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E130" s="16" t="s">
         <v>13</v>
@@ -8227,7 +8280,7 @@
         <v>129</v>
       </c>
       <c r="C133" s="16" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="D133" s="49" t="s">
         <v>11</v>
@@ -8248,7 +8301,7 @@
         <v>130</v>
       </c>
       <c r="C134" s="16" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="D134" s="49" t="s">
         <v>11</v>
@@ -8417,15 +8470,15 @@
       <c r="H143" s="50"/>
     </row>
     <row r="145" spans="2:10">
-      <c r="B145" s="68" t="s">
+      <c r="B145" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="C145" s="68"/>
-      <c r="D145" s="68"/>
-      <c r="E145" s="68"/>
-      <c r="F145" s="68"/>
-      <c r="G145" s="68"/>
-      <c r="H145" s="68"/>
+      <c r="C145" s="71"/>
+      <c r="D145" s="71"/>
+      <c r="E145" s="71"/>
+      <c r="F145" s="71"/>
+      <c r="G145" s="71"/>
+      <c r="H145" s="71"/>
     </row>
     <row r="146" spans="2:10">
       <c r="B146" s="19" t="s">
@@ -8483,7 +8536,7 @@
       </c>
       <c r="J147" s="13">
         <f>Q181</f>
-        <v>1.4006012768370522</v>
+        <v>2.1557797184298213</v>
       </c>
     </row>
     <row r="148" spans="2:10">
@@ -8492,19 +8545,19 @@
       </c>
       <c r="C148" s="53">
         <f t="shared" ref="C148:G160" si="1">COUNTIF(C$4:C$142,$B148)</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D148" s="51">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E148" s="53">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F148" s="51">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G148" s="18">
         <f t="shared" si="0"/>
@@ -8522,19 +8575,19 @@
       </c>
       <c r="C149" s="51">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D149" s="53">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E149" s="51">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F149" s="53">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G149" s="18">
         <f t="shared" si="0"/>
@@ -8552,11 +8605,11 @@
       </c>
       <c r="C150" s="53">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D150" s="51">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E150" s="53">
         <f t="shared" si="1"/>
@@ -8582,19 +8635,19 @@
       </c>
       <c r="C151" s="51">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D151" s="53">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E151" s="51">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F151" s="53">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G151" s="18">
         <f t="shared" si="0"/>
@@ -8612,19 +8665,19 @@
       </c>
       <c r="C152" s="53">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D152" s="51">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E152" s="53">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F152" s="51">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G152" s="18">
         <f t="shared" si="0"/>
@@ -8642,19 +8695,19 @@
       </c>
       <c r="C153" s="53">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D153" s="51">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E153" s="53">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F153" s="51">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G153" s="18">
         <f t="shared" si="0"/>
@@ -8672,11 +8725,11 @@
       </c>
       <c r="C154" s="51">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D154" s="53">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E154" s="51">
         <f t="shared" si="1"/>
@@ -8684,7 +8737,7 @@
       </c>
       <c r="F154" s="53">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G154" s="18">
         <f t="shared" si="0"/>
@@ -8702,11 +8755,11 @@
       </c>
       <c r="C155" s="53">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D155" s="51">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E155" s="53">
         <f t="shared" si="1"/>
@@ -8732,19 +8785,19 @@
       </c>
       <c r="C156" s="51">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D156" s="53">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E156" s="51">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F156" s="53">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G156" s="18">
         <f t="shared" si="0"/>
@@ -8766,15 +8819,15 @@
       </c>
       <c r="D157" s="51">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E157" s="53">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F157" s="51">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G157" s="18">
         <f t="shared" si="0"/>
@@ -8901,33 +8954,33 @@
       </c>
     </row>
     <row r="165" spans="2:26">
-      <c r="B165" s="64" t="s">
+      <c r="B165" s="67" t="s">
         <v>45</v>
       </c>
-      <c r="C165" s="64"/>
-      <c r="D165" s="64"/>
-      <c r="E165" s="64"/>
-      <c r="F165" s="64"/>
-      <c r="G165" s="64"/>
-      <c r="H165" s="64"/>
-      <c r="K165" s="64" t="s">
+      <c r="C165" s="67"/>
+      <c r="D165" s="67"/>
+      <c r="E165" s="67"/>
+      <c r="F165" s="67"/>
+      <c r="G165" s="67"/>
+      <c r="H165" s="67"/>
+      <c r="K165" s="67" t="s">
         <v>47</v>
       </c>
-      <c r="L165" s="64"/>
-      <c r="M165" s="64"/>
-      <c r="N165" s="64"/>
-      <c r="O165" s="64"/>
-      <c r="P165" s="64"/>
-      <c r="Q165" s="64"/>
-      <c r="T165" s="64" t="s">
+      <c r="L165" s="67"/>
+      <c r="M165" s="67"/>
+      <c r="N165" s="67"/>
+      <c r="O165" s="67"/>
+      <c r="P165" s="67"/>
+      <c r="Q165" s="67"/>
+      <c r="T165" s="67" t="s">
         <v>50</v>
       </c>
-      <c r="U165" s="64"/>
-      <c r="V165" s="64"/>
-      <c r="W165" s="64"/>
-      <c r="X165" s="64"/>
-      <c r="Y165" s="64"/>
-      <c r="Z165" s="64"/>
+      <c r="U165" s="67"/>
+      <c r="V165" s="67"/>
+      <c r="W165" s="67"/>
+      <c r="X165" s="67"/>
+      <c r="Y165" s="67"/>
+      <c r="Z165" s="67"/>
     </row>
     <row r="166" spans="2:26">
       <c r="B166" s="18" t="s">
@@ -9034,7 +9087,7 @@
       </c>
       <c r="N167" s="18">
         <f>C167*D167*E167*(F173+F174+F175+F176+F177)*E186</f>
-        <v>4.3250423815536951E-4</v>
+        <v>2.9863387872632659E-4</v>
       </c>
       <c r="O167" s="18">
         <f>C167*D167*E167*F167*(G178+G180+SUM(G173:G177)+G179*SUM(H173:H177))*F186</f>
@@ -9061,19 +9114,19 @@
       </c>
       <c r="C168" s="18">
         <f t="shared" ref="C168:C180" si="4">C148/C$161</f>
-        <v>0.10071942446043165</v>
+        <v>0.11510791366906475</v>
       </c>
       <c r="D168" s="18">
         <f t="shared" si="3"/>
-        <v>9.6296296296296297E-2</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="E168" s="18">
         <f t="shared" si="3"/>
-        <v>9.420289855072464E-2</v>
+        <v>0.11594202898550725</v>
       </c>
       <c r="F168" s="18">
         <f t="shared" si="3"/>
-        <v>0.11851851851851852</v>
+        <v>0.14814814814814814</v>
       </c>
       <c r="G168" s="18">
         <f t="shared" si="3"/>
@@ -9095,15 +9148,15 @@
       </c>
       <c r="N168" s="18">
         <f>((1-$H168)*($C168+C$167)*($D168+D$167)*($E168+E$167)*(1-F$167-$F168)+H168*($C168+C$167+C$179)*($D168+D$167+D$179)*($E168+E$167+E$179)*(1-F$167-$F168-F$179))*$E187-(1-F$167-F168-$H168*F$179)*$E187*PRODUCT(C$167:E$167)</f>
-        <v>9.3462089495044309E-2</v>
+        <v>0.12949685718887238</v>
       </c>
       <c r="O168" s="18">
         <f>((1-$H168)*($C168+C$167)*($D168+D$167)*($E168+E$167)*(F$167+$F168)*(1-G$167-G168)+H168*($C168+C$167+C$179)*($D168+D$167+D$179)*($E168+E$167+E$179)*(F$167+$F168+F$179)*(1-G$167-G168-G$179))*F187-(1-G$167-G168-$H168*G$179)*$F187*PRODUCT(C$167:F$167)</f>
-        <v>0.14902131789415304</v>
+        <v>0.2529095524042127</v>
       </c>
       <c r="P168" s="18">
         <f>((1-$H168)*($C168+C$167)*($D168+D$167)*($E168+E$167)*(F$167+$F168)*(G$167+G168)+H168*($C168+C$167+C$179)*($D168+D$167+D$179)*($E168+E$167+E$179)*(F$167+$F168+F$179)*(+G$167+G168+G$179))*G187-PRODUCT(C$167:G$167)*G187</f>
-        <v>0.12300373597548518</v>
+        <v>0.20445639710420457</v>
       </c>
       <c r="Q168" s="18"/>
       <c r="T168" s="18" t="s">
@@ -9124,19 +9177,19 @@
       </c>
       <c r="C169" s="18">
         <f t="shared" si="4"/>
-        <v>0.1079136690647482</v>
+        <v>0.1223021582733813</v>
       </c>
       <c r="D169" s="18">
         <f t="shared" si="3"/>
-        <v>9.6296296296296297E-2</v>
+        <v>0.1037037037037037</v>
       </c>
       <c r="E169" s="18">
         <f t="shared" si="3"/>
-        <v>0.10144927536231885</v>
+        <v>0.11594202898550725</v>
       </c>
       <c r="F169" s="18">
         <f t="shared" si="3"/>
-        <v>0.11851851851851852</v>
+        <v>0.15555555555555556</v>
       </c>
       <c r="G169" s="18">
         <f t="shared" si="3"/>
@@ -9157,15 +9210,15 @@
       </c>
       <c r="N169" s="18">
         <f t="shared" ref="N169:N177" si="5">((1-$H169)*($C169+C$167)*($D169+D$167)*($E169+E$167)*(1-F$167-$F169)+H169*($C169+C$167+C$179)*($D169+D$167+D$179)*($E169+E$167+E$179)*(1-F$167-$F169-F$179))*$E188-(1-F$167-F169-$H169*F$179)*$E188*PRODUCT(C$167:E$167)</f>
-        <v>0.10381124757188553</v>
+        <v>0.12761348497533631</v>
       </c>
       <c r="O169" s="18">
         <f t="shared" ref="O169:O177" si="6">((1-$H169)*($C169+C$167)*($D169+D$167)*($E169+E$167)*(F$167+$F169)*(1-G$167-G169)+H169*($C169+C$167+C$179)*($D169+D$167+D$179)*($E169+E$167+E$179)*(F$167+$F169+F$179)*(1-G$167-G169-G$179))*F188-(1-G$167-G169-$H169*G$179)*$F188*PRODUCT(C$167:F$167)</f>
-        <v>9.8186658963211965E-2</v>
+        <v>0.2075680352103394</v>
       </c>
       <c r="P169" s="18">
         <f t="shared" ref="P169:P177" si="7">((1-$H169)*($C169+C$167)*($D169+D$167)*($E169+E$167)*(F$167+$F169)*(G$167+G169)+H169*($C169+C$167+C$179)*($D169+D$167+D$179)*($E169+E$167+E$179)*(F$167+$F169+F$179)*(+G$167+G169+G$179))*G188-PRODUCT(C$167:G$167)*G188</f>
-        <v>8.5613656595094206E-2</v>
+        <v>0.13351307932252171</v>
       </c>
       <c r="Q169" s="18"/>
       <c r="T169" s="18" t="s">
@@ -9184,11 +9237,11 @@
       </c>
       <c r="C170" s="18">
         <f t="shared" si="4"/>
-        <v>0.11510791366906475</v>
+        <v>0.1079136690647482</v>
       </c>
       <c r="D170" s="18">
         <f t="shared" si="3"/>
-        <v>0.1037037037037037</v>
+        <v>0.12592592592592591</v>
       </c>
       <c r="E170" s="18">
         <f t="shared" si="3"/>
@@ -9217,15 +9270,15 @@
       </c>
       <c r="N170" s="18">
         <f t="shared" si="5"/>
-        <v>6.5124492241008761E-2</v>
+        <v>7.207356024813566E-2</v>
       </c>
       <c r="O170" s="18">
         <f t="shared" si="6"/>
-        <v>7.0393331049276461E-2</v>
+        <v>0.11660982632579057</v>
       </c>
       <c r="P170" s="18">
         <f t="shared" si="7"/>
-        <v>7.2142550814745701E-2</v>
+        <v>7.9427489885463193E-2</v>
       </c>
       <c r="Q170" s="18"/>
       <c r="T170" s="18" t="s">
@@ -9244,19 +9297,19 @@
       </c>
       <c r="C171" s="18">
         <f t="shared" si="4"/>
-        <v>0.1223021582733813</v>
+        <v>0.12949640287769784</v>
       </c>
       <c r="D171" s="18">
         <f t="shared" si="3"/>
-        <v>0.1037037037037037</v>
+        <v>0.11851851851851852</v>
       </c>
       <c r="E171" s="18">
         <f t="shared" si="3"/>
-        <v>9.420289855072464E-2</v>
+        <v>0.10144927536231885</v>
       </c>
       <c r="F171" s="18">
         <f t="shared" si="3"/>
-        <v>0.12592592592592591</v>
+        <v>0.14814814814814814</v>
       </c>
       <c r="G171" s="18">
         <f t="shared" si="3"/>
@@ -9277,15 +9330,15 @@
       </c>
       <c r="N171" s="18">
         <f t="shared" si="5"/>
-        <v>7.4100050577453475E-2</v>
+        <v>8.7676241501825541E-2</v>
       </c>
       <c r="O171" s="18">
         <f t="shared" si="6"/>
-        <v>8.2431728928916939E-2</v>
+        <v>0.16956441700191158</v>
       </c>
       <c r="P171" s="18">
         <f t="shared" si="7"/>
-        <v>6.664872241454653E-2</v>
+        <v>9.0391789004314674E-2</v>
       </c>
       <c r="Q171" s="18"/>
       <c r="T171" s="18" t="s">
@@ -9304,19 +9357,19 @@
       </c>
       <c r="C172" s="18">
         <f t="shared" si="4"/>
-        <v>0.15827338129496402</v>
+        <v>0.16546762589928057</v>
       </c>
       <c r="D172" s="18">
         <f t="shared" si="3"/>
-        <v>0.1037037037037037</v>
+        <v>0.11851851851851852</v>
       </c>
       <c r="E172" s="18">
         <f t="shared" si="3"/>
-        <v>0.10144927536231885</v>
+        <v>0.12318840579710146</v>
       </c>
       <c r="F172" s="18">
         <f>F152/F$161</f>
-        <v>0.12592592592592591</v>
+        <v>0.13333333333333333</v>
       </c>
       <c r="G172" s="18">
         <f t="shared" si="3"/>
@@ -9337,15 +9390,15 @@
       </c>
       <c r="N172" s="18">
         <f t="shared" si="5"/>
-        <v>7.9583051376460628E-2</v>
+        <v>0.12476923453185923</v>
       </c>
       <c r="O172" s="18">
         <f t="shared" si="6"/>
-        <v>7.4954682794392657E-2</v>
+        <v>0.20517937543606915</v>
       </c>
       <c r="P172" s="18">
         <f t="shared" si="7"/>
-        <v>7.0562253148965498E-2</v>
+        <v>9.5677035127029741E-2</v>
       </c>
       <c r="Q172" s="18"/>
       <c r="T172" s="18" t="s">
@@ -9364,19 +9417,19 @@
       </c>
       <c r="C173" s="18">
         <f t="shared" si="4"/>
-        <v>5.0359712230215826E-2</v>
+        <v>3.5971223021582732E-2</v>
       </c>
       <c r="D173" s="18">
         <f t="shared" si="3"/>
-        <v>8.8888888888888892E-2</v>
+        <v>7.407407407407407E-2</v>
       </c>
       <c r="E173" s="18">
         <f t="shared" si="3"/>
-        <v>8.6956521739130432E-2</v>
+        <v>5.0724637681159424E-2</v>
       </c>
       <c r="F173" s="18">
         <f t="shared" si="3"/>
-        <v>8.1481481481481488E-2</v>
+        <v>5.185185185185185E-2</v>
       </c>
       <c r="G173" s="18">
         <f t="shared" si="3"/>
@@ -9397,15 +9450,15 @@
       </c>
       <c r="N173" s="18">
         <f t="shared" si="5"/>
-        <v>9.5170720169783143E-3</v>
+        <v>4.9287579924167562E-3</v>
       </c>
       <c r="O173" s="18">
         <f t="shared" si="6"/>
-        <v>8.362741853277544E-3</v>
+        <v>3.2144401138048304E-3</v>
       </c>
       <c r="P173" s="18">
         <f t="shared" si="7"/>
-        <v>1.8372455248890618E-3</v>
+        <v>7.5628186490882927E-4</v>
       </c>
       <c r="Q173" s="18"/>
       <c r="T173" s="18" t="s">
@@ -9424,11 +9477,11 @@
       </c>
       <c r="C174" s="18">
         <f t="shared" si="4"/>
-        <v>4.3165467625899283E-2</v>
+        <v>2.8776978417266189E-2</v>
       </c>
       <c r="D174" s="18">
         <f t="shared" si="3"/>
-        <v>9.6296296296296297E-2</v>
+        <v>8.8888888888888892E-2</v>
       </c>
       <c r="E174" s="18">
         <f t="shared" si="3"/>
@@ -9436,7 +9489,7 @@
       </c>
       <c r="F174" s="18">
         <f t="shared" si="3"/>
-        <v>8.1481481481481488E-2</v>
+        <v>4.4444444444444446E-2</v>
       </c>
       <c r="G174" s="18">
         <f t="shared" si="3"/>
@@ -9457,15 +9510,15 @@
       </c>
       <c r="N174" s="18">
         <f t="shared" si="5"/>
-        <v>1.0813605438468205E-2</v>
+        <v>8.4221719905500265E-3</v>
       </c>
       <c r="O174" s="18">
         <f t="shared" si="6"/>
-        <v>9.3964837825007714E-3</v>
+        <v>4.8057537120596901E-3</v>
       </c>
       <c r="P174" s="18">
         <f t="shared" si="7"/>
-        <v>2.2278501355176834E-3</v>
+        <v>1.194350672613707E-3</v>
       </c>
       <c r="Q174" s="18"/>
       <c r="T174" s="18" t="s">
@@ -9484,11 +9537,11 @@
       </c>
       <c r="C175" s="18">
         <f t="shared" si="4"/>
-        <v>7.1942446043165464E-2</v>
+        <v>7.9136690647482008E-2</v>
       </c>
       <c r="D175" s="18">
         <f t="shared" si="3"/>
-        <v>7.407407407407407E-2</v>
+        <v>5.185185185185185E-2</v>
       </c>
       <c r="E175" s="18">
         <f t="shared" si="3"/>
@@ -9517,15 +9570,15 @@
       </c>
       <c r="N175" s="18">
         <f t="shared" si="5"/>
-        <v>9.9031826710439721E-3</v>
+        <v>8.2980508123996644E-3</v>
       </c>
       <c r="O175" s="18">
         <f t="shared" si="6"/>
-        <v>3.0360890776748792E-3</v>
+        <v>2.5717310936057692E-3</v>
       </c>
       <c r="P175" s="18">
         <f t="shared" si="7"/>
-        <v>6.6710684173620037E-4</v>
+        <v>5.735981700041036E-4</v>
       </c>
       <c r="Q175" s="18"/>
       <c r="T175" s="18" t="s">
@@ -9544,19 +9597,19 @@
       </c>
       <c r="C176" s="18">
         <f t="shared" si="4"/>
-        <v>6.4748201438848921E-2</v>
+        <v>5.0359712230215826E-2</v>
       </c>
       <c r="D176" s="18">
         <f>D156/D$161</f>
-        <v>9.6296296296296297E-2</v>
+        <v>8.1481481481481488E-2</v>
       </c>
       <c r="E176" s="18">
         <f t="shared" si="3"/>
-        <v>5.7971014492753624E-2</v>
+        <v>5.0724637681159424E-2</v>
       </c>
       <c r="F176" s="18">
         <f t="shared" si="3"/>
-        <v>6.6666666666666666E-2</v>
+        <v>4.4444444444444446E-2</v>
       </c>
       <c r="G176" s="18">
         <f t="shared" si="3"/>
@@ -9577,15 +9630,15 @@
       </c>
       <c r="N176" s="18">
         <f t="shared" si="5"/>
-        <v>9.2989891921306609E-3</v>
+        <v>6.5327221030791185E-3</v>
       </c>
       <c r="O176" s="18">
         <f t="shared" si="6"/>
-        <v>4.6228475630449928E-3</v>
+        <v>2.5045529217488783E-3</v>
       </c>
       <c r="P176" s="18">
         <f t="shared" si="7"/>
-        <v>1.3878185666515996E-3</v>
+        <v>7.8390391008658071E-4</v>
       </c>
       <c r="Q176" s="18"/>
       <c r="T176" s="18" t="s">
@@ -9608,15 +9661,15 @@
       </c>
       <c r="D177" s="18">
         <f>D157/D$161</f>
-        <v>6.6666666666666666E-2</v>
+        <v>5.185185185185185E-2</v>
       </c>
       <c r="E177" s="18">
         <f t="shared" si="3"/>
-        <v>0.10144927536231885</v>
+        <v>7.9710144927536225E-2</v>
       </c>
       <c r="F177" s="18">
         <f t="shared" si="3"/>
-        <v>5.185185185185185E-2</v>
+        <v>4.4444444444444446E-2</v>
       </c>
       <c r="G177" s="18">
         <f t="shared" si="3"/>
@@ -9637,15 +9690,15 @@
       </c>
       <c r="N177" s="18">
         <f t="shared" si="5"/>
-        <v>1.3031105011899462E-2</v>
+        <v>9.3037998426787703E-3</v>
       </c>
       <c r="O177" s="18">
         <f t="shared" si="6"/>
-        <v>5.336647992611649E-3</v>
+        <v>3.4949562311541813E-3</v>
       </c>
       <c r="P177" s="18">
         <f t="shared" si="7"/>
-        <v>1.5885311278954742E-3</v>
+        <v>1.0677518901620129E-3</v>
       </c>
       <c r="Q177" s="18"/>
       <c r="T177" s="18" t="s">
@@ -9824,7 +9877,7 @@
       </c>
       <c r="D181" s="25">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0.99999999999999989</v>
       </c>
       <c r="E181" s="25">
         <f t="shared" si="9"/>
@@ -9832,7 +9885,7 @@
       </c>
       <c r="F181" s="25">
         <f t="shared" si="9"/>
-        <v>0.99999999999999989</v>
+        <v>0.99999999999999978</v>
       </c>
       <c r="G181" s="26">
         <f t="shared" si="9"/>
@@ -9852,7 +9905,7 @@
       <c r="P181" s="26"/>
       <c r="Q181" s="26">
         <f>SUM(L167:P180)</f>
-        <v>1.4006012768370522</v>
+        <v>2.1557797184298213</v>
       </c>
       <c r="T181" s="24" t="s">
         <v>41</v>
@@ -9868,14 +9921,14 @@
       <c r="X183" s="41"/>
     </row>
     <row r="184" spans="2:26">
-      <c r="B184" s="65" t="s">
+      <c r="B184" s="68" t="s">
         <v>46</v>
       </c>
-      <c r="C184" s="66"/>
-      <c r="D184" s="66"/>
-      <c r="E184" s="66"/>
-      <c r="F184" s="66"/>
-      <c r="G184" s="67"/>
+      <c r="C184" s="69"/>
+      <c r="D184" s="69"/>
+      <c r="E184" s="69"/>
+      <c r="F184" s="69"/>
+      <c r="G184" s="70"/>
       <c r="K184" s="20" t="s">
         <v>5</v>
       </c>
@@ -9896,7 +9949,7 @@
       </c>
       <c r="R184" s="13">
         <f>((1-H$168)*IF(K184="Wild",C$167,C$168)*IF(L184="Wild",D$167,D$168)*IF(M184="Wild",E$167,E$168)*(1-F$167-F$168)+H$168*IF(K184="Wild",C$167,C$168+C$179)*IF(L184="Wild",D$167,D$168+D$179)*IF(M184="Wild",E$167,E$168+E$179)*(1-F$167-F$168-F$179))*E$187</f>
-        <v>2.0593925541578673E-3</v>
+        <v>2.4169354485153003E-3</v>
       </c>
       <c r="X184" s="41"/>
     </row>
@@ -9939,7 +9992,7 @@
       </c>
       <c r="R185" s="13">
         <f t="shared" ref="R185:R191" si="10">((1-H$168)*IF(K185="Wild",C$167,C$168)*IF(L185="Wild",D$167,D$168)*IF(M185="Wild",E$167,E$168)*(1-F$167-F$168)+H$168*IF(K185="Wild",C$167,C$168+C$179)*IF(L185="Wild",D$167,D$168+D$179)*IF(M185="Wild",E$167,E$168+E$179)*(1-F$167-F$168-F$179))*E$187</f>
-        <v>2.7238478864220041E-3</v>
+        <v>3.0105687165716891E-3</v>
       </c>
     </row>
     <row r="186" spans="2:26">
@@ -9986,7 +10039,7 @@
       </c>
       <c r="R186" s="13">
         <f t="shared" si="10"/>
-        <v>2.9435325788183821E-3</v>
+        <v>3.2225805980204002E-3</v>
       </c>
     </row>
     <row r="187" spans="2:26">
@@ -10033,7 +10086,7 @@
       </c>
       <c r="R187" s="13">
         <f t="shared" si="10"/>
-        <v>1.3885095600910783E-2</v>
+        <v>1.7300169526214777E-2</v>
       </c>
     </row>
     <row r="188" spans="2:26">
@@ -10054,7 +10107,7 @@
       </c>
       <c r="F188" s="35">
         <f>Paytable!F6</f>
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="G188" s="35">
         <f>Paytable!G6</f>
@@ -10080,7 +10133,7 @@
       </c>
       <c r="R188" s="13">
         <f t="shared" si="10"/>
-        <v>1.0534870389186424E-2</v>
+        <v>1.3907979423035411E-2</v>
       </c>
     </row>
     <row r="189" spans="2:26">
@@ -10101,7 +10154,7 @@
       </c>
       <c r="F189" s="35">
         <f>Paytable!F7</f>
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="G189" s="35">
         <f>Paytable!G7</f>
@@ -10127,7 +10180,7 @@
       </c>
       <c r="R189" s="13">
         <f t="shared" si="10"/>
-        <v>9.7328597290775882E-3</v>
+        <v>1.2975127144661081E-2</v>
       </c>
     </row>
     <row r="190" spans="2:26">
@@ -10148,7 +10201,7 @@
       </c>
       <c r="F190" s="35">
         <f>Paytable!F8</f>
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="G190" s="35">
         <f>Paytable!G8</f>
@@ -10174,11 +10227,11 @@
       </c>
       <c r="R190" s="13">
         <f t="shared" si="10"/>
-        <v>5.1582490756471262E-2</v>
+        <v>7.6663496331853709E-2</v>
       </c>
       <c r="S190" s="13">
         <f>SUM(R184:R190)</f>
-        <v>9.3462089495044309E-2</v>
+        <v>0.12949685718887238</v>
       </c>
     </row>
     <row r="191" spans="2:26">
@@ -10195,11 +10248,11 @@
       </c>
       <c r="E191" s="35">
         <f>Paytable!E9</f>
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F191" s="35">
         <f>Paytable!F9</f>
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="G191" s="35">
         <f>Paytable!G9</f>
@@ -10216,7 +10269,7 @@
       </c>
       <c r="R191" s="13">
         <f t="shared" si="10"/>
-        <v>5.9302751982367877E-4</v>
+        <v>5.7243207991151837E-4</v>
       </c>
     </row>
     <row r="192" spans="2:26">
@@ -10245,7 +10298,7 @@
       </c>
       <c r="R192" s="13">
         <f>(1-F167-F168-F179*0.1)*50*C167*D167*E167</f>
-        <v>5.9366355546802501E-4</v>
+        <v>5.730681155558645E-4</v>
       </c>
     </row>
     <row r="193" spans="2:7">
@@ -10382,12 +10435,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B184:G184"/>
     <mergeCell ref="C2:H2"/>
     <mergeCell ref="B145:H145"/>
     <mergeCell ref="B165:H165"/>
     <mergeCell ref="K165:Q165"/>
     <mergeCell ref="T165:Z165"/>
-    <mergeCell ref="B184:G184"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:Z1048576">
     <cfRule type="containsText" dxfId="13" priority="1" operator="containsText" text="Inner">
@@ -10445,8 +10498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93C67964-F486-43D8-9E65-63372F03F592}">
   <dimension ref="B2:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10460,7 +10513,7 @@
         <v>88</v>
       </c>
       <c r="C2">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="2:3">
@@ -10530,12 +10583,1247 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A2:N51"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:14">
+      <c r="C2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="J2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K2" t="s">
+        <v>93</v>
+      </c>
+      <c r="L2" t="s">
+        <v>95</v>
+      </c>
+      <c r="M2" t="s">
+        <v>60</v>
+      </c>
+      <c r="N2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>450</v>
+      </c>
+      <c r="F3">
+        <v>150</v>
+      </c>
+      <c r="G3">
+        <v>450</v>
+      </c>
+      <c r="J3">
+        <f>C3*D3/D$10</f>
+        <v>0.15</v>
+      </c>
+      <c r="K3">
+        <f>F3*G3/G$10/70</f>
+        <v>0.32142857142857145</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>500</v>
+      </c>
+      <c r="F4">
+        <v>250</v>
+      </c>
+      <c r="G4">
+        <v>500</v>
+      </c>
+      <c r="J4">
+        <f>C4*D4/D$10</f>
+        <v>0.5</v>
+      </c>
+      <c r="K4">
+        <f>F4*G4/G$10/70</f>
+        <v>0.59523809523809523</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>600</v>
+      </c>
+      <c r="F5">
+        <v>500</v>
+      </c>
+      <c r="G5">
+        <v>600</v>
+      </c>
+      <c r="J5">
+        <f>C5*D5/D$10</f>
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <f>F5*G5/G$10/70</f>
+        <v>1.4285714285714286</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>750</v>
+      </c>
+      <c r="F6">
+        <v>750</v>
+      </c>
+      <c r="G6">
+        <v>750</v>
+      </c>
+      <c r="J6">
+        <f>C6*D6/D$10</f>
+        <v>1.75</v>
+      </c>
+      <c r="K6">
+        <f>F6*G6/G$10/70</f>
+        <v>2.6785714285714284</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="C7">
+        <v>10</v>
+      </c>
+      <c r="D7">
+        <v>500</v>
+      </c>
+      <c r="F7">
+        <v>1000</v>
+      </c>
+      <c r="G7">
+        <v>500</v>
+      </c>
+      <c r="J7">
+        <f>C7*D7/D$10</f>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="K7">
+        <f>F7*G7/G$10/70</f>
+        <v>2.3809523809523809</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="C8">
+        <v>20</v>
+      </c>
+      <c r="D8">
+        <v>200</v>
+      </c>
+      <c r="F8">
+        <v>1500</v>
+      </c>
+      <c r="G8">
+        <v>200</v>
+      </c>
+      <c r="J8">
+        <f>C8*D8/D$10</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="K8">
+        <f>F8*G8/G$10/70</f>
+        <v>1.4285714285714286</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="J9">
+        <f>SUM(J3:J8)</f>
+        <v>6.3999999999999995</v>
+      </c>
+      <c r="K9">
+        <f>SUM(K3:K8)</f>
+        <v>8.8333333333333339</v>
+      </c>
+      <c r="L9">
+        <f>J9*K9</f>
+        <v>56.533333333333331</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="C10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10">
+        <f>SUM(D3:D8)</f>
+        <v>3000</v>
+      </c>
+      <c r="F10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10">
+        <f>SUM(G3:G8)</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" t="s">
+        <v>97</v>
+      </c>
+      <c r="B12" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12" t="s">
+        <v>91</v>
+      </c>
+      <c r="D12" t="s">
+        <v>96</v>
+      </c>
+      <c r="E12" t="s">
+        <v>78</v>
+      </c>
+      <c r="F12" t="s">
+        <v>60</v>
+      </c>
+      <c r="H12" t="s">
+        <v>98</v>
+      </c>
+      <c r="I12" t="s">
+        <v>102</v>
+      </c>
+      <c r="J12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13">
+        <v>150</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <f>A13*B13</f>
+        <v>150</v>
+      </c>
+      <c r="D13">
+        <f>C13/70</f>
+        <v>2.1428571428571428</v>
+      </c>
+      <c r="E13">
+        <v>750</v>
+      </c>
+      <c r="F13" s="74">
+        <f>E13*D13/E$50</f>
+        <v>7.8975078975078977E-3</v>
+      </c>
+      <c r="I13">
+        <f>POWER(D13 - 0.96,2)/600*E13/E$50</f>
+        <v>8.5942937371508791E-6</v>
+      </c>
+      <c r="J13">
+        <f>SQRT(SUM(I13:I48))</f>
+        <v>2.6721853465781709</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14">
+        <v>250</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <f>A14*B14</f>
+        <v>250</v>
+      </c>
+      <c r="D14">
+        <f>C14/70</f>
+        <v>3.5714285714285716</v>
+      </c>
+      <c r="E14">
+        <v>750</v>
+      </c>
+      <c r="F14" s="74">
+        <f t="shared" ref="F14:F48" si="0">E14*D14/E$50</f>
+        <v>1.3162513162513163E-2</v>
+      </c>
+      <c r="I14">
+        <f t="shared" ref="I14:I48" si="1">POWER(D14 - 0.96,2)/600*E14/E$50</f>
+        <v>4.1889184174898468E-5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15">
+        <v>150</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <f>A15*B15</f>
+        <v>450</v>
+      </c>
+      <c r="D15">
+        <f>C15/70</f>
+        <v>6.4285714285714288</v>
+      </c>
+      <c r="E15">
+        <v>4000</v>
+      </c>
+      <c r="F15" s="74">
+        <f t="shared" si="0"/>
+        <v>0.12636012636012636</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="1"/>
+        <v>9.7969773855488161E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16">
+        <v>500</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <f>A16*B16</f>
+        <v>500</v>
+      </c>
+      <c r="D16">
+        <f>C16/70</f>
+        <v>7.1428571428571432</v>
+      </c>
+      <c r="E16">
+        <v>4000</v>
+      </c>
+      <c r="F16" s="74">
+        <f t="shared" si="0"/>
+        <v>0.1404001404001404</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="1"/>
+        <v>1.2523414397700113E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17">
+        <v>750</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <f>A17*B17</f>
+        <v>750</v>
+      </c>
+      <c r="D17">
+        <f>C17/70</f>
+        <v>10.714285714285714</v>
+      </c>
+      <c r="E17">
+        <v>1000</v>
+      </c>
+      <c r="F17" s="74">
+        <f t="shared" si="0"/>
+        <v>5.2650052650052646E-2</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="1"/>
+        <v>7.7924725467582606E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18">
+        <v>250</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <f>A18*B18</f>
+        <v>750</v>
+      </c>
+      <c r="D18">
+        <f>C18/70</f>
+        <v>10.714285714285714</v>
+      </c>
+      <c r="E18">
+        <v>5000</v>
+      </c>
+      <c r="F18" s="74">
+        <f t="shared" si="0"/>
+        <v>0.26325026325026324</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="1"/>
+        <v>3.8962362733791305E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19">
+        <v>150</v>
+      </c>
+      <c r="B19">
+        <v>5</v>
+      </c>
+      <c r="C19">
+        <f>A19*B19</f>
+        <v>750</v>
+      </c>
+      <c r="D19">
+        <f>C19/70</f>
+        <v>10.714285714285714</v>
+      </c>
+      <c r="E19">
+        <v>5000</v>
+      </c>
+      <c r="F19" s="74">
+        <f t="shared" si="0"/>
+        <v>0.26325026325026324</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="1"/>
+        <v>3.8962362733791305E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20">
+        <v>1000</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <f>A20*B20</f>
+        <v>1000</v>
+      </c>
+      <c r="D20">
+        <f>C20/70</f>
+        <v>14.285714285714286</v>
+      </c>
+      <c r="E20">
+        <v>2000</v>
+      </c>
+      <c r="F20" s="74">
+        <f t="shared" si="0"/>
+        <v>0.1404001404001404</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="1"/>
+        <v>2.9086758595330024E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21">
+        <v>150</v>
+      </c>
+      <c r="B21">
+        <v>7</v>
+      </c>
+      <c r="C21">
+        <f>A21*B21</f>
+        <v>1050</v>
+      </c>
+      <c r="D21">
+        <f>C21/70</f>
+        <v>15</v>
+      </c>
+      <c r="E21">
+        <v>5000</v>
+      </c>
+      <c r="F21" s="74">
+        <f t="shared" si="0"/>
+        <v>0.36855036855036855</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="1"/>
+        <v>8.0721375921375908E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22">
+        <v>250</v>
+      </c>
+      <c r="B22">
+        <v>5</v>
+      </c>
+      <c r="C22">
+        <f>A22*B22</f>
+        <v>1250</v>
+      </c>
+      <c r="D22">
+        <f>C22/70</f>
+        <v>17.857142857142858</v>
+      </c>
+      <c r="E22">
+        <v>7500</v>
+      </c>
+      <c r="F22" s="74">
+        <f t="shared" si="0"/>
+        <v>0.65812565812565804</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="1"/>
+        <v>1.753768038910896E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23">
+        <v>1500</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <f>A23*B23</f>
+        <v>1500</v>
+      </c>
+      <c r="D23">
+        <f>C23/70</f>
+        <v>21.428571428571427</v>
+      </c>
+      <c r="E23">
+        <v>1000</v>
+      </c>
+      <c r="F23" s="74">
+        <f t="shared" si="0"/>
+        <v>0.10530010530010529</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="1"/>
+        <v>3.4313056210199056E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24">
+        <v>500</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="C24">
+        <f>A24*B24</f>
+        <v>1500</v>
+      </c>
+      <c r="D24">
+        <f>C24/70</f>
+        <v>21.428571428571427</v>
+      </c>
+      <c r="E24">
+        <v>7500</v>
+      </c>
+      <c r="F24" s="74">
+        <f t="shared" si="0"/>
+        <v>0.78975078975078972</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="1"/>
+        <v>2.5734792157649296E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25">
+        <v>150</v>
+      </c>
+      <c r="B25">
+        <v>10</v>
+      </c>
+      <c r="C25">
+        <f>A25*B25</f>
+        <v>1500</v>
+      </c>
+      <c r="D25">
+        <f>C25/70</f>
+        <v>21.428571428571427</v>
+      </c>
+      <c r="E25">
+        <v>7500</v>
+      </c>
+      <c r="F25" s="74">
+        <f t="shared" si="0"/>
+        <v>0.78975078975078972</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="1"/>
+        <v>2.5734792157649296E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26">
+        <v>250</v>
+      </c>
+      <c r="B26">
+        <v>7</v>
+      </c>
+      <c r="C26">
+        <f>A26*B26</f>
+        <v>1750</v>
+      </c>
+      <c r="D26">
+        <f>C26/70</f>
+        <v>25</v>
+      </c>
+      <c r="E26">
+        <v>7500</v>
+      </c>
+      <c r="F26" s="74">
+        <f t="shared" si="0"/>
+        <v>0.92137592137592139</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="1"/>
+        <v>3.5498869778869777E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27">
+        <v>750</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27">
+        <f>A27*B27</f>
+        <v>2250</v>
+      </c>
+      <c r="D27">
+        <f>C27/70</f>
+        <v>32.142857142857146</v>
+      </c>
+      <c r="E27">
+        <v>10000</v>
+      </c>
+      <c r="F27" s="74">
+        <f t="shared" si="0"/>
+        <v>1.5795015795015797</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="1"/>
+        <v>7.9637230105801551E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28">
+        <v>500</v>
+      </c>
+      <c r="B28">
+        <v>5</v>
+      </c>
+      <c r="C28">
+        <f>A28*B28</f>
+        <v>2500</v>
+      </c>
+      <c r="D28">
+        <f>C28/70</f>
+        <v>35.714285714285715</v>
+      </c>
+      <c r="E28">
+        <v>10000</v>
+      </c>
+      <c r="F28" s="74">
+        <f t="shared" si="0"/>
+        <v>1.7550017550017551</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="1"/>
+        <v>9.8923863678149385E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29">
+        <v>250</v>
+      </c>
+      <c r="B29">
+        <v>10</v>
+      </c>
+      <c r="C29">
+        <f>A29*B29</f>
+        <v>2500</v>
+      </c>
+      <c r="D29">
+        <f>C29/70</f>
+        <v>35.714285714285715</v>
+      </c>
+      <c r="E29">
+        <v>10000</v>
+      </c>
+      <c r="F29" s="74">
+        <f t="shared" si="0"/>
+        <v>1.7550017550017551</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="1"/>
+        <v>9.8923863678149385E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30">
+        <v>1000</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30">
+        <f>A30*B30</f>
+        <v>3000</v>
+      </c>
+      <c r="D30">
+        <f>C30/70</f>
+        <v>42.857142857142854</v>
+      </c>
+      <c r="E30">
+        <v>15000</v>
+      </c>
+      <c r="F30" s="74">
+        <f t="shared" si="0"/>
+        <v>3.1590031590031589</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="1"/>
+        <v>0.21564749135034847</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31">
+        <v>150</v>
+      </c>
+      <c r="B31">
+        <v>20</v>
+      </c>
+      <c r="C31">
+        <f>A31*B31</f>
+        <v>3000</v>
+      </c>
+      <c r="D31">
+        <f>C31/70</f>
+        <v>42.857142857142854</v>
+      </c>
+      <c r="E31">
+        <v>15000</v>
+      </c>
+      <c r="F31" s="74">
+        <f t="shared" si="0"/>
+        <v>3.1590031590031589</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="1"/>
+        <v>0.21564749135034847</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32">
+        <v>500</v>
+      </c>
+      <c r="B32">
+        <v>7</v>
+      </c>
+      <c r="C32">
+        <f>A32*B32</f>
+        <v>3500</v>
+      </c>
+      <c r="D32">
+        <f>C32/70</f>
+        <v>50</v>
+      </c>
+      <c r="E32">
+        <v>15000</v>
+      </c>
+      <c r="F32" s="74">
+        <f t="shared" si="0"/>
+        <v>3.6855036855036856</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="1"/>
+        <v>0.29544491400491402</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33">
+        <v>750</v>
+      </c>
+      <c r="B33">
+        <v>5</v>
+      </c>
+      <c r="C33">
+        <f>A33*B33</f>
+        <v>3750</v>
+      </c>
+      <c r="D33">
+        <f>C33/70</f>
+        <v>53.571428571428569</v>
+      </c>
+      <c r="E33">
+        <v>12500</v>
+      </c>
+      <c r="F33" s="74">
+        <f t="shared" si="0"/>
+        <v>3.2906282906282907</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="1"/>
+        <v>0.28337043574186427</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34">
+        <v>1500</v>
+      </c>
+      <c r="B34">
+        <v>3</v>
+      </c>
+      <c r="C34">
+        <f>A34*B34</f>
+        <v>4500</v>
+      </c>
+      <c r="D34">
+        <f>C34/70</f>
+        <v>64.285714285714292</v>
+      </c>
+      <c r="E34">
+        <v>10000</v>
+      </c>
+      <c r="F34" s="74">
+        <f t="shared" si="0"/>
+        <v>3.1590031590031593</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="1"/>
+        <v>0.32843129318557901</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35">
+        <v>1000</v>
+      </c>
+      <c r="B35">
+        <v>5</v>
+      </c>
+      <c r="C35">
+        <f>A35*B35</f>
+        <v>5000</v>
+      </c>
+      <c r="D35">
+        <f>C35/70</f>
+        <v>71.428571428571431</v>
+      </c>
+      <c r="E35">
+        <v>9000</v>
+      </c>
+      <c r="F35" s="74">
+        <f t="shared" si="0"/>
+        <v>3.1590031590031589</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="1"/>
+        <v>0.36603092573835433</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36">
+        <v>500</v>
+      </c>
+      <c r="B36">
+        <v>10</v>
+      </c>
+      <c r="C36">
+        <f>A36*B36</f>
+        <v>5000</v>
+      </c>
+      <c r="D36">
+        <f>C36/70</f>
+        <v>71.428571428571431</v>
+      </c>
+      <c r="E36">
+        <v>7500</v>
+      </c>
+      <c r="F36" s="74">
+        <f t="shared" si="0"/>
+        <v>2.6325026325026322</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="1"/>
+        <v>0.30502577144862864</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37">
+        <v>250</v>
+      </c>
+      <c r="B37">
+        <v>20</v>
+      </c>
+      <c r="C37">
+        <f>A37*B37</f>
+        <v>5000</v>
+      </c>
+      <c r="D37">
+        <f>C37/70</f>
+        <v>71.428571428571431</v>
+      </c>
+      <c r="E37">
+        <v>6000</v>
+      </c>
+      <c r="F37" s="74">
+        <f t="shared" si="0"/>
+        <v>2.1060021060021059</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="1"/>
+        <v>0.24402061715890291</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38">
+        <v>750</v>
+      </c>
+      <c r="B38">
+        <v>7</v>
+      </c>
+      <c r="C38">
+        <f>A38*B38</f>
+        <v>5250</v>
+      </c>
+      <c r="D38">
+        <f>C38/70</f>
+        <v>75</v>
+      </c>
+      <c r="E38">
+        <v>5000</v>
+      </c>
+      <c r="F38" s="74">
+        <f t="shared" si="0"/>
+        <v>1.8427518427518428</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="1"/>
+        <v>0.22448491400491405</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39">
+        <v>1000</v>
+      </c>
+      <c r="B39">
+        <v>7</v>
+      </c>
+      <c r="C39">
+        <f>A39*B39</f>
+        <v>7000</v>
+      </c>
+      <c r="D39">
+        <f>C39/70</f>
+        <v>100</v>
+      </c>
+      <c r="E39">
+        <v>3000</v>
+      </c>
+      <c r="F39" s="74">
+        <f t="shared" si="0"/>
+        <v>1.4742014742014742</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="1"/>
+        <v>0.24100544471744476</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40">
+        <v>1500</v>
+      </c>
+      <c r="B40">
+        <v>5</v>
+      </c>
+      <c r="C40">
+        <f>A40*B40</f>
+        <v>7500</v>
+      </c>
+      <c r="D40">
+        <f>C40/70</f>
+        <v>107.14285714285714</v>
+      </c>
+      <c r="E40">
+        <v>3000</v>
+      </c>
+      <c r="F40" s="74">
+        <f t="shared" si="0"/>
+        <v>1.5795015795015794</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="1"/>
+        <v>0.2770220921626636</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41">
+        <v>750</v>
+      </c>
+      <c r="B41">
+        <v>10</v>
+      </c>
+      <c r="C41">
+        <f>A41*B41</f>
+        <v>7500</v>
+      </c>
+      <c r="D41">
+        <f>C41/70</f>
+        <v>107.14285714285714</v>
+      </c>
+      <c r="E41">
+        <v>3000</v>
+      </c>
+      <c r="F41" s="74">
+        <f t="shared" si="0"/>
+        <v>1.5795015795015794</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="1"/>
+        <v>0.2770220921626636</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42">
+        <v>1000</v>
+      </c>
+      <c r="B42">
+        <v>10</v>
+      </c>
+      <c r="C42">
+        <f>A42*B42</f>
+        <v>10000</v>
+      </c>
+      <c r="D42">
+        <f>C42/70</f>
+        <v>142.85714285714286</v>
+      </c>
+      <c r="E42">
+        <v>2500</v>
+      </c>
+      <c r="F42" s="74">
+        <f t="shared" si="0"/>
+        <v>1.7550017550017551</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="1"/>
+        <v>0.41226042487756775</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43">
+        <v>500</v>
+      </c>
+      <c r="B43">
+        <v>20</v>
+      </c>
+      <c r="C43">
+        <f>A43*B43</f>
+        <v>10000</v>
+      </c>
+      <c r="D43">
+        <f>C43/70</f>
+        <v>142.85714285714286</v>
+      </c>
+      <c r="E43">
+        <v>2500</v>
+      </c>
+      <c r="F43" s="74">
+        <f t="shared" si="0"/>
+        <v>1.7550017550017551</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="1"/>
+        <v>0.41226042487756775</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44">
+        <v>1500</v>
+      </c>
+      <c r="B44">
+        <v>7</v>
+      </c>
+      <c r="C44">
+        <f>A44*B44</f>
+        <v>10500</v>
+      </c>
+      <c r="D44">
+        <f>C44/70</f>
+        <v>150</v>
+      </c>
+      <c r="E44">
+        <v>2000</v>
+      </c>
+      <c r="F44" s="74">
+        <f t="shared" si="0"/>
+        <v>1.4742014742014742</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="1"/>
+        <v>0.36384801965601965</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45">
+        <v>1500</v>
+      </c>
+      <c r="B45">
+        <v>10</v>
+      </c>
+      <c r="C45">
+        <f>A45*B45</f>
+        <v>15000</v>
+      </c>
+      <c r="D45">
+        <f>C45/70</f>
+        <v>214.28571428571428</v>
+      </c>
+      <c r="E45">
+        <v>1500</v>
+      </c>
+      <c r="F45" s="74">
+        <f t="shared" si="0"/>
+        <v>1.5795015795015794</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="1"/>
+        <v>0.55906462377776645</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46">
+        <v>750</v>
+      </c>
+      <c r="B46">
+        <v>20</v>
+      </c>
+      <c r="C46">
+        <f>A46*B46</f>
+        <v>15000</v>
+      </c>
+      <c r="D46">
+        <f>C46/70</f>
+        <v>214.28571428571428</v>
+      </c>
+      <c r="E46">
+        <v>1250</v>
+      </c>
+      <c r="F46" s="74">
+        <f t="shared" si="0"/>
+        <v>1.3162513162513161</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="1"/>
+        <v>0.46588718648147209</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47">
+        <v>1000</v>
+      </c>
+      <c r="B47">
+        <v>20</v>
+      </c>
+      <c r="C47">
+        <f>A47*B47</f>
+        <v>20000</v>
+      </c>
+      <c r="D47">
+        <f>C47/70</f>
+        <v>285.71428571428572</v>
+      </c>
+      <c r="E47">
+        <v>750</v>
+      </c>
+      <c r="F47" s="74">
+        <f t="shared" si="0"/>
+        <v>1.053001053001053</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="1"/>
+        <v>0.49806513042170197</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48">
+        <v>1500</v>
+      </c>
+      <c r="B48">
+        <v>20</v>
+      </c>
+      <c r="C48">
+        <f>A48*B48</f>
+        <v>30000</v>
+      </c>
+      <c r="D48">
+        <f>C48/70</f>
+        <v>428.57142857142856</v>
+      </c>
+      <c r="E48">
+        <v>500</v>
+      </c>
+      <c r="F48" s="74">
+        <f t="shared" si="0"/>
+        <v>1.053001053001053</v>
+      </c>
+      <c r="I48">
+        <f t="shared" si="1"/>
+        <v>0.74877777987263705</v>
+      </c>
+    </row>
+    <row r="50" spans="5:8">
+      <c r="E50">
+        <f>SUM(E13:E48)</f>
+        <v>203500</v>
+      </c>
+      <c r="F50">
+        <f>SUM(F13:F48)</f>
+        <v>50.542295542295555</v>
+      </c>
+    </row>
+    <row r="51" spans="5:8">
+      <c r="E51" t="s">
+        <v>100</v>
+      </c>
+      <c r="F51" t="s">
+        <v>99</v>
+      </c>
+      <c r="G51" t="s">
+        <v>103</v>
+      </c>
+      <c r="H51" s="75">
+        <f>F50/600</f>
+        <v>8.4237159237159256E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A13:D48">
+    <sortCondition ref="D13:D48"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -10643,13 +11931,13 @@
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="B9" s="60" t="s">
+      <c r="B9" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="60"/>
-      <c r="D9" s="60"/>
-      <c r="E9" s="60"/>
-      <c r="F9" s="60"/>
+      <c r="C9" s="63"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="63"/>
+      <c r="F9" s="63"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="44">
@@ -11670,7 +12958,7 @@
   <dimension ref="B3:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11752,7 +13040,7 @@
         <v>50</v>
       </c>
       <c r="F6">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="G6">
         <v>1500</v>
@@ -11772,7 +13060,7 @@
         <v>30</v>
       </c>
       <c r="F7">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="G7">
         <v>1000</v>
@@ -11792,7 +13080,7 @@
         <v>30</v>
       </c>
       <c r="F8">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="G8">
         <v>750</v>
@@ -11809,10 +13097,10 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F9">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="G9">
         <v>500</v>
@@ -11945,10 +13233,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B2:H42"/>
+  <dimension ref="A2:H42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11995,7 +13283,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="57">
-        <f t="shared" ref="C5:C22" si="0">D5*50</f>
+        <f t="shared" ref="C5:C23" si="0">D5*50</f>
         <v>100</v>
       </c>
       <c r="D5">
@@ -12037,7 +13325,7 @@
       <c r="D8">
         <v>5</v>
       </c>
-      <c r="H8" s="69"/>
+      <c r="H8" s="60"/>
     </row>
     <row r="9" spans="2:8">
       <c r="B9" s="57">
@@ -12135,7 +13423,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="2:4">
+    <row r="17" spans="1:4">
       <c r="B17" s="57">
         <v>14</v>
       </c>
@@ -12147,7 +13435,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="2:4">
+    <row r="18" spans="1:4">
       <c r="B18" s="57">
         <v>15</v>
       </c>
@@ -12159,7 +13447,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="2:4">
+    <row r="19" spans="1:4">
       <c r="B19" s="57">
         <v>16</v>
       </c>
@@ -12171,52 +13459,65 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="2:4">
+    <row r="20" spans="1:4">
       <c r="B20" s="57">
         <v>17</v>
       </c>
       <c r="C20" s="6">
         <f t="shared" si="0"/>
-        <v>10000</v>
+        <v>7500</v>
       </c>
       <c r="D20">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="B21" s="57">
         <v>18</v>
       </c>
       <c r="C21" s="6">
         <f t="shared" si="0"/>
-        <v>15000</v>
+        <v>12500</v>
       </c>
       <c r="D21">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4">
-      <c r="B22" s="58">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="36"/>
+      <c r="B22" s="73">
         <v>19</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C22" s="72">
+        <f t="shared" si="0"/>
+        <v>25000</v>
+      </c>
+      <c r="D22">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="B23" s="58">
+        <v>20</v>
+      </c>
+      <c r="C23" s="7">
         <f t="shared" si="0"/>
         <v>38850</v>
       </c>
-      <c r="D22">
+      <c r="D23">
         <v>777</v>
       </c>
     </row>
-    <row r="29" spans="2:4">
+    <row r="29" spans="1:4">
       <c r="B29" s="3"/>
     </row>
-    <row r="30" spans="2:4">
+    <row r="30" spans="1:4">
       <c r="B30" s="3"/>
     </row>
-    <row r="31" spans="2:4">
+    <row r="31" spans="1:4">
       <c r="B31" s="3"/>
     </row>
-    <row r="32" spans="2:4">
+    <row r="32" spans="1:4">
       <c r="B32" s="3"/>
     </row>
     <row r="33" spans="2:2">
@@ -12284,7 +13585,7 @@
       <c r="B3" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="70">
+      <c r="C3" s="61">
         <v>1000</v>
       </c>
       <c r="D3" s="57">
@@ -12295,7 +13596,7 @@
       <c r="B4" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="70">
+      <c r="C4" s="61">
         <v>1000</v>
       </c>
       <c r="D4" s="57">
@@ -12306,7 +13607,7 @@
       <c r="B5" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="70">
+      <c r="C5" s="61">
         <v>1000</v>
       </c>
       <c r="D5" s="57">
@@ -12317,7 +13618,7 @@
       <c r="B6" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="70">
+      <c r="C6" s="61">
         <v>1000</v>
       </c>
       <c r="D6" s="57">
@@ -12328,7 +13629,7 @@
       <c r="B7" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="C7" s="71">
+      <c r="C7" s="62">
         <v>1000</v>
       </c>
       <c r="D7" s="58">
@@ -12422,14 +13723,14 @@
   <sheetData>
     <row r="2" spans="2:8" ht="15.75" thickBot="1">
       <c r="B2" s="12"/>
-      <c r="C2" s="61" t="s">
+      <c r="C2" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="63"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="66"/>
     </row>
     <row r="3" spans="2:8">
       <c r="B3" s="12"/>
@@ -12821,7 +14122,7 @@
       </c>
       <c r="I19" s="21">
         <f>I62</f>
-        <v>0.60268384021061638</v>
+        <v>0.67339141347579123</v>
       </c>
     </row>
     <row r="20" spans="2:9">
@@ -13730,7 +15031,7 @@
       <c r="H62" s="32"/>
       <c r="I62" s="21">
         <f>I127</f>
-        <v>0.60268384021061638</v>
+        <v>0.67339141347579123</v>
       </c>
     </row>
     <row r="63" spans="2:9">
@@ -14532,7 +15833,7 @@
       <c r="H100" s="32"/>
       <c r="I100" s="21">
         <f>I127</f>
-        <v>0.60268384021061638</v>
+        <v>0.67339141347579123</v>
       </c>
     </row>
     <row r="101" spans="2:9">
@@ -15103,7 +16404,7 @@
       <c r="H127" s="32"/>
       <c r="I127" s="21">
         <f>J147</f>
-        <v>0.60268384021061638</v>
+        <v>0.67339141347579123</v>
       </c>
     </row>
     <row r="128" spans="2:9">
@@ -15402,15 +16703,15 @@
       <c r="H143" s="50"/>
     </row>
     <row r="145" spans="2:13">
-      <c r="B145" s="68" t="s">
+      <c r="B145" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="C145" s="68"/>
-      <c r="D145" s="68"/>
-      <c r="E145" s="68"/>
-      <c r="F145" s="68"/>
-      <c r="G145" s="68"/>
-      <c r="H145" s="68"/>
+      <c r="C145" s="71"/>
+      <c r="D145" s="71"/>
+      <c r="E145" s="71"/>
+      <c r="F145" s="71"/>
+      <c r="G145" s="71"/>
+      <c r="H145" s="71"/>
     </row>
     <row r="146" spans="2:13">
       <c r="B146" s="19" t="s">
@@ -15468,7 +16769,7 @@
       </c>
       <c r="J147" s="13">
         <f>Q181</f>
-        <v>0.60268384021061638</v>
+        <v>0.67339141347579123</v>
       </c>
     </row>
     <row r="148" spans="2:13">
@@ -15893,33 +17194,33 @@
       </c>
     </row>
     <row r="165" spans="2:26">
-      <c r="B165" s="64" t="s">
+      <c r="B165" s="67" t="s">
         <v>45</v>
       </c>
-      <c r="C165" s="64"/>
-      <c r="D165" s="64"/>
-      <c r="E165" s="64"/>
-      <c r="F165" s="64"/>
-      <c r="G165" s="64"/>
-      <c r="H165" s="64"/>
-      <c r="K165" s="64" t="s">
+      <c r="C165" s="67"/>
+      <c r="D165" s="67"/>
+      <c r="E165" s="67"/>
+      <c r="F165" s="67"/>
+      <c r="G165" s="67"/>
+      <c r="H165" s="67"/>
+      <c r="K165" s="67" t="s">
         <v>47</v>
       </c>
-      <c r="L165" s="64"/>
-      <c r="M165" s="64"/>
-      <c r="N165" s="64"/>
-      <c r="O165" s="64"/>
-      <c r="P165" s="64"/>
-      <c r="Q165" s="64"/>
-      <c r="T165" s="64" t="s">
+      <c r="L165" s="67"/>
+      <c r="M165" s="67"/>
+      <c r="N165" s="67"/>
+      <c r="O165" s="67"/>
+      <c r="P165" s="67"/>
+      <c r="Q165" s="67"/>
+      <c r="T165" s="67" t="s">
         <v>50</v>
       </c>
-      <c r="U165" s="64"/>
-      <c r="V165" s="64"/>
-      <c r="W165" s="64"/>
-      <c r="X165" s="64"/>
-      <c r="Y165" s="64"/>
-      <c r="Z165" s="64"/>
+      <c r="U165" s="67"/>
+      <c r="V165" s="67"/>
+      <c r="W165" s="67"/>
+      <c r="X165" s="67"/>
+      <c r="Y165" s="67"/>
+      <c r="Z165" s="67"/>
     </row>
     <row r="166" spans="2:26">
       <c r="B166" s="18" t="s">
@@ -16153,7 +17454,7 @@
       </c>
       <c r="O169" s="18">
         <f t="shared" ref="O169:O177" si="11">((1-$H169)*($C169+C$167)*($D169+D$167)*($E169+E$167)*(F$167+$F169)*(1-G$167-G169)+H169*($C169+C$167+C$179)*($D169+D$167+D$179)*($E169+E$167+E$179)*(F$167+$F169+F$179)*(1-G$167-G169-G$179))*F188-(1-G$167-G169-$H169*G$179)*$F188*PRODUCT(C$167:F$167)</f>
-        <v>4.0417420659078648E-2</v>
+        <v>5.3889894212104862E-2</v>
       </c>
       <c r="P169" s="18">
         <f t="shared" ref="P169:P177" si="12">((1-$H169)*($C169+C$167)*($D169+D$167)*($E169+E$167)*(F$167+$F169)*(G$167+G169)+H169*($C169+C$167+C$179)*($D169+D$167+D$179)*($E169+E$167+E$179)*(F$167+$F169+F$179)*(+G$167+G169+G$179))*G188-PRODUCT(C$167:G$167)*G188</f>
@@ -16213,7 +17514,7 @@
       </c>
       <c r="O170" s="18">
         <f t="shared" si="11"/>
-        <v>1.646621339952373E-2</v>
+        <v>2.4699320099285597E-2</v>
       </c>
       <c r="P170" s="18">
         <f t="shared" si="12"/>
@@ -16273,7 +17574,7 @@
       </c>
       <c r="O171" s="18">
         <f t="shared" si="11"/>
-        <v>3.2759340721663352E-2</v>
+        <v>4.9139011082495028E-2</v>
       </c>
       <c r="P171" s="18">
         <f t="shared" si="12"/>
@@ -16329,11 +17630,11 @@
       </c>
       <c r="N172" s="18">
         <f t="shared" si="10"/>
-        <v>4.8709412371262542E-2</v>
+        <v>5.8451294845515055E-2</v>
       </c>
       <c r="O172" s="18">
         <f t="shared" si="11"/>
-        <v>2.2880440177302726E-2</v>
+        <v>4.5760880354605453E-2</v>
       </c>
       <c r="P172" s="18">
         <f t="shared" si="12"/>
@@ -16844,7 +18145,7 @@
       <c r="P181" s="26"/>
       <c r="Q181" s="26">
         <f>SUM(L167:P180)</f>
-        <v>0.60268384021061638</v>
+        <v>0.67339141347579123</v>
       </c>
       <c r="T181" s="24" t="s">
         <v>41</v>
@@ -16860,14 +18161,14 @@
       <c r="X183" s="41"/>
     </row>
     <row r="184" spans="2:26">
-      <c r="B184" s="65" t="s">
+      <c r="B184" s="68" t="s">
         <v>46</v>
       </c>
-      <c r="C184" s="66"/>
-      <c r="D184" s="66"/>
-      <c r="E184" s="66"/>
-      <c r="F184" s="66"/>
-      <c r="G184" s="67"/>
+      <c r="C184" s="69"/>
+      <c r="D184" s="69"/>
+      <c r="E184" s="69"/>
+      <c r="F184" s="69"/>
+      <c r="G184" s="70"/>
       <c r="K184" s="20" t="s">
         <v>5</v>
       </c>
@@ -17046,7 +18347,7 @@
       </c>
       <c r="F188" s="35">
         <f>Paytable!F6</f>
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="G188" s="35">
         <f>Paytable!G6</f>
@@ -17093,7 +18394,7 @@
       </c>
       <c r="F189" s="35">
         <f>Paytable!F7</f>
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="G189" s="35">
         <f>Paytable!G7</f>
@@ -17140,7 +18441,7 @@
       </c>
       <c r="F190" s="35">
         <f>Paytable!F8</f>
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="G190" s="35">
         <f>Paytable!G8</f>
@@ -17187,11 +18488,11 @@
       </c>
       <c r="E191" s="35">
         <f>Paytable!E9</f>
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F191" s="35">
         <f>Paytable!F9</f>
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="G191" s="35">
         <f>Paytable!G9</f>
@@ -17457,14 +18758,14 @@
   <sheetData>
     <row r="2" spans="2:8" ht="15.75" thickBot="1">
       <c r="B2" s="12"/>
-      <c r="C2" s="61" t="s">
+      <c r="C2" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="63"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="66"/>
     </row>
     <row r="3" spans="2:8">
       <c r="B3" s="12"/>
@@ -17856,7 +19157,7 @@
       </c>
       <c r="I19" s="21">
         <f>I62</f>
-        <v>0.54572066807162323</v>
+        <v>0.59451002144083454</v>
       </c>
     </row>
     <row r="20" spans="2:9">
@@ -18765,7 +20066,7 @@
       <c r="H62" s="32"/>
       <c r="I62" s="21">
         <f>I127</f>
-        <v>0.54572066807162323</v>
+        <v>0.59451002144083454</v>
       </c>
     </row>
     <row r="63" spans="2:9">
@@ -19567,7 +20868,7 @@
       <c r="H100" s="32"/>
       <c r="I100" s="21">
         <f>I127</f>
-        <v>0.54572066807162323</v>
+        <v>0.59451002144083454</v>
       </c>
     </row>
     <row r="101" spans="2:9">
@@ -20138,7 +21439,7 @@
       <c r="H127" s="32"/>
       <c r="I127" s="21">
         <f>J147</f>
-        <v>0.54572066807162323</v>
+        <v>0.59451002144083454</v>
       </c>
     </row>
     <row r="128" spans="2:9">
@@ -20437,15 +21738,15 @@
       <c r="H143" s="50"/>
     </row>
     <row r="145" spans="2:13">
-      <c r="B145" s="68" t="s">
+      <c r="B145" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="C145" s="68"/>
-      <c r="D145" s="68"/>
-      <c r="E145" s="68"/>
-      <c r="F145" s="68"/>
-      <c r="G145" s="68"/>
-      <c r="H145" s="68"/>
+      <c r="C145" s="71"/>
+      <c r="D145" s="71"/>
+      <c r="E145" s="71"/>
+      <c r="F145" s="71"/>
+      <c r="G145" s="71"/>
+      <c r="H145" s="71"/>
     </row>
     <row r="146" spans="2:13">
       <c r="B146" s="19" t="s">
@@ -20502,7 +21803,7 @@
       </c>
       <c r="J147" s="13">
         <f>Q181</f>
-        <v>0.54572066807162323</v>
+        <v>0.59451002144083454</v>
       </c>
     </row>
     <row r="148" spans="2:13">
@@ -20916,33 +22217,33 @@
       </c>
     </row>
     <row r="165" spans="2:26">
-      <c r="B165" s="64" t="s">
+      <c r="B165" s="67" t="s">
         <v>45</v>
       </c>
-      <c r="C165" s="64"/>
-      <c r="D165" s="64"/>
-      <c r="E165" s="64"/>
-      <c r="F165" s="64"/>
-      <c r="G165" s="64"/>
-      <c r="H165" s="64"/>
-      <c r="K165" s="64" t="s">
+      <c r="C165" s="67"/>
+      <c r="D165" s="67"/>
+      <c r="E165" s="67"/>
+      <c r="F165" s="67"/>
+      <c r="G165" s="67"/>
+      <c r="H165" s="67"/>
+      <c r="K165" s="67" t="s">
         <v>47</v>
       </c>
-      <c r="L165" s="64"/>
-      <c r="M165" s="64"/>
-      <c r="N165" s="64"/>
-      <c r="O165" s="64"/>
-      <c r="P165" s="64"/>
-      <c r="Q165" s="64"/>
-      <c r="T165" s="64" t="s">
+      <c r="L165" s="67"/>
+      <c r="M165" s="67"/>
+      <c r="N165" s="67"/>
+      <c r="O165" s="67"/>
+      <c r="P165" s="67"/>
+      <c r="Q165" s="67"/>
+      <c r="T165" s="67" t="s">
         <v>50</v>
       </c>
-      <c r="U165" s="64"/>
-      <c r="V165" s="64"/>
-      <c r="W165" s="64"/>
-      <c r="X165" s="64"/>
-      <c r="Y165" s="64"/>
-      <c r="Z165" s="64"/>
+      <c r="U165" s="67"/>
+      <c r="V165" s="67"/>
+      <c r="W165" s="67"/>
+      <c r="X165" s="67"/>
+      <c r="Y165" s="67"/>
+      <c r="Z165" s="67"/>
     </row>
     <row r="166" spans="2:26">
       <c r="B166" s="18" t="s">
@@ -21176,7 +22477,7 @@
       </c>
       <c r="O169" s="18">
         <f t="shared" ref="O169:O177" si="5">((1-$H169)*($C169+C$167)*($D169+D$167)*($E169+E$167)*(F$167+$F169)*(1-G$167-G169)+H169*($C169+C$167+C$179)*($D169+D$167+D$179)*($E169+E$167+E$179)*(F$167+$F169+F$179)*(1-G$167-G169-G$179))*F188-(1-G$167-G169-$H169*G$179)*$F188*PRODUCT(C$167:F$167)</f>
-        <v>2.3175576144536622E-2</v>
+        <v>3.0900768192715495E-2</v>
       </c>
       <c r="P169" s="18">
         <f t="shared" ref="P169:P177" si="6">((1-$H169)*($C169+C$167)*($D169+D$167)*($E169+E$167)*(F$167+$F169)*(G$167+G169)+H169*($C169+C$167+C$179)*($D169+D$167+D$179)*($E169+E$167+E$179)*(F$167+$F169+F$179)*(+G$167+G169+G$179))*G188-PRODUCT(C$167:G$167)*G188</f>
@@ -21236,7 +22537,7 @@
       </c>
       <c r="O170" s="18">
         <f t="shared" si="5"/>
-        <v>1.8310184073958836E-2</v>
+        <v>2.7465276110938255E-2</v>
       </c>
       <c r="P170" s="18">
         <f t="shared" si="6"/>
@@ -21296,7 +22597,7 @@
       </c>
       <c r="O171" s="18">
         <f t="shared" si="5"/>
-        <v>1.931771099404082E-2</v>
+        <v>2.8976566491061229E-2</v>
       </c>
       <c r="P171" s="18">
         <f t="shared" si="6"/>
@@ -21352,11 +22653,11 @@
       </c>
       <c r="N172" s="18">
         <f t="shared" si="4"/>
-        <v>1.590708291308909E-2</v>
+        <v>1.9088499495706911E-2</v>
       </c>
       <c r="O172" s="18">
         <f t="shared" si="5"/>
-        <v>1.9068797204414803E-2</v>
+        <v>3.8137594408829606E-2</v>
       </c>
       <c r="P172" s="18">
         <f t="shared" si="6"/>
@@ -21867,7 +23168,7 @@
       <c r="P181" s="26"/>
       <c r="Q181" s="26">
         <f>SUM(L167:P180)</f>
-        <v>0.54572066807162323</v>
+        <v>0.59451002144083454</v>
       </c>
       <c r="T181" s="24" t="s">
         <v>41</v>
@@ -21883,14 +23184,14 @@
       <c r="X183" s="41"/>
     </row>
     <row r="184" spans="2:26">
-      <c r="B184" s="65" t="s">
+      <c r="B184" s="68" t="s">
         <v>46</v>
       </c>
-      <c r="C184" s="66"/>
-      <c r="D184" s="66"/>
-      <c r="E184" s="66"/>
-      <c r="F184" s="66"/>
-      <c r="G184" s="67"/>
+      <c r="C184" s="69"/>
+      <c r="D184" s="69"/>
+      <c r="E184" s="69"/>
+      <c r="F184" s="69"/>
+      <c r="G184" s="70"/>
       <c r="K184" s="20" t="s">
         <v>5</v>
       </c>
@@ -22069,7 +23370,7 @@
       </c>
       <c r="F188" s="35">
         <f>Paytable!F6</f>
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="G188" s="35">
         <f>Paytable!G6</f>
@@ -22116,7 +23417,7 @@
       </c>
       <c r="F189" s="35">
         <f>Paytable!F7</f>
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="G189" s="35">
         <f>Paytable!G7</f>
@@ -22163,7 +23464,7 @@
       </c>
       <c r="F190" s="35">
         <f>Paytable!F8</f>
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="G190" s="35">
         <f>Paytable!G8</f>
@@ -22210,11 +23511,11 @@
       </c>
       <c r="E191" s="35">
         <f>Paytable!E9</f>
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F191" s="35">
         <f>Paytable!F9</f>
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="G191" s="35">
         <f>Paytable!G9</f>
@@ -22397,12 +23698,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="T165:Z165"/>
     <mergeCell ref="B184:G184"/>
     <mergeCell ref="C2:H2"/>
     <mergeCell ref="B145:H145"/>
     <mergeCell ref="B165:H165"/>
     <mergeCell ref="K165:Q165"/>
-    <mergeCell ref="T165:Z165"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:Z2 L3:Z142 A3:J142 A143:Z1048576">
     <cfRule type="containsText" dxfId="30" priority="1" operator="containsText" text="Inner">

</xml_diff>

<commit_message>
Also saved Excel doc for last commit
</commit_message>
<xml_diff>
--- a/AnimalWill/AnimalWillMaths.xlsx
+++ b/AnimalWill/AnimalWillMaths.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\konstantin.d\source\repos\AnimalWill\AnimalWill\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{817C64FB-CC46-4C44-8239-D1FC8E92C790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7C52CC7-E5F8-462C-9C7C-18089BDD8473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="9" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10585,8 +10585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A2:N51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10835,19 +10835,23 @@
         <v>2.1428571428571428</v>
       </c>
       <c r="E13">
-        <v>750</v>
+        <v>1000</v>
       </c>
       <c r="F13" s="74">
         <f>E13*D13/E$50</f>
-        <v>7.8975078975078977E-3</v>
+        <v>1.1045655375552282E-2</v>
+      </c>
+      <c r="G13">
+        <f>1/(E13/E$50)</f>
+        <v>194</v>
       </c>
       <c r="I13">
-        <f>POWER(D13 - 0.96,2)/600*E13/E$50</f>
-        <v>8.5942937371508791E-6</v>
+        <f>POWER(D13 - 0.96,2)/686*E13/E$50</f>
+        <v>1.0513292510055027E-5</v>
       </c>
       <c r="J13">
         <f>SQRT(SUM(I13:I48))</f>
-        <v>2.6721853465781709</v>
+        <v>2.5482050206059284</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -10866,15 +10870,19 @@
         <v>3.5714285714285716</v>
       </c>
       <c r="E14">
-        <v>750</v>
+        <v>1000</v>
       </c>
       <c r="F14" s="74">
         <f t="shared" ref="F14:F48" si="0">E14*D14/E$50</f>
-        <v>1.3162513162513163E-2</v>
+        <v>1.8409425625920472E-2</v>
+      </c>
+      <c r="G14">
+        <f t="shared" ref="G14:G47" si="1">1/(E14/E$50)</f>
+        <v>194</v>
       </c>
       <c r="I14">
-        <f t="shared" ref="I14:I48" si="1">POWER(D14 - 0.96,2)/600*E14/E$50</f>
-        <v>4.1889184174898468E-5</v>
+        <f t="shared" ref="I14:I48" si="2">POWER(D14 - 0.96,2)/686*E14/E$50</f>
+        <v>5.1242517385061092E-5</v>
       </c>
     </row>
     <row r="15" spans="1:14">
@@ -10893,15 +10901,19 @@
         <v>6.4285714285714288</v>
       </c>
       <c r="E15">
-        <v>4000</v>
+        <v>1000</v>
       </c>
       <c r="F15" s="74">
         <f t="shared" si="0"/>
-        <v>0.12636012636012636</v>
+        <v>3.3136966126656849E-2</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>194</v>
       </c>
       <c r="I15">
-        <f t="shared" si="1"/>
-        <v>9.7969773855488161E-4</v>
+        <f t="shared" si="2"/>
+        <v>2.2470975826837004E-4</v>
       </c>
     </row>
     <row r="16" spans="1:14">
@@ -10924,11 +10936,15 @@
       </c>
       <c r="F16" s="74">
         <f t="shared" si="0"/>
-        <v>0.1404001404001404</v>
+        <v>0.14727540500736377</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="1"/>
+        <v>48.5</v>
       </c>
       <c r="I16">
-        <f t="shared" si="1"/>
-        <v>1.2523414397700113E-3</v>
+        <f t="shared" si="2"/>
+        <v>1.14898026656787E-3</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -10951,11 +10967,15 @@
       </c>
       <c r="F17" s="74">
         <f t="shared" si="0"/>
-        <v>5.2650052650052646E-2</v>
+        <v>5.5228276877761412E-2</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="1"/>
+        <v>194</v>
       </c>
       <c r="I17">
-        <f t="shared" si="1"/>
-        <v>7.7924725467582606E-4</v>
+        <f t="shared" si="2"/>
+        <v>7.1493259742657549E-4</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -10978,11 +10998,15 @@
       </c>
       <c r="F18" s="74">
         <f t="shared" si="0"/>
-        <v>0.26325026325026324</v>
+        <v>0.27614138438880703</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="1"/>
+        <v>38.800000000000004</v>
       </c>
       <c r="I18">
-        <f t="shared" si="1"/>
-        <v>3.8962362733791305E-3</v>
+        <f t="shared" si="2"/>
+        <v>3.5746629871328773E-3</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -11001,15 +11025,19 @@
         <v>10.714285714285714</v>
       </c>
       <c r="E19">
-        <v>5000</v>
+        <v>2000</v>
       </c>
       <c r="F19" s="74">
         <f t="shared" si="0"/>
-        <v>0.26325026325026324</v>
+        <v>0.11045655375552282</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="1"/>
+        <v>97</v>
       </c>
       <c r="I19">
-        <f t="shared" si="1"/>
-        <v>3.8962362733791305E-3</v>
+        <f>POWER(D19 - 0.96,2)/686*E19/E$50</f>
+        <v>1.429865194853151E-3</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -11032,11 +11060,15 @@
       </c>
       <c r="F20" s="74">
         <f t="shared" si="0"/>
-        <v>0.1404001404001404</v>
+        <v>0.14727540500736377</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="1"/>
+        <v>97</v>
       </c>
       <c r="I20">
-        <f t="shared" si="1"/>
-        <v>2.9086758595330024E-3</v>
+        <f t="shared" si="2"/>
+        <v>2.6686102194777707E-3</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -11055,15 +11087,19 @@
         <v>15</v>
       </c>
       <c r="E21">
-        <v>5000</v>
+        <v>2000</v>
       </c>
       <c r="F21" s="74">
         <f t="shared" si="0"/>
-        <v>0.36855036855036855</v>
+        <v>0.15463917525773196</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="1"/>
+        <v>97</v>
       </c>
       <c r="I21">
-        <f t="shared" si="1"/>
-        <v>8.0721375921375908E-3</v>
+        <f t="shared" si="2"/>
+        <v>2.9623636199693419E-3</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -11086,11 +11122,15 @@
       </c>
       <c r="F22" s="74">
         <f t="shared" si="0"/>
-        <v>0.65812565812565804</v>
+        <v>0.69035346097201766</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="1"/>
+        <v>25.866666666666667</v>
       </c>
       <c r="I22">
-        <f t="shared" si="1"/>
-        <v>1.753768038910896E-2</v>
+        <f t="shared" si="2"/>
+        <v>1.6090219526841726E-2</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -11113,11 +11153,15 @@
       </c>
       <c r="F23" s="74">
         <f t="shared" si="0"/>
-        <v>0.10530010530010529</v>
+        <v>0.11045655375552282</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="1"/>
+        <v>194</v>
       </c>
       <c r="I23">
-        <f t="shared" si="1"/>
-        <v>3.4313056210199056E-3</v>
+        <f t="shared" si="2"/>
+        <v>3.1481050789466088E-3</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -11140,11 +11184,15 @@
       </c>
       <c r="F24" s="74">
         <f t="shared" si="0"/>
-        <v>0.78975078975078972</v>
+        <v>0.82842415316642115</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="1"/>
+        <v>25.866666666666667</v>
       </c>
       <c r="I24">
-        <f t="shared" si="1"/>
-        <v>2.5734792157649296E-2</v>
+        <f t="shared" si="2"/>
+        <v>2.3610788092099568E-2</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -11163,15 +11211,19 @@
         <v>21.428571428571427</v>
       </c>
       <c r="E25">
-        <v>7500</v>
+        <v>2000</v>
       </c>
       <c r="F25" s="74">
         <f t="shared" si="0"/>
-        <v>0.78975078975078972</v>
+        <v>0.22091310751104565</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="1"/>
+        <v>97</v>
       </c>
       <c r="I25">
-        <f t="shared" si="1"/>
-        <v>2.5734792157649296E-2</v>
+        <f t="shared" si="2"/>
+        <v>6.2962101578932176E-3</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -11190,15 +11242,19 @@
         <v>25</v>
       </c>
       <c r="E26">
-        <v>7500</v>
+        <v>10000</v>
       </c>
       <c r="F26" s="74">
         <f t="shared" si="0"/>
-        <v>0.92137592137592139</v>
+        <v>1.2886597938144331</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="1"/>
+        <v>19.400000000000002</v>
       </c>
       <c r="I26">
-        <f t="shared" si="1"/>
-        <v>3.5498869778869777E-2</v>
+        <f t="shared" si="2"/>
+        <v>4.3425325358420246E-2</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -11217,15 +11273,19 @@
         <v>32.142857142857146</v>
       </c>
       <c r="E27">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="F27" s="74">
         <f t="shared" si="0"/>
-        <v>1.5795015795015797</v>
+        <v>2.4852724594992637</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="1"/>
+        <v>12.933333333333334</v>
       </c>
       <c r="I27">
-        <f t="shared" si="1"/>
-        <v>7.9637230105801551E-2</v>
+        <f t="shared" si="2"/>
+        <v>0.10959663591323941</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -11244,15 +11304,19 @@
         <v>35.714285714285715</v>
       </c>
       <c r="E28">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="F28" s="74">
         <f t="shared" si="0"/>
-        <v>1.7550017550017551</v>
+        <v>2.7614138438880707</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="1"/>
+        <v>12.933333333333334</v>
       </c>
       <c r="I28">
-        <f t="shared" si="1"/>
-        <v>9.8923863678149385E-2</v>
+        <f t="shared" si="2"/>
+        <v>0.13613887193541718</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -11271,15 +11335,19 @@
         <v>35.714285714285715</v>
       </c>
       <c r="E29">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="F29" s="74">
         <f t="shared" si="0"/>
-        <v>1.7550017550017551</v>
+        <v>2.7614138438880707</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="1"/>
+        <v>12.933333333333334</v>
       </c>
       <c r="I29">
-        <f t="shared" si="1"/>
-        <v>9.8923863678149385E-2</v>
+        <f t="shared" si="2"/>
+        <v>0.13613887193541718</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -11302,11 +11370,15 @@
       </c>
       <c r="F30" s="74">
         <f t="shared" si="0"/>
-        <v>3.1590031590031589</v>
+        <v>3.3136966126656846</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="1"/>
+        <v>12.933333333333334</v>
       </c>
       <c r="I30">
-        <f t="shared" si="1"/>
-        <v>0.21564749135034847</v>
+        <f t="shared" si="2"/>
+        <v>0.19784916814851933</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -11325,15 +11397,19 @@
         <v>42.857142857142854</v>
       </c>
       <c r="E31">
-        <v>15000</v>
+        <v>2000</v>
       </c>
       <c r="F31" s="74">
         <f t="shared" si="0"/>
-        <v>3.1590031590031589</v>
+        <v>0.4418262150220913</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="1"/>
+        <v>97</v>
       </c>
       <c r="I31">
-        <f t="shared" si="1"/>
-        <v>0.21564749135034847</v>
+        <f t="shared" si="2"/>
+        <v>2.6379889086469242E-2</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -11356,11 +11432,15 @@
       </c>
       <c r="F32" s="74">
         <f t="shared" si="0"/>
-        <v>3.6855036855036856</v>
+        <v>3.865979381443299</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="1"/>
+        <v>12.933333333333334</v>
       </c>
       <c r="I32">
-        <f t="shared" si="1"/>
-        <v>0.29544491400491402</v>
+        <f t="shared" si="2"/>
+        <v>0.27106056325328365</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -11383,11 +11463,15 @@
       </c>
       <c r="F33" s="74">
         <f t="shared" si="0"/>
-        <v>3.2906282906282907</v>
+        <v>3.4517673048600885</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="1"/>
+        <v>15.520000000000001</v>
       </c>
       <c r="I33">
-        <f t="shared" si="1"/>
-        <v>0.28337043574186427</v>
+        <f t="shared" si="2"/>
+        <v>0.25998264407503252</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -11410,11 +11494,15 @@
       </c>
       <c r="F34" s="74">
         <f t="shared" si="0"/>
-        <v>3.1590031590031593</v>
+        <v>3.3136966126656855</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="1"/>
+        <v>19.400000000000002</v>
       </c>
       <c r="I34">
-        <f t="shared" si="1"/>
-        <v>0.32843129318557901</v>
+        <f t="shared" si="2"/>
+        <v>0.30132443342519905</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -11437,11 +11525,15 @@
       </c>
       <c r="F35" s="74">
         <f t="shared" si="0"/>
-        <v>3.1590031590031589</v>
+        <v>3.3136966126656846</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="1"/>
+        <v>21.555555555555554</v>
       </c>
       <c r="I35">
-        <f t="shared" si="1"/>
-        <v>0.36603092573835433</v>
+        <f t="shared" si="2"/>
+        <v>0.33582080515052953</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -11464,11 +11556,15 @@
       </c>
       <c r="F36" s="74">
         <f t="shared" si="0"/>
-        <v>2.6325026325026322</v>
+        <v>2.7614138438880707</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="1"/>
+        <v>25.866666666666667</v>
       </c>
       <c r="I36">
-        <f t="shared" si="1"/>
-        <v>0.30502577144862864</v>
+        <f t="shared" si="2"/>
+        <v>0.27985067095877458</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -11491,11 +11587,15 @@
       </c>
       <c r="F37" s="74">
         <f t="shared" si="0"/>
-        <v>2.1060021060021059</v>
+        <v>2.2091310751104567</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="1"/>
+        <v>32.333333333333329</v>
       </c>
       <c r="I37">
-        <f t="shared" si="1"/>
-        <v>0.24402061715890291</v>
+        <f t="shared" si="2"/>
+        <v>0.22388053676701969</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -11518,11 +11618,15 @@
       </c>
       <c r="F38" s="74">
         <f t="shared" si="0"/>
-        <v>1.8427518427518428</v>
+        <v>1.9329896907216495</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="1"/>
+        <v>38.800000000000004</v>
       </c>
       <c r="I38">
-        <f t="shared" si="1"/>
-        <v>0.22448491400491405</v>
+        <f t="shared" si="2"/>
+        <v>0.20595719996393258</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -11545,11 +11649,15 @@
       </c>
       <c r="F39" s="74">
         <f t="shared" si="0"/>
-        <v>1.4742014742014742</v>
+        <v>1.5463917525773196</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="1"/>
+        <v>64.666666666666657</v>
       </c>
       <c r="I39">
-        <f t="shared" si="1"/>
-        <v>0.24100544471744476</v>
+        <f t="shared" si="2"/>
+        <v>0.22111421959063451</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -11572,11 +11680,15 @@
       </c>
       <c r="F40" s="74">
         <f t="shared" si="0"/>
-        <v>1.5795015795015794</v>
+        <v>1.6568483063328423</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="1"/>
+        <v>64.666666666666657</v>
       </c>
       <c r="I40">
-        <f t="shared" si="1"/>
-        <v>0.2770220921626636</v>
+        <f t="shared" si="2"/>
+        <v>0.25415825683824667</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -11599,11 +11711,15 @@
       </c>
       <c r="F41" s="74">
         <f t="shared" si="0"/>
-        <v>1.5795015795015794</v>
+        <v>1.6568483063328423</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="1"/>
+        <v>64.666666666666657</v>
       </c>
       <c r="I41">
-        <f t="shared" si="1"/>
-        <v>0.2770220921626636</v>
+        <f t="shared" si="2"/>
+        <v>0.25415825683824667</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -11626,11 +11742,15 @@
       </c>
       <c r="F42" s="74">
         <f t="shared" si="0"/>
-        <v>1.7550017550017551</v>
+        <v>1.8409425625920472</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="1"/>
+        <v>77.600000000000009</v>
       </c>
       <c r="I42">
-        <f t="shared" si="1"/>
-        <v>0.41226042487756775</v>
+        <f t="shared" si="2"/>
+        <v>0.37823478312607844</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -11653,11 +11773,15 @@
       </c>
       <c r="F43" s="74">
         <f t="shared" si="0"/>
-        <v>1.7550017550017551</v>
+        <v>1.8409425625920472</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="1"/>
+        <v>77.600000000000009</v>
       </c>
       <c r="I43">
-        <f t="shared" si="1"/>
-        <v>0.41226042487756775</v>
+        <f t="shared" si="2"/>
+        <v>0.37823478312607844</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -11680,11 +11804,15 @@
       </c>
       <c r="F44" s="74">
         <f t="shared" si="0"/>
-        <v>1.4742014742014742</v>
+        <v>1.5463917525773196</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="1"/>
+        <v>97</v>
       </c>
       <c r="I44">
-        <f t="shared" si="1"/>
-        <v>0.36384801965601965</v>
+        <f t="shared" si="2"/>
+        <v>0.33381806377926715</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -11707,11 +11835,15 @@
       </c>
       <c r="F45" s="74">
         <f t="shared" si="0"/>
-        <v>1.5795015795015794</v>
+        <v>1.6568483063328423</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="1"/>
+        <v>129.33333333333331</v>
       </c>
       <c r="I45">
-        <f t="shared" si="1"/>
-        <v>0.55906462377776645</v>
+        <f t="shared" si="2"/>
+        <v>0.51292259447616007</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -11734,11 +11866,15 @@
       </c>
       <c r="F46" s="74">
         <f t="shared" si="0"/>
-        <v>1.3162513162513161</v>
+        <v>1.3807069219440353</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="1"/>
+        <v>155.20000000000002</v>
       </c>
       <c r="I46">
-        <f t="shared" si="1"/>
-        <v>0.46588718648147209</v>
+        <f t="shared" si="2"/>
+        <v>0.42743549539680004</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -11761,11 +11897,15 @@
       </c>
       <c r="F47" s="74">
         <f t="shared" si="0"/>
-        <v>1.053001053001053</v>
+        <v>1.1045655375552283</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="1"/>
+        <v>258.66666666666663</v>
       </c>
       <c r="I47">
-        <f t="shared" si="1"/>
-        <v>0.49806513042170197</v>
+        <f t="shared" si="2"/>
+        <v>0.45695765399664728</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -11788,21 +11928,25 @@
       </c>
       <c r="F48" s="74">
         <f t="shared" si="0"/>
-        <v>1.053001053001053</v>
+        <v>1.1045655375552283</v>
+      </c>
+      <c r="G48">
+        <f>1/(E48/E$50)</f>
+        <v>388</v>
       </c>
       <c r="I48">
-        <f t="shared" si="1"/>
-        <v>0.74877777987263705</v>
+        <f t="shared" si="2"/>
+        <v>0.68697790059247532</v>
       </c>
     </row>
     <row r="50" spans="5:8">
       <c r="E50">
         <f>SUM(E13:E48)</f>
-        <v>203500</v>
+        <v>194000</v>
       </c>
       <c r="F50">
         <f>SUM(F13:F48)</f>
-        <v>50.542295542295555</v>
+        <v>52.039764359351977</v>
       </c>
     </row>
     <row r="51" spans="5:8">
@@ -11817,7 +11961,7 @@
       </c>
       <c r="H51" s="75">
         <f>F50/600</f>
-        <v>8.4237159237159256E-2</v>
+        <v>8.6732940598919964E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>